<commit_message>
Atualizado por script em 11-11-2023 08:45
</commit_message>
<xml_diff>
--- a/2023/algeria_ligue-1_2023-2024.xlsx
+++ b/2023/algeria_ligue-1_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V30"/>
+  <dimension ref="A1:V34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -849,71 +849,71 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>MC Alger</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Ben Aknoun</t>
+          <t>Kabylie</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>1.4</v>
+        <v>2.84</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>16/09/2023 03:43</t>
+          <t>15/09/2023 13:42</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>1.3</v>
+        <v>3.8</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>16/09/2023 10:40</t>
+          <t>16/09/2023 16:12</t>
         </is>
       </c>
       <c r="N5" t="n">
-        <v>4.19</v>
+        <v>2.63</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>16/09/2023 03:43</t>
+          <t>15/09/2023 13:42</t>
         </is>
       </c>
       <c r="P5" t="n">
-        <v>4.81</v>
+        <v>2.84</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>16/09/2023 16:47</t>
+          <t>16/09/2023 15:03</t>
         </is>
       </c>
       <c r="R5" t="n">
-        <v>8.529999999999999</v>
+        <v>2.72</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>16/09/2023 03:43</t>
+          <t>15/09/2023 13:42</t>
         </is>
       </c>
       <c r="T5" t="n">
-        <v>12.64</v>
+        <v>2.26</v>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>16/09/2023 16:47</t>
+          <t>16/09/2023 16:12</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/mc-alger-es-ben-aknoun/WjyqCu9h/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-kabylie/YFXa8c8H/</t>
         </is>
       </c>
     </row>
@@ -941,71 +941,71 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Magra</t>
+          <t>MC Alger</t>
         </is>
       </c>
       <c r="G6" t="n">
+        <v>4</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Ben Aknoun</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
         <v>0</v>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Kabylie</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>1</v>
-      </c>
       <c r="J6" t="n">
-        <v>2.84</v>
+        <v>1.4</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>15/09/2023 13:42</t>
+          <t>16/09/2023 03:43</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>3.8</v>
+        <v>1.3</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>16/09/2023 16:12</t>
+          <t>16/09/2023 10:40</t>
         </is>
       </c>
       <c r="N6" t="n">
-        <v>2.63</v>
+        <v>4.19</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>15/09/2023 13:42</t>
+          <t>16/09/2023 03:43</t>
         </is>
       </c>
       <c r="P6" t="n">
-        <v>2.84</v>
+        <v>4.81</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>16/09/2023 15:03</t>
+          <t>16/09/2023 16:47</t>
         </is>
       </c>
       <c r="R6" t="n">
-        <v>2.72</v>
+        <v>8.529999999999999</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>15/09/2023 13:42</t>
+          <t>16/09/2023 03:43</t>
         </is>
       </c>
       <c r="T6" t="n">
-        <v>2.26</v>
+        <v>12.64</v>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>16/09/2023 16:12</t>
+          <t>16/09/2023 16:47</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-kabylie/YFXa8c8H/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/mc-alger-es-ben-aknoun/WjyqCu9h/</t>
         </is>
       </c>
     </row>
@@ -1953,71 +1953,71 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Khenchela</t>
+          <t>US Souf</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Kabylie</t>
+          <t>Oran</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>2.63</v>
+        <v>2.49</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>28/09/2023 04:12</t>
+          <t>28/09/2023 19:27</t>
         </is>
       </c>
       <c r="L17" t="n">
-        <v>2.05</v>
+        <v>2.14</v>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>29/09/2023 16:41</t>
+          <t>29/09/2023 13:29</t>
         </is>
       </c>
       <c r="N17" t="n">
-        <v>2.62</v>
+        <v>2.88</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>28/09/2023 04:12</t>
+          <t>28/09/2023 19:27</t>
         </is>
       </c>
       <c r="P17" t="n">
-        <v>2.75</v>
+        <v>2.74</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>29/09/2023 16:41</t>
+          <t>29/09/2023 14:49</t>
         </is>
       </c>
       <c r="R17" t="n">
-        <v>3.02</v>
+        <v>3.18</v>
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>28/09/2023 04:12</t>
+          <t>28/09/2023 19:27</t>
         </is>
       </c>
       <c r="T17" t="n">
-        <v>4.88</v>
+        <v>4.43</v>
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>29/09/2023 16:27</t>
+          <t>29/09/2023 15:47</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-kabylie/pUZYGLcr/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-oran/6qOsFaSf/</t>
         </is>
       </c>
     </row>
@@ -2045,71 +2045,71 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Khenchela</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Oran</t>
+          <t>Kabylie</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="n">
-        <v>2.49</v>
+        <v>2.63</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>28/09/2023 19:27</t>
+          <t>28/09/2023 04:12</t>
         </is>
       </c>
       <c r="L18" t="n">
-        <v>2.14</v>
+        <v>2.05</v>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>29/09/2023 13:29</t>
+          <t>29/09/2023 16:41</t>
         </is>
       </c>
       <c r="N18" t="n">
-        <v>2.88</v>
+        <v>2.62</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>28/09/2023 19:27</t>
+          <t>28/09/2023 04:12</t>
         </is>
       </c>
       <c r="P18" t="n">
-        <v>2.74</v>
+        <v>2.75</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>29/09/2023 14:49</t>
+          <t>29/09/2023 16:41</t>
         </is>
       </c>
       <c r="R18" t="n">
-        <v>3.18</v>
+        <v>3.02</v>
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>28/09/2023 19:27</t>
+          <t>28/09/2023 04:12</t>
         </is>
       </c>
       <c r="T18" t="n">
-        <v>4.43</v>
+        <v>4.88</v>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>29/09/2023 15:47</t>
+          <t>29/09/2023 16:27</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-oran/6qOsFaSf/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-kabylie/pUZYGLcr/</t>
         </is>
       </c>
     </row>
@@ -3214,6 +3214,374 @@
       <c r="V30" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/algeria/ligue-1/usm-alger-khenchela/pGf02Mrk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>45240.64583333334</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Paradou</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>1</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Oran</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>19/10/2023 04:42</t>
+        </is>
+      </c>
+      <c r="L31" t="n">
+        <v>1.46</v>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>10/11/2023 14:57</t>
+        </is>
+      </c>
+      <c r="N31" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>19/10/2023 04:42</t>
+        </is>
+      </c>
+      <c r="P31" t="n">
+        <v>3.91</v>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>10/11/2023 14:57</t>
+        </is>
+      </c>
+      <c r="R31" t="n">
+        <v>6.42</v>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>19/10/2023 04:42</t>
+        </is>
+      </c>
+      <c r="T31" t="n">
+        <v>8.550000000000001</v>
+      </c>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>10/11/2023 14:57</t>
+        </is>
+      </c>
+      <c r="V31" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/paradou-oran/ALKA1eA0/</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>45240.64583333334</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>US Souf</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>3</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Constantine</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>4</v>
+      </c>
+      <c r="J32" t="n">
+        <v>3.14</v>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>10/11/2023 06:42</t>
+        </is>
+      </c>
+      <c r="L32" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>10/11/2023 15:16</t>
+        </is>
+      </c>
+      <c r="N32" t="n">
+        <v>2.82</v>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>10/11/2023 06:42</t>
+        </is>
+      </c>
+      <c r="P32" t="n">
+        <v>2.86</v>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>10/11/2023 13:35</t>
+        </is>
+      </c>
+      <c r="R32" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>10/11/2023 06:42</t>
+        </is>
+      </c>
+      <c r="T32" t="n">
+        <v>2.53</v>
+      </c>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>10/11/2023 15:16</t>
+        </is>
+      </c>
+      <c r="V32" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-constantine/6mEJaZvD/</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>45240.65625</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>ES Setif</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
+        <v>1</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Kabylie</t>
+        </is>
+      </c>
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>09/11/2023 04:12</t>
+        </is>
+      </c>
+      <c r="L33" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>10/11/2023 12:22</t>
+        </is>
+      </c>
+      <c r="N33" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>09/11/2023 04:12</t>
+        </is>
+      </c>
+      <c r="P33" t="n">
+        <v>3.06</v>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>10/11/2023 13:50</t>
+        </is>
+      </c>
+      <c r="R33" t="n">
+        <v>2.89</v>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>09/11/2023 04:12</t>
+        </is>
+      </c>
+      <c r="T33" t="n">
+        <v>3.93</v>
+      </c>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>10/11/2023 12:22</t>
+        </is>
+      </c>
+      <c r="V33" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/es-setif-kabylie/Cp59MdnQ/</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>45240.70833333334</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>USM Alger</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>2</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>CR Belouizdad</t>
+        </is>
+      </c>
+      <c r="I34" t="n">
+        <v>1</v>
+      </c>
+      <c r="J34" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>09/11/2023 05:12</t>
+        </is>
+      </c>
+      <c r="L34" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>10/11/2023 16:57</t>
+        </is>
+      </c>
+      <c r="N34" t="n">
+        <v>2.83</v>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>09/11/2023 05:12</t>
+        </is>
+      </c>
+      <c r="P34" t="n">
+        <v>2.82</v>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>10/11/2023 16:57</t>
+        </is>
+      </c>
+      <c r="R34" t="n">
+        <v>3.35</v>
+      </c>
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>09/11/2023 05:12</t>
+        </is>
+      </c>
+      <c r="T34" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>10/11/2023 16:57</t>
+        </is>
+      </c>
+      <c r="V34" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/usm-alger-cr-belouizdad/IRsxIGfs/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 11-11-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/algeria_ligue-1_2023-2024.xlsx
+++ b/2023/algeria_ligue-1_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V34"/>
+  <dimension ref="A1:V38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -573,7 +573,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>El Bayadh</t>
+          <t>Khenchela</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -581,14 +581,14 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Constantine</t>
+          <t>ES Setif</t>
         </is>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>2.28</v>
+        <v>1.95</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -596,15 +596,15 @@
         </is>
       </c>
       <c r="L2" t="n">
-        <v>2.37</v>
+        <v>1.62</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>15/09/2023 16:57</t>
+          <t>15/09/2023 16:54</t>
         </is>
       </c>
       <c r="N2" t="n">
-        <v>2.8</v>
+        <v>2.95</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -612,15 +612,15 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>2.87</v>
+        <v>3.48</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>15/09/2023 16:57</t>
+          <t>15/09/2023 16:54</t>
         </is>
       </c>
       <c r="R2" t="n">
-        <v>3.28</v>
+        <v>4.13</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
@@ -628,16 +628,16 @@
         </is>
       </c>
       <c r="T2" t="n">
-        <v>3.48</v>
+        <v>6.62</v>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>15/09/2023 16:57</t>
+          <t>15/09/2023 16:54</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-constantine/QkUiAJw5/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-es-setif/rRvmBaOb/</t>
         </is>
       </c>
     </row>
@@ -665,7 +665,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Khenchela</t>
+          <t>El Bayadh</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -673,14 +673,14 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>ES Setif</t>
+          <t>Constantine</t>
         </is>
       </c>
       <c r="I3" t="n">
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>1.95</v>
+        <v>2.28</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
@@ -688,15 +688,15 @@
         </is>
       </c>
       <c r="L3" t="n">
-        <v>1.62</v>
+        <v>2.37</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>15/09/2023 16:54</t>
+          <t>15/09/2023 16:57</t>
         </is>
       </c>
       <c r="N3" t="n">
-        <v>2.95</v>
+        <v>2.8</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -704,32 +704,32 @@
         </is>
       </c>
       <c r="P3" t="n">
+        <v>2.87</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>15/09/2023 16:57</t>
+        </is>
+      </c>
+      <c r="R3" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>14/09/2023 05:12</t>
+        </is>
+      </c>
+      <c r="T3" t="n">
         <v>3.48</v>
       </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>15/09/2023 16:54</t>
-        </is>
-      </c>
-      <c r="R3" t="n">
-        <v>4.13</v>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>14/09/2023 05:12</t>
-        </is>
-      </c>
-      <c r="T3" t="n">
-        <v>6.62</v>
-      </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>15/09/2023 16:54</t>
+          <t>15/09/2023 16:57</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-es-setif/rRvmBaOb/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-constantine/QkUiAJw5/</t>
         </is>
       </c>
     </row>
@@ -1861,7 +1861,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Magra</t>
+          <t>Khenchela</t>
         </is>
       </c>
       <c r="G16" t="n">
@@ -1869,14 +1869,14 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Biskra</t>
+          <t>Kabylie</t>
         </is>
       </c>
       <c r="I16" t="n">
         <v>1</v>
       </c>
       <c r="J16" t="n">
-        <v>1.98</v>
+        <v>2.63</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
@@ -1884,15 +1884,15 @@
         </is>
       </c>
       <c r="L16" t="n">
-        <v>2.1</v>
+        <v>2.05</v>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>29/09/2023 16:44</t>
+          <t>29/09/2023 16:41</t>
         </is>
       </c>
       <c r="N16" t="n">
-        <v>2.89</v>
+        <v>2.62</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1900,15 +1900,15 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>2.77</v>
+        <v>2.75</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>29/09/2023 16:44</t>
+          <t>29/09/2023 16:41</t>
         </is>
       </c>
       <c r="R16" t="n">
-        <v>3.97</v>
+        <v>3.02</v>
       </c>
       <c r="S16" t="inlineStr">
         <is>
@@ -1916,16 +1916,16 @@
         </is>
       </c>
       <c r="T16" t="n">
-        <v>4.54</v>
+        <v>4.88</v>
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>29/09/2023 16:44</t>
+          <t>29/09/2023 16:27</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-biskra/OKYxGuDl/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-kabylie/pUZYGLcr/</t>
         </is>
       </c>
     </row>
@@ -1953,71 +1953,71 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Oran</t>
+          <t>Biskra</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" t="n">
-        <v>2.49</v>
+        <v>1.98</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>28/09/2023 19:27</t>
+          <t>28/09/2023 04:12</t>
         </is>
       </c>
       <c r="L17" t="n">
-        <v>2.14</v>
+        <v>2.1</v>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>29/09/2023 13:29</t>
+          <t>29/09/2023 16:44</t>
         </is>
       </c>
       <c r="N17" t="n">
-        <v>2.88</v>
+        <v>2.89</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>28/09/2023 19:27</t>
+          <t>28/09/2023 04:12</t>
         </is>
       </c>
       <c r="P17" t="n">
-        <v>2.74</v>
+        <v>2.77</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>29/09/2023 14:49</t>
+          <t>29/09/2023 16:44</t>
         </is>
       </c>
       <c r="R17" t="n">
-        <v>3.18</v>
+        <v>3.97</v>
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>28/09/2023 19:27</t>
+          <t>28/09/2023 04:12</t>
         </is>
       </c>
       <c r="T17" t="n">
-        <v>4.43</v>
+        <v>4.54</v>
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>29/09/2023 15:47</t>
+          <t>29/09/2023 16:44</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-oran/6qOsFaSf/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-biskra/OKYxGuDl/</t>
         </is>
       </c>
     </row>
@@ -2045,71 +2045,71 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Khenchela</t>
+          <t>US Souf</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Kabylie</t>
+          <t>Oran</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>2.63</v>
+        <v>2.49</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>28/09/2023 04:12</t>
+          <t>28/09/2023 19:27</t>
         </is>
       </c>
       <c r="L18" t="n">
-        <v>2.05</v>
+        <v>2.14</v>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>29/09/2023 16:41</t>
+          <t>29/09/2023 13:29</t>
         </is>
       </c>
       <c r="N18" t="n">
-        <v>2.62</v>
+        <v>2.88</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>28/09/2023 04:12</t>
+          <t>28/09/2023 19:27</t>
         </is>
       </c>
       <c r="P18" t="n">
-        <v>2.75</v>
+        <v>2.74</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>29/09/2023 16:41</t>
+          <t>29/09/2023 14:49</t>
         </is>
       </c>
       <c r="R18" t="n">
-        <v>3.02</v>
+        <v>3.18</v>
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>28/09/2023 04:12</t>
+          <t>28/09/2023 19:27</t>
         </is>
       </c>
       <c r="T18" t="n">
-        <v>4.88</v>
+        <v>4.43</v>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>29/09/2023 16:27</t>
+          <t>29/09/2023 15:47</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-kabylie/pUZYGLcr/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-oran/6qOsFaSf/</t>
         </is>
       </c>
     </row>
@@ -3582,6 +3582,374 @@
       <c r="V34" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/algeria/ligue-1/usm-alger-cr-belouizdad/IRsxIGfs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>45241.625</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Khenchela</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Biskra</t>
+        </is>
+      </c>
+      <c r="I35" t="n">
+        <v>1</v>
+      </c>
+      <c r="J35" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>10/11/2023 03:13</t>
+        </is>
+      </c>
+      <c r="L35" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>11/11/2023 10:24</t>
+        </is>
+      </c>
+      <c r="N35" t="n">
+        <v>3.19</v>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>10/11/2023 03:13</t>
+        </is>
+      </c>
+      <c r="P35" t="n">
+        <v>4.87</v>
+      </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>11/11/2023 14:54</t>
+        </is>
+      </c>
+      <c r="R35" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>10/11/2023 03:13</t>
+        </is>
+      </c>
+      <c r="T35" t="n">
+        <v>13.77</v>
+      </c>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>11/11/2023 14:54</t>
+        </is>
+      </c>
+      <c r="V35" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-biskra/GbL62yef/</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>45241.625</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Magra</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>3</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Ben Aknoun</t>
+        </is>
+      </c>
+      <c r="I36" t="n">
+        <v>1</v>
+      </c>
+      <c r="J36" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>11/11/2023 10:12</t>
+        </is>
+      </c>
+      <c r="L36" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>11/11/2023 14:48</t>
+        </is>
+      </c>
+      <c r="N36" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>11/11/2023 10:12</t>
+        </is>
+      </c>
+      <c r="P36" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>11/11/2023 14:48</t>
+        </is>
+      </c>
+      <c r="R36" t="n">
+        <v>5.97</v>
+      </c>
+      <c r="S36" t="inlineStr">
+        <is>
+          <t>11/11/2023 10:12</t>
+        </is>
+      </c>
+      <c r="T36" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>11/11/2023 14:48</t>
+        </is>
+      </c>
+      <c r="V36" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-es-ben-aknoun/lCJE0FP6/</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>45241.70833333334</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>ASO Chlef</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>MC Alger</t>
+        </is>
+      </c>
+      <c r="I37" t="n">
+        <v>1</v>
+      </c>
+      <c r="J37" t="n">
+        <v>2.11</v>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>19/10/2023 06:12</t>
+        </is>
+      </c>
+      <c r="L37" t="n">
+        <v>2.68</v>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>11/11/2023 16:47</t>
+        </is>
+      </c>
+      <c r="N37" t="n">
+        <v>2.84</v>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>19/10/2023 06:12</t>
+        </is>
+      </c>
+      <c r="P37" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>11/11/2023 16:20</t>
+        </is>
+      </c>
+      <c r="R37" t="n">
+        <v>3.64</v>
+      </c>
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>19/10/2023 06:12</t>
+        </is>
+      </c>
+      <c r="T37" t="n">
+        <v>3.05</v>
+      </c>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>11/11/2023 16:47</t>
+        </is>
+      </c>
+      <c r="V37" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/aso-chlef-mc-alger/bs15NxXJ/</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>45241.75</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Saoura</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>El Bayadh</t>
+        </is>
+      </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>10/11/2023 06:12</t>
+        </is>
+      </c>
+      <c r="L38" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>11/11/2023 17:14</t>
+        </is>
+      </c>
+      <c r="N38" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>10/11/2023 06:12</t>
+        </is>
+      </c>
+      <c r="P38" t="n">
+        <v>3.62</v>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>11/11/2023 17:34</t>
+        </is>
+      </c>
+      <c r="R38" t="n">
+        <v>4.94</v>
+      </c>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>10/11/2023 06:12</t>
+        </is>
+      </c>
+      <c r="T38" t="n">
+        <v>7.47</v>
+      </c>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>11/11/2023 17:34</t>
+        </is>
+      </c>
+      <c r="V38" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/saoura-el-bayadh/pvDNbgfJ/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 14-11-2023 20:48
</commit_message>
<xml_diff>
--- a/2023/algeria_ligue-1_2023-2024.xlsx
+++ b/2023/algeria_ligue-1_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V38"/>
+  <dimension ref="A1:V40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -573,7 +573,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Khenchela</t>
+          <t>El Bayadh</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -581,14 +581,14 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>ES Setif</t>
+          <t>Constantine</t>
         </is>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>1.95</v>
+        <v>2.28</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -596,15 +596,15 @@
         </is>
       </c>
       <c r="L2" t="n">
-        <v>1.62</v>
+        <v>2.37</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>15/09/2023 16:54</t>
+          <t>15/09/2023 16:57</t>
         </is>
       </c>
       <c r="N2" t="n">
-        <v>2.95</v>
+        <v>2.8</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -612,32 +612,32 @@
         </is>
       </c>
       <c r="P2" t="n">
+        <v>2.87</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>15/09/2023 16:57</t>
+        </is>
+      </c>
+      <c r="R2" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>14/09/2023 05:12</t>
+        </is>
+      </c>
+      <c r="T2" t="n">
         <v>3.48</v>
       </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>15/09/2023 16:54</t>
-        </is>
-      </c>
-      <c r="R2" t="n">
-        <v>4.13</v>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>14/09/2023 05:12</t>
-        </is>
-      </c>
-      <c r="T2" t="n">
-        <v>6.62</v>
-      </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>15/09/2023 16:54</t>
+          <t>15/09/2023 16:57</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-es-setif/rRvmBaOb/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-constantine/QkUiAJw5/</t>
         </is>
       </c>
     </row>
@@ -665,7 +665,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>El Bayadh</t>
+          <t>Khenchela</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -673,14 +673,14 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Constantine</t>
+          <t>ES Setif</t>
         </is>
       </c>
       <c r="I3" t="n">
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>2.28</v>
+        <v>1.95</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
@@ -688,15 +688,15 @@
         </is>
       </c>
       <c r="L3" t="n">
-        <v>2.37</v>
+        <v>1.62</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>15/09/2023 16:57</t>
+          <t>15/09/2023 16:54</t>
         </is>
       </c>
       <c r="N3" t="n">
-        <v>2.8</v>
+        <v>2.95</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -704,15 +704,15 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>2.87</v>
+        <v>3.48</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>15/09/2023 16:57</t>
+          <t>15/09/2023 16:54</t>
         </is>
       </c>
       <c r="R3" t="n">
-        <v>3.28</v>
+        <v>4.13</v>
       </c>
       <c r="S3" t="inlineStr">
         <is>
@@ -720,16 +720,16 @@
         </is>
       </c>
       <c r="T3" t="n">
-        <v>3.48</v>
+        <v>6.62</v>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>15/09/2023 16:57</t>
+          <t>15/09/2023 16:54</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-constantine/QkUiAJw5/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-es-setif/rRvmBaOb/</t>
         </is>
       </c>
     </row>
@@ -849,71 +849,71 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Magra</t>
+          <t>MC Alger</t>
         </is>
       </c>
       <c r="G5" t="n">
+        <v>4</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Ben Aknoun</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
         <v>0</v>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Kabylie</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>1</v>
-      </c>
       <c r="J5" t="n">
-        <v>2.84</v>
+        <v>1.4</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>15/09/2023 13:42</t>
+          <t>16/09/2023 03:43</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>3.8</v>
+        <v>1.3</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>16/09/2023 16:12</t>
+          <t>16/09/2023 10:40</t>
         </is>
       </c>
       <c r="N5" t="n">
-        <v>2.63</v>
+        <v>4.19</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>15/09/2023 13:42</t>
+          <t>16/09/2023 03:43</t>
         </is>
       </c>
       <c r="P5" t="n">
-        <v>2.84</v>
+        <v>4.81</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>16/09/2023 15:03</t>
+          <t>16/09/2023 16:47</t>
         </is>
       </c>
       <c r="R5" t="n">
-        <v>2.72</v>
+        <v>8.529999999999999</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>15/09/2023 13:42</t>
+          <t>16/09/2023 03:43</t>
         </is>
       </c>
       <c r="T5" t="n">
-        <v>2.26</v>
+        <v>12.64</v>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>16/09/2023 16:12</t>
+          <t>16/09/2023 16:47</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-kabylie/YFXa8c8H/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/mc-alger-es-ben-aknoun/WjyqCu9h/</t>
         </is>
       </c>
     </row>
@@ -941,71 +941,71 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>MC Alger</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Ben Aknoun</t>
+          <t>Kabylie</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>1.4</v>
+        <v>2.84</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>16/09/2023 03:43</t>
+          <t>15/09/2023 13:42</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>1.3</v>
+        <v>3.8</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>16/09/2023 10:40</t>
+          <t>16/09/2023 16:12</t>
         </is>
       </c>
       <c r="N6" t="n">
-        <v>4.19</v>
+        <v>2.63</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>16/09/2023 03:43</t>
+          <t>15/09/2023 13:42</t>
         </is>
       </c>
       <c r="P6" t="n">
-        <v>4.81</v>
+        <v>2.84</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>16/09/2023 16:47</t>
+          <t>16/09/2023 15:03</t>
         </is>
       </c>
       <c r="R6" t="n">
-        <v>8.529999999999999</v>
+        <v>2.72</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>16/09/2023 03:43</t>
+          <t>15/09/2023 13:42</t>
         </is>
       </c>
       <c r="T6" t="n">
-        <v>12.64</v>
+        <v>2.26</v>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>16/09/2023 16:47</t>
+          <t>16/09/2023 16:12</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/mc-alger-es-ben-aknoun/WjyqCu9h/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-kabylie/YFXa8c8H/</t>
         </is>
       </c>
     </row>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Constantine</t>
+          <t>Ben Aknoun</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -1133,63 +1133,63 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>MC Alger</t>
+          <t>ASO Chlef</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" t="n">
-        <v>1.98</v>
+        <v>2.81</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>21/09/2023 05:12</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>3.68</v>
+        <v>2.51</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>22/09/2023 16:51</t>
+          <t>22/09/2023 16:00</t>
         </is>
       </c>
       <c r="N8" t="n">
-        <v>2.89</v>
+        <v>3.04</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>21/09/2023 05:12</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="P8" t="n">
-        <v>2.92</v>
+        <v>3.06</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>22/09/2023 16:51</t>
+          <t>22/09/2023 16:34</t>
         </is>
       </c>
       <c r="R8" t="n">
-        <v>3.97</v>
+        <v>2.64</v>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>21/09/2023 05:12</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="T8" t="n">
-        <v>2.26</v>
+        <v>3.01</v>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>22/09/2023 16:51</t>
+          <t>22/09/2023 16:00</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-mc-alger/Eoq3MszL/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/es-ben-aknoun-aso-chlef/WMgbNNKE/</t>
         </is>
       </c>
     </row>
@@ -1217,7 +1217,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Ben Aknoun</t>
+          <t>Constantine</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -1225,63 +1225,63 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>ASO Chlef</t>
+          <t>MC Alger</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>2.81</v>
+        <v>1.98</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>21/09/2023 05:12</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>2.51</v>
+        <v>3.68</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>22/09/2023 16:00</t>
+          <t>22/09/2023 16:51</t>
         </is>
       </c>
       <c r="N9" t="n">
-        <v>3.04</v>
+        <v>2.89</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>21/09/2023 05:12</t>
         </is>
       </c>
       <c r="P9" t="n">
-        <v>3.06</v>
+        <v>2.92</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>22/09/2023 16:34</t>
+          <t>22/09/2023 16:51</t>
         </is>
       </c>
       <c r="R9" t="n">
-        <v>2.64</v>
+        <v>3.97</v>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>21/09/2023 05:12</t>
         </is>
       </c>
       <c r="T9" t="n">
-        <v>3.01</v>
+        <v>2.26</v>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>22/09/2023 16:00</t>
+          <t>22/09/2023 16:51</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/es-ben-aknoun-aso-chlef/WMgbNNKE/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-mc-alger/Eoq3MszL/</t>
         </is>
       </c>
     </row>
@@ -1861,71 +1861,71 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Khenchela</t>
+          <t>US Souf</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Kabylie</t>
+          <t>Oran</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>2.63</v>
+        <v>2.49</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>28/09/2023 04:12</t>
+          <t>28/09/2023 19:27</t>
         </is>
       </c>
       <c r="L16" t="n">
-        <v>2.05</v>
+        <v>2.14</v>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>29/09/2023 16:41</t>
+          <t>29/09/2023 13:29</t>
         </is>
       </c>
       <c r="N16" t="n">
-        <v>2.62</v>
+        <v>2.88</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>28/09/2023 04:12</t>
+          <t>28/09/2023 19:27</t>
         </is>
       </c>
       <c r="P16" t="n">
-        <v>2.75</v>
+        <v>2.74</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>29/09/2023 16:41</t>
+          <t>29/09/2023 14:49</t>
         </is>
       </c>
       <c r="R16" t="n">
-        <v>3.02</v>
+        <v>3.18</v>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>28/09/2023 04:12</t>
+          <t>28/09/2023 19:27</t>
         </is>
       </c>
       <c r="T16" t="n">
-        <v>4.88</v>
+        <v>4.43</v>
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>29/09/2023 16:27</t>
+          <t>29/09/2023 15:47</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-kabylie/pUZYGLcr/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-oran/6qOsFaSf/</t>
         </is>
       </c>
     </row>
@@ -2045,71 +2045,71 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Khenchela</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Oran</t>
+          <t>Kabylie</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="n">
-        <v>2.49</v>
+        <v>2.63</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>28/09/2023 19:27</t>
+          <t>28/09/2023 04:12</t>
         </is>
       </c>
       <c r="L18" t="n">
-        <v>2.14</v>
+        <v>2.05</v>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>29/09/2023 13:29</t>
+          <t>29/09/2023 16:41</t>
         </is>
       </c>
       <c r="N18" t="n">
-        <v>2.88</v>
+        <v>2.62</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>28/09/2023 19:27</t>
+          <t>28/09/2023 04:12</t>
         </is>
       </c>
       <c r="P18" t="n">
-        <v>2.74</v>
+        <v>2.75</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>29/09/2023 14:49</t>
+          <t>29/09/2023 16:41</t>
         </is>
       </c>
       <c r="R18" t="n">
-        <v>3.18</v>
+        <v>3.02</v>
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>28/09/2023 19:27</t>
+          <t>28/09/2023 04:12</t>
         </is>
       </c>
       <c r="T18" t="n">
-        <v>4.43</v>
+        <v>4.88</v>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>29/09/2023 15:47</t>
+          <t>29/09/2023 16:27</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-oran/6qOsFaSf/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-kabylie/pUZYGLcr/</t>
         </is>
       </c>
     </row>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Biskra</t>
+          <t>Oran</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -2513,14 +2513,14 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Paradou</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>2.18</v>
+        <v>1.98</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
@@ -2528,15 +2528,15 @@
         </is>
       </c>
       <c r="L23" t="n">
-        <v>2.03</v>
+        <v>1.65</v>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>06/10/2023 19:34</t>
+          <t>06/10/2023 17:55</t>
         </is>
       </c>
       <c r="N23" t="n">
-        <v>2.84</v>
+        <v>2.89</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2544,15 +2544,15 @@
         </is>
       </c>
       <c r="P23" t="n">
-        <v>3</v>
+        <v>3.28</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>06/10/2023 18:05</t>
+          <t>06/10/2023 19:03</t>
         </is>
       </c>
       <c r="R23" t="n">
-        <v>3.56</v>
+        <v>3.98</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
@@ -2560,16 +2560,16 @@
         </is>
       </c>
       <c r="T23" t="n">
-        <v>4.33</v>
+        <v>5.91</v>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>06/10/2023 19:34</t>
+          <t>06/10/2023 17:55</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-paradou/hhWUzskE/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-magra/WrVYZ04K/</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Oran</t>
+          <t>Biskra</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -2605,14 +2605,14 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Magra</t>
+          <t>Paradou</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J24" t="n">
-        <v>1.98</v>
+        <v>2.18</v>
       </c>
       <c r="K24" t="inlineStr">
         <is>
@@ -2620,15 +2620,15 @@
         </is>
       </c>
       <c r="L24" t="n">
-        <v>1.65</v>
+        <v>2.03</v>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>06/10/2023 17:55</t>
+          <t>06/10/2023 19:34</t>
         </is>
       </c>
       <c r="N24" t="n">
-        <v>2.89</v>
+        <v>2.84</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2636,15 +2636,15 @@
         </is>
       </c>
       <c r="P24" t="n">
-        <v>3.28</v>
+        <v>3</v>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>06/10/2023 19:03</t>
+          <t>06/10/2023 18:05</t>
         </is>
       </c>
       <c r="R24" t="n">
-        <v>3.98</v>
+        <v>3.56</v>
       </c>
       <c r="S24" t="inlineStr">
         <is>
@@ -2652,16 +2652,16 @@
         </is>
       </c>
       <c r="T24" t="n">
-        <v>5.91</v>
+        <v>4.33</v>
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>06/10/2023 17:55</t>
+          <t>06/10/2023 19:34</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-magra/WrVYZ04K/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-paradou/hhWUzskE/</t>
         </is>
       </c>
     </row>
@@ -3950,6 +3950,190 @@
       <c r="V38" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/algeria/ligue-1/saoura-el-bayadh/pvDNbgfJ/</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>45244.625</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Paradou</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>CR Belouizdad</t>
+        </is>
+      </c>
+      <c r="I39" t="n">
+        <v>1</v>
+      </c>
+      <c r="J39" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>23/10/2023 04:42</t>
+        </is>
+      </c>
+      <c r="L39" t="n">
+        <v>2.76</v>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>14/11/2023 14:57</t>
+        </is>
+      </c>
+      <c r="N39" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>23/10/2023 04:42</t>
+        </is>
+      </c>
+      <c r="P39" t="n">
+        <v>2.93</v>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>14/11/2023 14:57</t>
+        </is>
+      </c>
+      <c r="R39" t="n">
+        <v>3.93</v>
+      </c>
+      <c r="S39" t="inlineStr">
+        <is>
+          <t>23/10/2023 04:42</t>
+        </is>
+      </c>
+      <c r="T39" t="n">
+        <v>2.82</v>
+      </c>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>14/11/2023 14:57</t>
+        </is>
+      </c>
+      <c r="V39" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/paradou-cr-belouizdad/W6DLQdR6/</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>45244.79166666666</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>ES Setif</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>2</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>USM Alger</t>
+        </is>
+      </c>
+      <c r="I40" t="n">
+        <v>1</v>
+      </c>
+      <c r="J40" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>23/10/2023 08:11</t>
+        </is>
+      </c>
+      <c r="L40" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>14/11/2023 18:47</t>
+        </is>
+      </c>
+      <c r="N40" t="n">
+        <v>2.93</v>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>23/10/2023 08:11</t>
+        </is>
+      </c>
+      <c r="P40" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>14/11/2023 18:37</t>
+        </is>
+      </c>
+      <c r="R40" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="S40" t="inlineStr">
+        <is>
+          <t>23/10/2023 08:11</t>
+        </is>
+      </c>
+      <c r="T40" t="n">
+        <v>3.84</v>
+      </c>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>14/11/2023 18:54</t>
+        </is>
+      </c>
+      <c r="V40" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/es-setif-usm-alger/EV2QPGtD/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 17-11-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/algeria_ligue-1_2023-2024.xlsx
+++ b/2023/algeria_ligue-1_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V40"/>
+  <dimension ref="A1:V44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1493,71 +1493,71 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Biskra</t>
+          <t>Oran</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Saoura</t>
         </is>
       </c>
       <c r="I12" t="n">
         <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>1.71</v>
+        <v>2.54</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>22/09/2023 15:13</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="L12" t="n">
-        <v>1.65</v>
+        <v>2.34</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>23/09/2023 19:13</t>
+          <t>23/09/2023 18:03</t>
         </is>
       </c>
       <c r="N12" t="n">
-        <v>3.22</v>
+        <v>2.65</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>22/09/2023 15:13</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="P12" t="n">
-        <v>3.47</v>
+        <v>2.71</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>23/09/2023 19:13</t>
+          <t>23/09/2023 18:03</t>
         </is>
       </c>
       <c r="R12" t="n">
-        <v>4.87</v>
+        <v>3.11</v>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>22/09/2023 15:13</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="T12" t="n">
-        <v>6.17</v>
+        <v>3.84</v>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>23/09/2023 19:13</t>
+          <t>23/09/2023 18:03</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-us-souf/KYnDaKS7/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-saoura/YyyeO358/</t>
         </is>
       </c>
     </row>
@@ -1585,71 +1585,71 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Oran</t>
+          <t>Biskra</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Saoura</t>
+          <t>US Souf</t>
         </is>
       </c>
       <c r="I13" t="n">
         <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>2.54</v>
+        <v>1.71</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>22/09/2023 15:13</t>
         </is>
       </c>
       <c r="L13" t="n">
-        <v>2.34</v>
+        <v>1.65</v>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>23/09/2023 18:03</t>
+          <t>23/09/2023 19:13</t>
         </is>
       </c>
       <c r="N13" t="n">
-        <v>2.65</v>
+        <v>3.22</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>22/09/2023 15:13</t>
         </is>
       </c>
       <c r="P13" t="n">
-        <v>2.71</v>
+        <v>3.47</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>23/09/2023 18:03</t>
+          <t>23/09/2023 19:13</t>
         </is>
       </c>
       <c r="R13" t="n">
-        <v>3.11</v>
+        <v>4.87</v>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>22/09/2023 15:13</t>
         </is>
       </c>
       <c r="T13" t="n">
-        <v>3.84</v>
+        <v>6.17</v>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>23/09/2023 18:03</t>
+          <t>23/09/2023 19:13</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-saoura/YyyeO358/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-us-souf/KYnDaKS7/</t>
         </is>
       </c>
     </row>
@@ -4134,6 +4134,374 @@
       <c r="V40" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/algeria/ligue-1/es-setif-usm-alger/EV2QPGtD/</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>45247.64583333334</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Constantine</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Magra</t>
+        </is>
+      </c>
+      <c r="I41" t="n">
+        <v>1</v>
+      </c>
+      <c r="J41" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>26/10/2023 04:42</t>
+        </is>
+      </c>
+      <c r="L41" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>17/11/2023 15:24</t>
+        </is>
+      </c>
+      <c r="N41" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>26/10/2023 04:42</t>
+        </is>
+      </c>
+      <c r="P41" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>17/11/2023 15:24</t>
+        </is>
+      </c>
+      <c r="R41" t="n">
+        <v>5.42</v>
+      </c>
+      <c r="S41" t="inlineStr">
+        <is>
+          <t>26/10/2023 04:42</t>
+        </is>
+      </c>
+      <c r="T41" t="n">
+        <v>10.79</v>
+      </c>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>17/11/2023 15:24</t>
+        </is>
+      </c>
+      <c r="V41" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-magra/jgeqGfPg/</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>45247.64583333334</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>El Bayadh</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>4</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>US Souf</t>
+        </is>
+      </c>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>16/11/2023 03:42</t>
+        </is>
+      </c>
+      <c r="L42" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>17/11/2023 15:18</t>
+        </is>
+      </c>
+      <c r="N42" t="n">
+        <v>3.74</v>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>16/11/2023 03:42</t>
+        </is>
+      </c>
+      <c r="P42" t="n">
+        <v>4.01</v>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>17/11/2023 15:18</t>
+        </is>
+      </c>
+      <c r="R42" t="n">
+        <v>7.38</v>
+      </c>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>16/11/2023 03:42</t>
+        </is>
+      </c>
+      <c r="T42" t="n">
+        <v>8.609999999999999</v>
+      </c>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>17/11/2023 15:18</t>
+        </is>
+      </c>
+      <c r="V42" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-us-souf/UqfmFEv0/</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E43" s="2" t="n">
+        <v>45247.69791666666</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Oran</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
+        <v>1</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Khenchela</t>
+        </is>
+      </c>
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" t="n">
+        <v>2.65</v>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>16/11/2023 03:42</t>
+        </is>
+      </c>
+      <c r="L43" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>17/11/2023 16:43</t>
+        </is>
+      </c>
+      <c r="N43" t="n">
+        <v>2.95</v>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>16/11/2023 03:42</t>
+        </is>
+      </c>
+      <c r="P43" t="n">
+        <v>2.83</v>
+      </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>17/11/2023 16:43</t>
+        </is>
+      </c>
+      <c r="R43" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="S43" t="inlineStr">
+        <is>
+          <t>16/11/2023 03:42</t>
+        </is>
+      </c>
+      <c r="T43" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>17/11/2023 16:43</t>
+        </is>
+      </c>
+      <c r="V43" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-khenchela/dIttHzAm/</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E44" s="2" t="n">
+        <v>45247.75</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>MC Alger</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>4</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Saoura</t>
+        </is>
+      </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>16/11/2023 06:12</t>
+        </is>
+      </c>
+      <c r="L44" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>17/11/2023 17:56</t>
+        </is>
+      </c>
+      <c r="N44" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>16/11/2023 06:12</t>
+        </is>
+      </c>
+      <c r="P44" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>17/11/2023 17:56</t>
+        </is>
+      </c>
+      <c r="R44" t="n">
+        <v>5.99</v>
+      </c>
+      <c r="S44" t="inlineStr">
+        <is>
+          <t>16/11/2023 06:12</t>
+        </is>
+      </c>
+      <c r="T44" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>17/11/2023 17:56</t>
+        </is>
+      </c>
+      <c r="V44" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/mc-alger-saoura/C8qhEYg6/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 20-11-2023 08:45
</commit_message>
<xml_diff>
--- a/2023/algeria_ligue-1_2023-2024.xlsx
+++ b/2023/algeria_ligue-1_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V44"/>
+  <dimension ref="A1:V48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Ben Aknoun</t>
+          <t>Constantine</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -1133,63 +1133,63 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>ASO Chlef</t>
+          <t>MC Alger</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>2.81</v>
+        <v>1.98</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>21/09/2023 05:12</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>2.51</v>
+        <v>3.68</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>22/09/2023 16:00</t>
+          <t>22/09/2023 16:51</t>
         </is>
       </c>
       <c r="N8" t="n">
-        <v>3.04</v>
+        <v>2.89</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>21/09/2023 05:12</t>
         </is>
       </c>
       <c r="P8" t="n">
-        <v>3.06</v>
+        <v>2.92</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>22/09/2023 16:34</t>
+          <t>22/09/2023 16:51</t>
         </is>
       </c>
       <c r="R8" t="n">
-        <v>2.64</v>
+        <v>3.97</v>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>21/09/2023 05:12</t>
         </is>
       </c>
       <c r="T8" t="n">
-        <v>3.01</v>
+        <v>2.26</v>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>22/09/2023 16:00</t>
+          <t>22/09/2023 16:51</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/es-ben-aknoun-aso-chlef/WMgbNNKE/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-mc-alger/Eoq3MszL/</t>
         </is>
       </c>
     </row>
@@ -1217,7 +1217,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Constantine</t>
+          <t>Ben Aknoun</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -1225,63 +1225,63 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>MC Alger</t>
+          <t>ASO Chlef</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" t="n">
-        <v>1.98</v>
+        <v>2.81</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>21/09/2023 05:12</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>3.68</v>
+        <v>2.51</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>22/09/2023 16:51</t>
+          <t>22/09/2023 16:00</t>
         </is>
       </c>
       <c r="N9" t="n">
-        <v>2.89</v>
+        <v>3.04</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>21/09/2023 05:12</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="P9" t="n">
-        <v>2.92</v>
+        <v>3.06</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>22/09/2023 16:51</t>
+          <t>22/09/2023 16:34</t>
         </is>
       </c>
       <c r="R9" t="n">
-        <v>3.97</v>
+        <v>2.64</v>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>21/09/2023 05:12</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="T9" t="n">
-        <v>2.26</v>
+        <v>3.01</v>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>22/09/2023 16:51</t>
+          <t>22/09/2023 16:00</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-mc-alger/Eoq3MszL/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/es-ben-aknoun-aso-chlef/WMgbNNKE/</t>
         </is>
       </c>
     </row>
@@ -1493,71 +1493,71 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Oran</t>
+          <t>Biskra</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Saoura</t>
+          <t>US Souf</t>
         </is>
       </c>
       <c r="I12" t="n">
         <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>2.54</v>
+        <v>1.71</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>22/09/2023 15:13</t>
         </is>
       </c>
       <c r="L12" t="n">
-        <v>2.34</v>
+        <v>1.65</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>23/09/2023 18:03</t>
+          <t>23/09/2023 19:13</t>
         </is>
       </c>
       <c r="N12" t="n">
-        <v>2.65</v>
+        <v>3.22</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>22/09/2023 15:13</t>
         </is>
       </c>
       <c r="P12" t="n">
-        <v>2.71</v>
+        <v>3.47</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>23/09/2023 18:03</t>
+          <t>23/09/2023 19:13</t>
         </is>
       </c>
       <c r="R12" t="n">
-        <v>3.11</v>
+        <v>4.87</v>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>22/09/2023 15:13</t>
         </is>
       </c>
       <c r="T12" t="n">
-        <v>3.84</v>
+        <v>6.17</v>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>23/09/2023 18:03</t>
+          <t>23/09/2023 19:13</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-saoura/YyyeO358/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-us-souf/KYnDaKS7/</t>
         </is>
       </c>
     </row>
@@ -1585,71 +1585,71 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Biskra</t>
+          <t>Oran</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Saoura</t>
         </is>
       </c>
       <c r="I13" t="n">
         <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>1.71</v>
+        <v>2.54</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>22/09/2023 15:13</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="L13" t="n">
-        <v>1.65</v>
+        <v>2.34</v>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>23/09/2023 19:13</t>
+          <t>23/09/2023 18:03</t>
         </is>
       </c>
       <c r="N13" t="n">
-        <v>3.22</v>
+        <v>2.65</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>22/09/2023 15:13</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="P13" t="n">
-        <v>3.47</v>
+        <v>2.71</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>23/09/2023 19:13</t>
+          <t>23/09/2023 18:03</t>
         </is>
       </c>
       <c r="R13" t="n">
-        <v>4.87</v>
+        <v>3.11</v>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>22/09/2023 15:13</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="T13" t="n">
-        <v>6.17</v>
+        <v>3.84</v>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>23/09/2023 19:13</t>
+          <t>23/09/2023 18:03</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-us-souf/KYnDaKS7/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-saoura/YyyeO358/</t>
         </is>
       </c>
     </row>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Oran</t>
+          <t>Biskra</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -2513,14 +2513,14 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Magra</t>
+          <t>Paradou</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J23" t="n">
-        <v>1.98</v>
+        <v>2.18</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
@@ -2528,15 +2528,15 @@
         </is>
       </c>
       <c r="L23" t="n">
-        <v>1.65</v>
+        <v>2.03</v>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>06/10/2023 17:55</t>
+          <t>06/10/2023 19:34</t>
         </is>
       </c>
       <c r="N23" t="n">
-        <v>2.89</v>
+        <v>2.84</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2544,15 +2544,15 @@
         </is>
       </c>
       <c r="P23" t="n">
-        <v>3.28</v>
+        <v>3</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>06/10/2023 19:03</t>
+          <t>06/10/2023 18:05</t>
         </is>
       </c>
       <c r="R23" t="n">
-        <v>3.98</v>
+        <v>3.56</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
@@ -2560,16 +2560,16 @@
         </is>
       </c>
       <c r="T23" t="n">
-        <v>5.91</v>
+        <v>4.33</v>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>06/10/2023 17:55</t>
+          <t>06/10/2023 19:34</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-magra/WrVYZ04K/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-paradou/hhWUzskE/</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Biskra</t>
+          <t>Oran</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -2605,14 +2605,14 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Paradou</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>2.18</v>
+        <v>1.98</v>
       </c>
       <c r="K24" t="inlineStr">
         <is>
@@ -2620,15 +2620,15 @@
         </is>
       </c>
       <c r="L24" t="n">
-        <v>2.03</v>
+        <v>1.65</v>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>06/10/2023 19:34</t>
+          <t>06/10/2023 17:55</t>
         </is>
       </c>
       <c r="N24" t="n">
-        <v>2.84</v>
+        <v>2.89</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2636,15 +2636,15 @@
         </is>
       </c>
       <c r="P24" t="n">
-        <v>3</v>
+        <v>3.28</v>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>06/10/2023 18:05</t>
+          <t>06/10/2023 19:03</t>
         </is>
       </c>
       <c r="R24" t="n">
-        <v>3.56</v>
+        <v>3.98</v>
       </c>
       <c r="S24" t="inlineStr">
         <is>
@@ -2652,16 +2652,16 @@
         </is>
       </c>
       <c r="T24" t="n">
-        <v>4.33</v>
+        <v>5.91</v>
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>06/10/2023 19:34</t>
+          <t>06/10/2023 17:55</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-paradou/hhWUzskE/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-magra/WrVYZ04K/</t>
         </is>
       </c>
     </row>
@@ -2689,71 +2689,71 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>CR Belouizdad</t>
+          <t>Ben Aknoun</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Khenchela</t>
+          <t>US Souf</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J25" t="n">
-        <v>1.46</v>
+        <v>1.37</v>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>06/10/2023 04:56</t>
+          <t>05/10/2023 09:12</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>1.41</v>
+        <v>1.84</v>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>07/10/2023 16:01</t>
+          <t>07/10/2023 11:15</t>
         </is>
       </c>
       <c r="N25" t="n">
-        <v>4.01</v>
+        <v>4.23</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>06/10/2023 04:56</t>
+          <t>05/10/2023 09:12</t>
         </is>
       </c>
       <c r="P25" t="n">
-        <v>4.17</v>
+        <v>3.29</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>07/10/2023 16:42</t>
+          <t>07/10/2023 14:50</t>
         </is>
       </c>
       <c r="R25" t="n">
-        <v>7.72</v>
+        <v>6.79</v>
       </c>
       <c r="S25" t="inlineStr">
         <is>
-          <t>06/10/2023 04:56</t>
+          <t>05/10/2023 09:12</t>
         </is>
       </c>
       <c r="T25" t="n">
-        <v>9.550000000000001</v>
+        <v>4.65</v>
       </c>
       <c r="U25" t="inlineStr">
         <is>
-          <t>07/10/2023 16:42</t>
+          <t>07/10/2023 11:15</t>
         </is>
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/cr-belouizdad-khenchela/Q56UOzdJ/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/es-ben-aknoun-us-souf/Q5UxZKJQ/</t>
         </is>
       </c>
     </row>
@@ -2781,71 +2781,71 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>El Bayadh</t>
+          <t>CR Belouizdad</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>ASO Chlef</t>
+          <t>Khenchela</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J26" t="n">
-        <v>1.79</v>
+        <v>1.46</v>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>07/10/2023 10:13</t>
+          <t>06/10/2023 04:56</t>
         </is>
       </c>
       <c r="L26" t="n">
-        <v>2.01</v>
+        <v>1.41</v>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>07/10/2023 14:14</t>
+          <t>07/10/2023 16:01</t>
         </is>
       </c>
       <c r="N26" t="n">
-        <v>3.23</v>
+        <v>4.01</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>07/10/2023 10:13</t>
+          <t>06/10/2023 04:56</t>
         </is>
       </c>
       <c r="P26" t="n">
-        <v>3.1</v>
+        <v>4.17</v>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>07/10/2023 16:16</t>
+          <t>07/10/2023 16:42</t>
         </is>
       </c>
       <c r="R26" t="n">
-        <v>4.85</v>
+        <v>7.72</v>
       </c>
       <c r="S26" t="inlineStr">
         <is>
-          <t>07/10/2023 10:13</t>
+          <t>06/10/2023 04:56</t>
         </is>
       </c>
       <c r="T26" t="n">
-        <v>4.24</v>
+        <v>9.550000000000001</v>
       </c>
       <c r="U26" t="inlineStr">
         <is>
-          <t>07/10/2023 16:40</t>
+          <t>07/10/2023 16:42</t>
         </is>
       </c>
       <c r="V26" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-aso-chlef/pjB9Tbsl/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/cr-belouizdad-khenchela/Q56UOzdJ/</t>
         </is>
       </c>
     </row>
@@ -2873,71 +2873,71 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Ben Aknoun</t>
+          <t>El Bayadh</t>
         </is>
       </c>
       <c r="G27" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>ASO Chlef</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
         <v>0</v>
       </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>US Souf</t>
-        </is>
-      </c>
-      <c r="I27" t="n">
-        <v>1</v>
-      </c>
       <c r="J27" t="n">
-        <v>1.37</v>
+        <v>1.79</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>05/10/2023 09:12</t>
+          <t>07/10/2023 10:13</t>
         </is>
       </c>
       <c r="L27" t="n">
-        <v>1.84</v>
+        <v>2.01</v>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>07/10/2023 11:15</t>
+          <t>07/10/2023 14:14</t>
         </is>
       </c>
       <c r="N27" t="n">
-        <v>4.23</v>
+        <v>3.23</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>05/10/2023 09:12</t>
+          <t>07/10/2023 10:13</t>
         </is>
       </c>
       <c r="P27" t="n">
-        <v>3.29</v>
+        <v>3.1</v>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>07/10/2023 14:50</t>
+          <t>07/10/2023 16:16</t>
         </is>
       </c>
       <c r="R27" t="n">
-        <v>6.79</v>
+        <v>4.85</v>
       </c>
       <c r="S27" t="inlineStr">
         <is>
-          <t>05/10/2023 09:12</t>
+          <t>07/10/2023 10:13</t>
         </is>
       </c>
       <c r="T27" t="n">
-        <v>4.65</v>
+        <v>4.24</v>
       </c>
       <c r="U27" t="inlineStr">
         <is>
-          <t>07/10/2023 11:15</t>
+          <t>07/10/2023 16:40</t>
         </is>
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/es-ben-aknoun-us-souf/Q5UxZKJQ/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-aso-chlef/pjB9Tbsl/</t>
         </is>
       </c>
     </row>
@@ -3609,71 +3609,71 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Khenchela</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Biskra</t>
+          <t>Ben Aknoun</t>
         </is>
       </c>
       <c r="I35" t="n">
         <v>1</v>
       </c>
       <c r="J35" t="n">
-        <v>1.74</v>
+        <v>1.61</v>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>10/11/2023 03:13</t>
+          <t>11/11/2023 10:12</t>
         </is>
       </c>
       <c r="L35" t="n">
-        <v>1.29</v>
+        <v>1.62</v>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>11/11/2023 10:24</t>
+          <t>11/11/2023 14:48</t>
         </is>
       </c>
       <c r="N35" t="n">
-        <v>3.19</v>
+        <v>3.51</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>10/11/2023 03:13</t>
+          <t>11/11/2023 10:12</t>
         </is>
       </c>
       <c r="P35" t="n">
-        <v>4.87</v>
+        <v>3.56</v>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>11/11/2023 14:54</t>
+          <t>11/11/2023 14:48</t>
         </is>
       </c>
       <c r="R35" t="n">
-        <v>4.9</v>
+        <v>5.97</v>
       </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>10/11/2023 03:13</t>
+          <t>11/11/2023 10:12</t>
         </is>
       </c>
       <c r="T35" t="n">
-        <v>13.77</v>
+        <v>6.3</v>
       </c>
       <c r="U35" t="inlineStr">
         <is>
-          <t>11/11/2023 14:54</t>
+          <t>11/11/2023 14:48</t>
         </is>
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-biskra/GbL62yef/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-es-ben-aknoun/lCJE0FP6/</t>
         </is>
       </c>
     </row>
@@ -3701,71 +3701,71 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Magra</t>
+          <t>Khenchela</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Ben Aknoun</t>
+          <t>Biskra</t>
         </is>
       </c>
       <c r="I36" t="n">
         <v>1</v>
       </c>
       <c r="J36" t="n">
-        <v>1.61</v>
+        <v>1.74</v>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>11/11/2023 10:12</t>
+          <t>10/11/2023 03:13</t>
         </is>
       </c>
       <c r="L36" t="n">
-        <v>1.62</v>
+        <v>1.29</v>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>11/11/2023 14:48</t>
+          <t>11/11/2023 10:24</t>
         </is>
       </c>
       <c r="N36" t="n">
-        <v>3.51</v>
+        <v>3.19</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>11/11/2023 10:12</t>
+          <t>10/11/2023 03:13</t>
         </is>
       </c>
       <c r="P36" t="n">
-        <v>3.56</v>
+        <v>4.87</v>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>11/11/2023 14:48</t>
+          <t>11/11/2023 14:54</t>
         </is>
       </c>
       <c r="R36" t="n">
-        <v>5.97</v>
+        <v>4.9</v>
       </c>
       <c r="S36" t="inlineStr">
         <is>
-          <t>11/11/2023 10:12</t>
+          <t>10/11/2023 03:13</t>
         </is>
       </c>
       <c r="T36" t="n">
-        <v>6.3</v>
+        <v>13.77</v>
       </c>
       <c r="U36" t="inlineStr">
         <is>
-          <t>11/11/2023 14:48</t>
+          <t>11/11/2023 14:54</t>
         </is>
       </c>
       <c r="V36" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-es-ben-aknoun/lCJE0FP6/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-biskra/GbL62yef/</t>
         </is>
       </c>
     </row>
@@ -4502,6 +4502,374 @@
       <c r="V44" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/algeria/ligue-1/mc-alger-saoura/C8qhEYg6/</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E45" s="2" t="n">
+        <v>45248.625</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Ben Aknoun</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Paradou</t>
+        </is>
+      </c>
+      <c r="I45" t="n">
+        <v>1</v>
+      </c>
+      <c r="J45" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>17/11/2023 01:11</t>
+        </is>
+      </c>
+      <c r="L45" t="n">
+        <v>4.23</v>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>18/11/2023 14:54</t>
+        </is>
+      </c>
+      <c r="N45" t="n">
+        <v>2.72</v>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>17/11/2023 01:11</t>
+        </is>
+      </c>
+      <c r="P45" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>18/11/2023 14:56</t>
+        </is>
+      </c>
+      <c r="R45" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>17/11/2023 01:11</t>
+        </is>
+      </c>
+      <c r="T45" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t>18/11/2023 14:54</t>
+        </is>
+      </c>
+      <c r="V45" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/es-ben-aknoun-paradou/QBmdDh9C/</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E46" s="2" t="n">
+        <v>45248.70833333334</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>ASO Chlef</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>2</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>ES Setif</t>
+        </is>
+      </c>
+      <c r="I46" t="n">
+        <v>1</v>
+      </c>
+      <c r="J46" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>17/11/2023 01:11</t>
+        </is>
+      </c>
+      <c r="L46" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>18/11/2023 16:56</t>
+        </is>
+      </c>
+      <c r="N46" t="n">
+        <v>3.19</v>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>17/11/2023 01:11</t>
+        </is>
+      </c>
+      <c r="P46" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>18/11/2023 16:58</t>
+        </is>
+      </c>
+      <c r="R46" t="n">
+        <v>4.76</v>
+      </c>
+      <c r="S46" t="inlineStr">
+        <is>
+          <t>17/11/2023 01:11</t>
+        </is>
+      </c>
+      <c r="T46" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>18/11/2023 16:58</t>
+        </is>
+      </c>
+      <c r="V46" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/aso-chlef-es-setif/KYn0CCOI/</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E47" s="2" t="n">
+        <v>45248.75</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Biskra</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>1</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>USM Alger</t>
+        </is>
+      </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" t="n">
+        <v>2.02</v>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>17/11/2023 01:11</t>
+        </is>
+      </c>
+      <c r="L47" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>18/11/2023 17:24</t>
+        </is>
+      </c>
+      <c r="N47" t="n">
+        <v>2.93</v>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>17/11/2023 01:11</t>
+        </is>
+      </c>
+      <c r="P47" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>18/11/2023 16:09</t>
+        </is>
+      </c>
+      <c r="R47" t="n">
+        <v>3.79</v>
+      </c>
+      <c r="S47" t="inlineStr">
+        <is>
+          <t>17/11/2023 01:11</t>
+        </is>
+      </c>
+      <c r="T47" t="n">
+        <v>2.87</v>
+      </c>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>18/11/2023 17:24</t>
+        </is>
+      </c>
+      <c r="V47" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-usm-alger/bPo4BWwP/</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E48" s="2" t="n">
+        <v>45249.79166666666</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>CR Belouizdad</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>1</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Kabylie</t>
+        </is>
+      </c>
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" t="n">
+        <v>1.86</v>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>18/11/2023 07:12</t>
+        </is>
+      </c>
+      <c r="L48" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>19/11/2023 18:32</t>
+        </is>
+      </c>
+      <c r="N48" t="n">
+        <v>3</v>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>18/11/2023 07:12</t>
+        </is>
+      </c>
+      <c r="P48" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>19/11/2023 18:32</t>
+        </is>
+      </c>
+      <c r="R48" t="n">
+        <v>4.32</v>
+      </c>
+      <c r="S48" t="inlineStr">
+        <is>
+          <t>18/11/2023 07:12</t>
+        </is>
+      </c>
+      <c r="T48" t="n">
+        <v>6.71</v>
+      </c>
+      <c r="U48" t="inlineStr">
+        <is>
+          <t>19/11/2023 18:32</t>
+        </is>
+      </c>
+      <c r="V48" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/cr-belouizdad-kabylie/xAHpKOsP/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 24-11-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/algeria_ligue-1_2023-2024.xlsx
+++ b/2023/algeria_ligue-1_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V48"/>
+  <dimension ref="A1:V50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2781,71 +2781,71 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>CR Belouizdad</t>
+          <t>El Bayadh</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Khenchela</t>
+          <t>ASO Chlef</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>1.46</v>
+        <v>1.79</v>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>06/10/2023 04:56</t>
+          <t>07/10/2023 10:13</t>
         </is>
       </c>
       <c r="L26" t="n">
-        <v>1.41</v>
+        <v>2.01</v>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>07/10/2023 16:01</t>
+          <t>07/10/2023 14:14</t>
         </is>
       </c>
       <c r="N26" t="n">
-        <v>4.01</v>
+        <v>3.23</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>06/10/2023 04:56</t>
+          <t>07/10/2023 10:13</t>
         </is>
       </c>
       <c r="P26" t="n">
-        <v>4.17</v>
+        <v>3.1</v>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>07/10/2023 16:42</t>
+          <t>07/10/2023 16:16</t>
         </is>
       </c>
       <c r="R26" t="n">
-        <v>7.72</v>
+        <v>4.85</v>
       </c>
       <c r="S26" t="inlineStr">
         <is>
-          <t>06/10/2023 04:56</t>
+          <t>07/10/2023 10:13</t>
         </is>
       </c>
       <c r="T26" t="n">
-        <v>9.550000000000001</v>
+        <v>4.24</v>
       </c>
       <c r="U26" t="inlineStr">
         <is>
-          <t>07/10/2023 16:42</t>
+          <t>07/10/2023 16:40</t>
         </is>
       </c>
       <c r="V26" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/cr-belouizdad-khenchela/Q56UOzdJ/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-aso-chlef/pjB9Tbsl/</t>
         </is>
       </c>
     </row>
@@ -2873,71 +2873,71 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>El Bayadh</t>
+          <t>CR Belouizdad</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>ASO Chlef</t>
+          <t>Khenchela</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J27" t="n">
-        <v>1.79</v>
+        <v>1.46</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>07/10/2023 10:13</t>
+          <t>06/10/2023 04:56</t>
         </is>
       </c>
       <c r="L27" t="n">
-        <v>2.01</v>
+        <v>1.41</v>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>07/10/2023 14:14</t>
+          <t>07/10/2023 16:01</t>
         </is>
       </c>
       <c r="N27" t="n">
-        <v>3.23</v>
+        <v>4.01</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>07/10/2023 10:13</t>
+          <t>06/10/2023 04:56</t>
         </is>
       </c>
       <c r="P27" t="n">
-        <v>3.1</v>
+        <v>4.17</v>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>07/10/2023 16:16</t>
+          <t>07/10/2023 16:42</t>
         </is>
       </c>
       <c r="R27" t="n">
-        <v>4.85</v>
+        <v>7.72</v>
       </c>
       <c r="S27" t="inlineStr">
         <is>
-          <t>07/10/2023 10:13</t>
+          <t>06/10/2023 04:56</t>
         </is>
       </c>
       <c r="T27" t="n">
-        <v>4.24</v>
+        <v>9.550000000000001</v>
       </c>
       <c r="U27" t="inlineStr">
         <is>
-          <t>07/10/2023 16:40</t>
+          <t>07/10/2023 16:42</t>
         </is>
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-aso-chlef/pjB9Tbsl/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/cr-belouizdad-khenchela/Q56UOzdJ/</t>
         </is>
       </c>
     </row>
@@ -3609,71 +3609,71 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Magra</t>
+          <t>Khenchela</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Ben Aknoun</t>
+          <t>Biskra</t>
         </is>
       </c>
       <c r="I35" t="n">
         <v>1</v>
       </c>
       <c r="J35" t="n">
-        <v>1.61</v>
+        <v>1.74</v>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>11/11/2023 10:12</t>
+          <t>10/11/2023 03:13</t>
         </is>
       </c>
       <c r="L35" t="n">
-        <v>1.62</v>
+        <v>1.29</v>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>11/11/2023 14:48</t>
+          <t>11/11/2023 10:24</t>
         </is>
       </c>
       <c r="N35" t="n">
-        <v>3.51</v>
+        <v>3.19</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>11/11/2023 10:12</t>
+          <t>10/11/2023 03:13</t>
         </is>
       </c>
       <c r="P35" t="n">
-        <v>3.56</v>
+        <v>4.87</v>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>11/11/2023 14:48</t>
+          <t>11/11/2023 14:54</t>
         </is>
       </c>
       <c r="R35" t="n">
-        <v>5.97</v>
+        <v>4.9</v>
       </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>11/11/2023 10:12</t>
+          <t>10/11/2023 03:13</t>
         </is>
       </c>
       <c r="T35" t="n">
-        <v>6.3</v>
+        <v>13.77</v>
       </c>
       <c r="U35" t="inlineStr">
         <is>
-          <t>11/11/2023 14:48</t>
+          <t>11/11/2023 14:54</t>
         </is>
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-es-ben-aknoun/lCJE0FP6/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-biskra/GbL62yef/</t>
         </is>
       </c>
     </row>
@@ -3701,71 +3701,71 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Khenchela</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Biskra</t>
+          <t>Ben Aknoun</t>
         </is>
       </c>
       <c r="I36" t="n">
         <v>1</v>
       </c>
       <c r="J36" t="n">
-        <v>1.74</v>
+        <v>1.61</v>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>10/11/2023 03:13</t>
+          <t>11/11/2023 10:12</t>
         </is>
       </c>
       <c r="L36" t="n">
-        <v>1.29</v>
+        <v>1.62</v>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>11/11/2023 10:24</t>
+          <t>11/11/2023 14:48</t>
         </is>
       </c>
       <c r="N36" t="n">
-        <v>3.19</v>
+        <v>3.51</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>10/11/2023 03:13</t>
+          <t>11/11/2023 10:12</t>
         </is>
       </c>
       <c r="P36" t="n">
-        <v>4.87</v>
+        <v>3.56</v>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>11/11/2023 14:54</t>
+          <t>11/11/2023 14:48</t>
         </is>
       </c>
       <c r="R36" t="n">
-        <v>4.9</v>
+        <v>5.97</v>
       </c>
       <c r="S36" t="inlineStr">
         <is>
-          <t>10/11/2023 03:13</t>
+          <t>11/11/2023 10:12</t>
         </is>
       </c>
       <c r="T36" t="n">
-        <v>13.77</v>
+        <v>6.3</v>
       </c>
       <c r="U36" t="inlineStr">
         <is>
-          <t>11/11/2023 14:54</t>
+          <t>11/11/2023 14:48</t>
         </is>
       </c>
       <c r="V36" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-biskra/GbL62yef/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-es-ben-aknoun/lCJE0FP6/</t>
         </is>
       </c>
     </row>
@@ -4870,6 +4870,190 @@
       <c r="V48" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/algeria/ligue-1/cr-belouizdad-kabylie/xAHpKOsP/</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E49" s="2" t="n">
+        <v>45254.63541666666</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Magra</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>1</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>El Bayadh</t>
+        </is>
+      </c>
+      <c r="I49" t="n">
+        <v>1</v>
+      </c>
+      <c r="J49" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>23/11/2023 07:47</t>
+        </is>
+      </c>
+      <c r="L49" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>24/11/2023 14:19</t>
+        </is>
+      </c>
+      <c r="N49" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>23/11/2023 07:47</t>
+        </is>
+      </c>
+      <c r="P49" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>24/11/2023 15:12</t>
+        </is>
+      </c>
+      <c r="R49" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="S49" t="inlineStr">
+        <is>
+          <t>23/11/2023 07:47</t>
+        </is>
+      </c>
+      <c r="T49" t="n">
+        <v>4.06</v>
+      </c>
+      <c r="U49" t="inlineStr">
+        <is>
+          <t>24/11/2023 14:19</t>
+        </is>
+      </c>
+      <c r="V49" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-el-bayadh/jog1n073/</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E50" s="2" t="n">
+        <v>45254.63541666666</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Paradou</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Constantine</t>
+        </is>
+      </c>
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>23/11/2023 07:47</t>
+        </is>
+      </c>
+      <c r="L50" t="n">
+        <v>1.98</v>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>24/11/2023 15:00</t>
+        </is>
+      </c>
+      <c r="N50" t="n">
+        <v>3.27</v>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>23/11/2023 07:47</t>
+        </is>
+      </c>
+      <c r="P50" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>24/11/2023 15:00</t>
+        </is>
+      </c>
+      <c r="R50" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="S50" t="inlineStr">
+        <is>
+          <t>23/11/2023 07:47</t>
+        </is>
+      </c>
+      <c r="T50" t="n">
+        <v>4.37</v>
+      </c>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>24/11/2023 15:00</t>
+        </is>
+      </c>
+      <c r="V50" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/paradou-constantine/dOgcmthc/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 26-11-2023 20:30
</commit_message>
<xml_diff>
--- a/2023/algeria_ligue-1_2023-2024.xlsx
+++ b/2023/algeria_ligue-1_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V50"/>
+  <dimension ref="A1:V54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Constantine</t>
+          <t>Ben Aknoun</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -1133,63 +1133,63 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>MC Alger</t>
+          <t>ASO Chlef</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" t="n">
-        <v>1.98</v>
+        <v>2.81</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>21/09/2023 05:12</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>3.68</v>
+        <v>2.51</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>22/09/2023 16:51</t>
+          <t>22/09/2023 16:00</t>
         </is>
       </c>
       <c r="N8" t="n">
-        <v>2.89</v>
+        <v>3.04</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>21/09/2023 05:12</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="P8" t="n">
-        <v>2.92</v>
+        <v>3.06</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>22/09/2023 16:51</t>
+          <t>22/09/2023 16:34</t>
         </is>
       </c>
       <c r="R8" t="n">
-        <v>3.97</v>
+        <v>2.64</v>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>21/09/2023 05:12</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="T8" t="n">
-        <v>2.26</v>
+        <v>3.01</v>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>22/09/2023 16:51</t>
+          <t>22/09/2023 16:00</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-mc-alger/Eoq3MszL/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/es-ben-aknoun-aso-chlef/WMgbNNKE/</t>
         </is>
       </c>
     </row>
@@ -1217,7 +1217,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Ben Aknoun</t>
+          <t>Constantine</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -1225,63 +1225,63 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>ASO Chlef</t>
+          <t>MC Alger</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>2.81</v>
+        <v>1.98</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>21/09/2023 05:12</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>2.51</v>
+        <v>3.68</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>22/09/2023 16:00</t>
+          <t>22/09/2023 16:51</t>
         </is>
       </c>
       <c r="N9" t="n">
-        <v>3.04</v>
+        <v>2.89</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>21/09/2023 05:12</t>
         </is>
       </c>
       <c r="P9" t="n">
-        <v>3.06</v>
+        <v>2.92</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>22/09/2023 16:34</t>
+          <t>22/09/2023 16:51</t>
         </is>
       </c>
       <c r="R9" t="n">
-        <v>2.64</v>
+        <v>3.97</v>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>21/09/2023 05:12</t>
         </is>
       </c>
       <c r="T9" t="n">
-        <v>3.01</v>
+        <v>2.26</v>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>22/09/2023 16:00</t>
+          <t>22/09/2023 16:51</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/es-ben-aknoun-aso-chlef/WMgbNNKE/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-mc-alger/Eoq3MszL/</t>
         </is>
       </c>
     </row>
@@ -1493,71 +1493,71 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Biskra</t>
+          <t>Oran</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Saoura</t>
         </is>
       </c>
       <c r="I12" t="n">
         <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>1.71</v>
+        <v>2.54</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>22/09/2023 15:13</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="L12" t="n">
-        <v>1.65</v>
+        <v>2.34</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>23/09/2023 19:13</t>
+          <t>23/09/2023 18:03</t>
         </is>
       </c>
       <c r="N12" t="n">
-        <v>3.22</v>
+        <v>2.65</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>22/09/2023 15:13</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="P12" t="n">
-        <v>3.47</v>
+        <v>2.71</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>23/09/2023 19:13</t>
+          <t>23/09/2023 18:03</t>
         </is>
       </c>
       <c r="R12" t="n">
-        <v>4.87</v>
+        <v>3.11</v>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>22/09/2023 15:13</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="T12" t="n">
-        <v>6.17</v>
+        <v>3.84</v>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>23/09/2023 19:13</t>
+          <t>23/09/2023 18:03</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-us-souf/KYnDaKS7/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-saoura/YyyeO358/</t>
         </is>
       </c>
     </row>
@@ -1585,71 +1585,71 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Oran</t>
+          <t>Biskra</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Saoura</t>
+          <t>US Souf</t>
         </is>
       </c>
       <c r="I13" t="n">
         <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>2.54</v>
+        <v>1.71</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>22/09/2023 15:13</t>
         </is>
       </c>
       <c r="L13" t="n">
-        <v>2.34</v>
+        <v>1.65</v>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>23/09/2023 18:03</t>
+          <t>23/09/2023 19:13</t>
         </is>
       </c>
       <c r="N13" t="n">
-        <v>2.65</v>
+        <v>3.22</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>22/09/2023 15:13</t>
         </is>
       </c>
       <c r="P13" t="n">
-        <v>2.71</v>
+        <v>3.47</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>23/09/2023 18:03</t>
+          <t>23/09/2023 19:13</t>
         </is>
       </c>
       <c r="R13" t="n">
-        <v>3.11</v>
+        <v>4.87</v>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>22/09/2023 15:13</t>
         </is>
       </c>
       <c r="T13" t="n">
-        <v>3.84</v>
+        <v>6.17</v>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>23/09/2023 18:03</t>
+          <t>23/09/2023 19:13</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-saoura/YyyeO358/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-us-souf/KYnDaKS7/</t>
         </is>
       </c>
     </row>
@@ -2689,71 +2689,71 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Ben Aknoun</t>
+          <t>CR Belouizdad</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Khenchela</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J25" t="n">
-        <v>1.37</v>
+        <v>1.46</v>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>05/10/2023 09:12</t>
+          <t>06/10/2023 04:56</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>1.84</v>
+        <v>1.41</v>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>07/10/2023 11:15</t>
+          <t>07/10/2023 16:01</t>
         </is>
       </c>
       <c r="N25" t="n">
-        <v>4.23</v>
+        <v>4.01</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>05/10/2023 09:12</t>
+          <t>06/10/2023 04:56</t>
         </is>
       </c>
       <c r="P25" t="n">
-        <v>3.29</v>
+        <v>4.17</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>07/10/2023 14:50</t>
+          <t>07/10/2023 16:42</t>
         </is>
       </c>
       <c r="R25" t="n">
-        <v>6.79</v>
+        <v>7.72</v>
       </c>
       <c r="S25" t="inlineStr">
         <is>
-          <t>05/10/2023 09:12</t>
+          <t>06/10/2023 04:56</t>
         </is>
       </c>
       <c r="T25" t="n">
-        <v>4.65</v>
+        <v>9.550000000000001</v>
       </c>
       <c r="U25" t="inlineStr">
         <is>
-          <t>07/10/2023 11:15</t>
+          <t>07/10/2023 16:42</t>
         </is>
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/es-ben-aknoun-us-souf/Q5UxZKJQ/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/cr-belouizdad-khenchela/Q56UOzdJ/</t>
         </is>
       </c>
     </row>
@@ -2873,71 +2873,71 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>CR Belouizdad</t>
+          <t>Ben Aknoun</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Khenchela</t>
+          <t>US Souf</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J27" t="n">
-        <v>1.46</v>
+        <v>1.37</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>06/10/2023 04:56</t>
+          <t>05/10/2023 09:12</t>
         </is>
       </c>
       <c r="L27" t="n">
-        <v>1.41</v>
+        <v>1.84</v>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>07/10/2023 16:01</t>
+          <t>07/10/2023 11:15</t>
         </is>
       </c>
       <c r="N27" t="n">
-        <v>4.01</v>
+        <v>4.23</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>06/10/2023 04:56</t>
+          <t>05/10/2023 09:12</t>
         </is>
       </c>
       <c r="P27" t="n">
-        <v>4.17</v>
+        <v>3.29</v>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>07/10/2023 16:42</t>
+          <t>07/10/2023 14:50</t>
         </is>
       </c>
       <c r="R27" t="n">
-        <v>7.72</v>
+        <v>6.79</v>
       </c>
       <c r="S27" t="inlineStr">
         <is>
-          <t>06/10/2023 04:56</t>
+          <t>05/10/2023 09:12</t>
         </is>
       </c>
       <c r="T27" t="n">
-        <v>9.550000000000001</v>
+        <v>4.65</v>
       </c>
       <c r="U27" t="inlineStr">
         <is>
-          <t>07/10/2023 16:42</t>
+          <t>07/10/2023 11:15</t>
         </is>
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/cr-belouizdad-khenchela/Q56UOzdJ/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/es-ben-aknoun-us-souf/Q5UxZKJQ/</t>
         </is>
       </c>
     </row>
@@ -4161,71 +4161,71 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Constantine</t>
+          <t>El Bayadh</t>
         </is>
       </c>
       <c r="G41" t="n">
+        <v>4</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>US Souf</t>
+        </is>
+      </c>
+      <c r="I41" t="n">
         <v>0</v>
       </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>Magra</t>
-        </is>
-      </c>
-      <c r="I41" t="n">
-        <v>1</v>
-      </c>
       <c r="J41" t="n">
-        <v>1.59</v>
+        <v>1.45</v>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>26/10/2023 04:42</t>
+          <t>16/11/2023 03:42</t>
         </is>
       </c>
       <c r="L41" t="n">
-        <v>1.31</v>
+        <v>1.45</v>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>17/11/2023 15:24</t>
+          <t>17/11/2023 15:18</t>
         </is>
       </c>
       <c r="N41" t="n">
-        <v>3.47</v>
+        <v>3.74</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>26/10/2023 04:42</t>
+          <t>16/11/2023 03:42</t>
         </is>
       </c>
       <c r="P41" t="n">
-        <v>4.98</v>
+        <v>4.01</v>
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>17/11/2023 15:24</t>
+          <t>17/11/2023 15:18</t>
         </is>
       </c>
       <c r="R41" t="n">
-        <v>5.42</v>
+        <v>7.38</v>
       </c>
       <c r="S41" t="inlineStr">
         <is>
-          <t>26/10/2023 04:42</t>
+          <t>16/11/2023 03:42</t>
         </is>
       </c>
       <c r="T41" t="n">
-        <v>10.79</v>
+        <v>8.609999999999999</v>
       </c>
       <c r="U41" t="inlineStr">
         <is>
-          <t>17/11/2023 15:24</t>
+          <t>17/11/2023 15:18</t>
         </is>
       </c>
       <c r="V41" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-magra/jgeqGfPg/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-us-souf/UqfmFEv0/</t>
         </is>
       </c>
     </row>
@@ -4253,71 +4253,71 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>El Bayadh</t>
+          <t>Constantine</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" t="n">
-        <v>1.45</v>
+        <v>1.59</v>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>16/11/2023 03:42</t>
+          <t>26/10/2023 04:42</t>
         </is>
       </c>
       <c r="L42" t="n">
-        <v>1.45</v>
+        <v>1.31</v>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>17/11/2023 15:18</t>
+          <t>17/11/2023 15:24</t>
         </is>
       </c>
       <c r="N42" t="n">
-        <v>3.74</v>
+        <v>3.47</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>16/11/2023 03:42</t>
+          <t>26/10/2023 04:42</t>
         </is>
       </c>
       <c r="P42" t="n">
-        <v>4.01</v>
+        <v>4.98</v>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>17/11/2023 15:18</t>
+          <t>17/11/2023 15:24</t>
         </is>
       </c>
       <c r="R42" t="n">
-        <v>7.38</v>
+        <v>5.42</v>
       </c>
       <c r="S42" t="inlineStr">
         <is>
-          <t>16/11/2023 03:42</t>
+          <t>26/10/2023 04:42</t>
         </is>
       </c>
       <c r="T42" t="n">
-        <v>8.609999999999999</v>
+        <v>10.79</v>
       </c>
       <c r="U42" t="inlineStr">
         <is>
-          <t>17/11/2023 15:18</t>
+          <t>17/11/2023 15:24</t>
         </is>
       </c>
       <c r="V42" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-us-souf/UqfmFEv0/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-magra/jgeqGfPg/</t>
         </is>
       </c>
     </row>
@@ -5054,6 +5054,374 @@
       <c r="V50" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/algeria/ligue-1/paradou-constantine/dOgcmthc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E51" s="2" t="n">
+        <v>45255.625</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Khenchela</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Ben Aknoun</t>
+        </is>
+      </c>
+      <c r="I51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>24/11/2023 03:13</t>
+        </is>
+      </c>
+      <c r="L51" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>25/11/2023 14:56</t>
+        </is>
+      </c>
+      <c r="N51" t="n">
+        <v>4.19</v>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>24/11/2023 03:13</t>
+        </is>
+      </c>
+      <c r="P51" t="n">
+        <v>4.72</v>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>25/11/2023 14:56</t>
+        </is>
+      </c>
+      <c r="R51" t="n">
+        <v>7.76</v>
+      </c>
+      <c r="S51" t="inlineStr">
+        <is>
+          <t>24/11/2023 03:13</t>
+        </is>
+      </c>
+      <c r="T51" t="n">
+        <v>11.86</v>
+      </c>
+      <c r="U51" t="inlineStr">
+        <is>
+          <t>25/11/2023 14:56</t>
+        </is>
+      </c>
+      <c r="V51" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-es-ben-aknoun/bwyflMxi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E52" s="2" t="n">
+        <v>45255.625</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>US Souf</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>3</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>MC Alger</t>
+        </is>
+      </c>
+      <c r="I52" t="n">
+        <v>4</v>
+      </c>
+      <c r="J52" t="n">
+        <v>4.45</v>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>24/11/2023 03:13</t>
+        </is>
+      </c>
+      <c r="L52" t="n">
+        <v>5.84</v>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>25/11/2023 14:56</t>
+        </is>
+      </c>
+      <c r="N52" t="n">
+        <v>2.95</v>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>24/11/2023 03:13</t>
+        </is>
+      </c>
+      <c r="P52" t="n">
+        <v>3.36</v>
+      </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>25/11/2023 14:56</t>
+        </is>
+      </c>
+      <c r="R52" t="n">
+        <v>1.89</v>
+      </c>
+      <c r="S52" t="inlineStr">
+        <is>
+          <t>24/11/2023 03:13</t>
+        </is>
+      </c>
+      <c r="T52" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="U52" t="inlineStr">
+        <is>
+          <t>25/11/2023 14:56</t>
+        </is>
+      </c>
+      <c r="V52" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-mc-alger/Uyh5oKM9/</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E53" s="2" t="n">
+        <v>45255.69791666666</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Kabylie</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>1</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Biskra</t>
+        </is>
+      </c>
+      <c r="I53" t="n">
+        <v>1</v>
+      </c>
+      <c r="J53" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>24/11/2023 07:24</t>
+        </is>
+      </c>
+      <c r="L53" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>25/11/2023 16:40</t>
+        </is>
+      </c>
+      <c r="N53" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>24/11/2023 07:24</t>
+        </is>
+      </c>
+      <c r="P53" t="n">
+        <v>3.59</v>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>25/11/2023 16:40</t>
+        </is>
+      </c>
+      <c r="R53" t="n">
+        <v>6.95</v>
+      </c>
+      <c r="S53" t="inlineStr">
+        <is>
+          <t>24/11/2023 07:24</t>
+        </is>
+      </c>
+      <c r="T53" t="n">
+        <v>8.02</v>
+      </c>
+      <c r="U53" t="inlineStr">
+        <is>
+          <t>25/11/2023 16:40</t>
+        </is>
+      </c>
+      <c r="V53" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/kabylie-biskra/Q3oEqbiM/</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E54" s="2" t="n">
+        <v>45255.73958333334</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Saoura</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>3</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>ASO Chlef</t>
+        </is>
+      </c>
+      <c r="I54" t="n">
+        <v>2</v>
+      </c>
+      <c r="J54" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>24/11/2023 07:24</t>
+        </is>
+      </c>
+      <c r="L54" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>25/11/2023 17:40</t>
+        </is>
+      </c>
+      <c r="N54" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>24/11/2023 07:24</t>
+        </is>
+      </c>
+      <c r="P54" t="n">
+        <v>3.07</v>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>25/11/2023 17:42</t>
+        </is>
+      </c>
+      <c r="R54" t="n">
+        <v>5.52</v>
+      </c>
+      <c r="S54" t="inlineStr">
+        <is>
+          <t>24/11/2023 07:24</t>
+        </is>
+      </c>
+      <c r="T54" t="n">
+        <v>4.06</v>
+      </c>
+      <c r="U54" t="inlineStr">
+        <is>
+          <t>25/11/2023 17:40</t>
+        </is>
+      </c>
+      <c r="V54" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/saoura-aso-chlef/nDnApvxG/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 01-12-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/algeria_ligue-1_2023-2024.xlsx
+++ b/2023/algeria_ligue-1_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V54"/>
+  <dimension ref="A1:V57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Ben Aknoun</t>
+          <t>Constantine</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -1133,63 +1133,63 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>ASO Chlef</t>
+          <t>MC Alger</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>2.81</v>
+        <v>1.98</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>21/09/2023 05:12</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>2.51</v>
+        <v>3.68</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>22/09/2023 16:00</t>
+          <t>22/09/2023 16:51</t>
         </is>
       </c>
       <c r="N8" t="n">
-        <v>3.04</v>
+        <v>2.89</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>21/09/2023 05:12</t>
         </is>
       </c>
       <c r="P8" t="n">
-        <v>3.06</v>
+        <v>2.92</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>22/09/2023 16:34</t>
+          <t>22/09/2023 16:51</t>
         </is>
       </c>
       <c r="R8" t="n">
-        <v>2.64</v>
+        <v>3.97</v>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>21/09/2023 05:12</t>
         </is>
       </c>
       <c r="T8" t="n">
-        <v>3.01</v>
+        <v>2.26</v>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>22/09/2023 16:00</t>
+          <t>22/09/2023 16:51</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/es-ben-aknoun-aso-chlef/WMgbNNKE/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-mc-alger/Eoq3MszL/</t>
         </is>
       </c>
     </row>
@@ -1217,7 +1217,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Constantine</t>
+          <t>Ben Aknoun</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -1225,63 +1225,63 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>MC Alger</t>
+          <t>ASO Chlef</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" t="n">
-        <v>1.98</v>
+        <v>2.81</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>21/09/2023 05:12</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>3.68</v>
+        <v>2.51</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>22/09/2023 16:51</t>
+          <t>22/09/2023 16:00</t>
         </is>
       </c>
       <c r="N9" t="n">
-        <v>2.89</v>
+        <v>3.04</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>21/09/2023 05:12</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="P9" t="n">
-        <v>2.92</v>
+        <v>3.06</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>22/09/2023 16:51</t>
+          <t>22/09/2023 16:34</t>
         </is>
       </c>
       <c r="R9" t="n">
-        <v>3.97</v>
+        <v>2.64</v>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>21/09/2023 05:12</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="T9" t="n">
-        <v>2.26</v>
+        <v>3.01</v>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>22/09/2023 16:51</t>
+          <t>22/09/2023 16:00</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-mc-alger/Eoq3MszL/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/es-ben-aknoun-aso-chlef/WMgbNNKE/</t>
         </is>
       </c>
     </row>
@@ -1493,71 +1493,71 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Oran</t>
+          <t>Biskra</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Saoura</t>
+          <t>US Souf</t>
         </is>
       </c>
       <c r="I12" t="n">
         <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>2.54</v>
+        <v>1.71</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>22/09/2023 15:13</t>
         </is>
       </c>
       <c r="L12" t="n">
-        <v>2.34</v>
+        <v>1.65</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>23/09/2023 18:03</t>
+          <t>23/09/2023 19:13</t>
         </is>
       </c>
       <c r="N12" t="n">
-        <v>2.65</v>
+        <v>3.22</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>22/09/2023 15:13</t>
         </is>
       </c>
       <c r="P12" t="n">
-        <v>2.71</v>
+        <v>3.47</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>23/09/2023 18:03</t>
+          <t>23/09/2023 19:13</t>
         </is>
       </c>
       <c r="R12" t="n">
-        <v>3.11</v>
+        <v>4.87</v>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>22/09/2023 15:13</t>
         </is>
       </c>
       <c r="T12" t="n">
-        <v>3.84</v>
+        <v>6.17</v>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>23/09/2023 18:03</t>
+          <t>23/09/2023 19:13</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-saoura/YyyeO358/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-us-souf/KYnDaKS7/</t>
         </is>
       </c>
     </row>
@@ -1585,71 +1585,71 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Biskra</t>
+          <t>Oran</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Saoura</t>
         </is>
       </c>
       <c r="I13" t="n">
         <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>1.71</v>
+        <v>2.54</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>22/09/2023 15:13</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="L13" t="n">
-        <v>1.65</v>
+        <v>2.34</v>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>23/09/2023 19:13</t>
+          <t>23/09/2023 18:03</t>
         </is>
       </c>
       <c r="N13" t="n">
-        <v>3.22</v>
+        <v>2.65</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>22/09/2023 15:13</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="P13" t="n">
-        <v>3.47</v>
+        <v>2.71</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>23/09/2023 19:13</t>
+          <t>23/09/2023 18:03</t>
         </is>
       </c>
       <c r="R13" t="n">
-        <v>4.87</v>
+        <v>3.11</v>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>22/09/2023 15:13</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="T13" t="n">
-        <v>6.17</v>
+        <v>3.84</v>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>23/09/2023 19:13</t>
+          <t>23/09/2023 18:03</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-us-souf/KYnDaKS7/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-saoura/YyyeO358/</t>
         </is>
       </c>
     </row>
@@ -4161,71 +4161,71 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>El Bayadh</t>
+          <t>Constantine</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" t="n">
-        <v>1.45</v>
+        <v>1.59</v>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>16/11/2023 03:42</t>
+          <t>26/10/2023 04:42</t>
         </is>
       </c>
       <c r="L41" t="n">
-        <v>1.45</v>
+        <v>1.31</v>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>17/11/2023 15:18</t>
+          <t>17/11/2023 15:24</t>
         </is>
       </c>
       <c r="N41" t="n">
-        <v>3.74</v>
+        <v>3.47</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>16/11/2023 03:42</t>
+          <t>26/10/2023 04:42</t>
         </is>
       </c>
       <c r="P41" t="n">
-        <v>4.01</v>
+        <v>4.98</v>
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>17/11/2023 15:18</t>
+          <t>17/11/2023 15:24</t>
         </is>
       </c>
       <c r="R41" t="n">
-        <v>7.38</v>
+        <v>5.42</v>
       </c>
       <c r="S41" t="inlineStr">
         <is>
-          <t>16/11/2023 03:42</t>
+          <t>26/10/2023 04:42</t>
         </is>
       </c>
       <c r="T41" t="n">
-        <v>8.609999999999999</v>
+        <v>10.79</v>
       </c>
       <c r="U41" t="inlineStr">
         <is>
-          <t>17/11/2023 15:18</t>
+          <t>17/11/2023 15:24</t>
         </is>
       </c>
       <c r="V41" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-us-souf/UqfmFEv0/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-magra/jgeqGfPg/</t>
         </is>
       </c>
     </row>
@@ -4253,71 +4253,71 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Constantine</t>
+          <t>El Bayadh</t>
         </is>
       </c>
       <c r="G42" t="n">
+        <v>4</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>US Souf</t>
+        </is>
+      </c>
+      <c r="I42" t="n">
         <v>0</v>
       </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>Magra</t>
-        </is>
-      </c>
-      <c r="I42" t="n">
-        <v>1</v>
-      </c>
       <c r="J42" t="n">
-        <v>1.59</v>
+        <v>1.45</v>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>26/10/2023 04:42</t>
+          <t>16/11/2023 03:42</t>
         </is>
       </c>
       <c r="L42" t="n">
-        <v>1.31</v>
+        <v>1.45</v>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>17/11/2023 15:24</t>
+          <t>17/11/2023 15:18</t>
         </is>
       </c>
       <c r="N42" t="n">
-        <v>3.47</v>
+        <v>3.74</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>26/10/2023 04:42</t>
+          <t>16/11/2023 03:42</t>
         </is>
       </c>
       <c r="P42" t="n">
-        <v>4.98</v>
+        <v>4.01</v>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>17/11/2023 15:24</t>
+          <t>17/11/2023 15:18</t>
         </is>
       </c>
       <c r="R42" t="n">
-        <v>5.42</v>
+        <v>7.38</v>
       </c>
       <c r="S42" t="inlineStr">
         <is>
-          <t>26/10/2023 04:42</t>
+          <t>16/11/2023 03:42</t>
         </is>
       </c>
       <c r="T42" t="n">
-        <v>10.79</v>
+        <v>8.609999999999999</v>
       </c>
       <c r="U42" t="inlineStr">
         <is>
-          <t>17/11/2023 15:24</t>
+          <t>17/11/2023 15:18</t>
         </is>
       </c>
       <c r="V42" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-magra/jgeqGfPg/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-us-souf/UqfmFEv0/</t>
         </is>
       </c>
     </row>
@@ -5422,6 +5422,282 @@
       <c r="V54" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/algeria/ligue-1/saoura-aso-chlef/nDnApvxG/</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E55" s="2" t="n">
+        <v>45261.63541666666</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>El Bayadh</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>1</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>Paradou</t>
+        </is>
+      </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>30/11/2023 07:50</t>
+        </is>
+      </c>
+      <c r="L55" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>01/12/2023 15:11</t>
+        </is>
+      </c>
+      <c r="N55" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>30/11/2023 07:50</t>
+        </is>
+      </c>
+      <c r="P55" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>01/12/2023 15:11</t>
+        </is>
+      </c>
+      <c r="R55" t="n">
+        <v>4.28</v>
+      </c>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>30/11/2023 07:50</t>
+        </is>
+      </c>
+      <c r="T55" t="n">
+        <v>4.27</v>
+      </c>
+      <c r="U55" t="inlineStr">
+        <is>
+          <t>01/12/2023 15:11</t>
+        </is>
+      </c>
+      <c r="V55" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-paradou/U99Qf5Er/</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E56" s="2" t="n">
+        <v>45261.69791666666</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>MC Alger</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>4</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Magra</t>
+        </is>
+      </c>
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>30/11/2023 07:50</t>
+        </is>
+      </c>
+      <c r="L56" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>01/12/2023 15:57</t>
+        </is>
+      </c>
+      <c r="N56" t="n">
+        <v>4.62</v>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>30/11/2023 07:50</t>
+        </is>
+      </c>
+      <c r="P56" t="n">
+        <v>5.76</v>
+      </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>01/12/2023 15:57</t>
+        </is>
+      </c>
+      <c r="R56" t="n">
+        <v>9.279999999999999</v>
+      </c>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>30/11/2023 07:50</t>
+        </is>
+      </c>
+      <c r="T56" t="n">
+        <v>15.13</v>
+      </c>
+      <c r="U56" t="inlineStr">
+        <is>
+          <t>01/12/2023 15:57</t>
+        </is>
+      </c>
+      <c r="V56" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/mc-alger-magra/bqEUgPTl/</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E57" s="2" t="n">
+        <v>45261.75</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Constantine</t>
+        </is>
+      </c>
+      <c r="G57" t="n">
+        <v>2</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Khenchela</t>
+        </is>
+      </c>
+      <c r="I57" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>30/11/2023 06:12</t>
+        </is>
+      </c>
+      <c r="L57" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>01/12/2023 17:55</t>
+        </is>
+      </c>
+      <c r="N57" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>30/11/2023 06:12</t>
+        </is>
+      </c>
+      <c r="P57" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>01/12/2023 17:55</t>
+        </is>
+      </c>
+      <c r="R57" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="S57" t="inlineStr">
+        <is>
+          <t>30/11/2023 06:12</t>
+        </is>
+      </c>
+      <c r="T57" t="n">
+        <v>6.62</v>
+      </c>
+      <c r="U57" t="inlineStr">
+        <is>
+          <t>01/12/2023 17:55</t>
+        </is>
+      </c>
+      <c r="V57" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-khenchela/S0Nbao6R/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 02-12-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/algeria_ligue-1_2023-2024.xlsx
+++ b/2023/algeria_ligue-1_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V57"/>
+  <dimension ref="A1:V60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -849,71 +849,71 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>MC Alger</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Ben Aknoun</t>
+          <t>Kabylie</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>1.4</v>
+        <v>2.84</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>16/09/2023 03:43</t>
+          <t>15/09/2023 13:42</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>1.3</v>
+        <v>3.8</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>16/09/2023 10:40</t>
+          <t>16/09/2023 16:12</t>
         </is>
       </c>
       <c r="N5" t="n">
-        <v>4.19</v>
+        <v>2.63</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>16/09/2023 03:43</t>
+          <t>15/09/2023 13:42</t>
         </is>
       </c>
       <c r="P5" t="n">
-        <v>4.81</v>
+        <v>2.84</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>16/09/2023 16:47</t>
+          <t>16/09/2023 15:03</t>
         </is>
       </c>
       <c r="R5" t="n">
-        <v>8.529999999999999</v>
+        <v>2.72</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>16/09/2023 03:43</t>
+          <t>15/09/2023 13:42</t>
         </is>
       </c>
       <c r="T5" t="n">
-        <v>12.64</v>
+        <v>2.26</v>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>16/09/2023 16:47</t>
+          <t>16/09/2023 16:12</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/mc-alger-es-ben-aknoun/WjyqCu9h/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-kabylie/YFXa8c8H/</t>
         </is>
       </c>
     </row>
@@ -941,71 +941,71 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Magra</t>
+          <t>MC Alger</t>
         </is>
       </c>
       <c r="G6" t="n">
+        <v>4</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Ben Aknoun</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
         <v>0</v>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Kabylie</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>1</v>
-      </c>
       <c r="J6" t="n">
-        <v>2.84</v>
+        <v>1.4</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>15/09/2023 13:42</t>
+          <t>16/09/2023 03:43</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>3.8</v>
+        <v>1.3</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>16/09/2023 16:12</t>
+          <t>16/09/2023 10:40</t>
         </is>
       </c>
       <c r="N6" t="n">
-        <v>2.63</v>
+        <v>4.19</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>15/09/2023 13:42</t>
+          <t>16/09/2023 03:43</t>
         </is>
       </c>
       <c r="P6" t="n">
-        <v>2.84</v>
+        <v>4.81</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>16/09/2023 15:03</t>
+          <t>16/09/2023 16:47</t>
         </is>
       </c>
       <c r="R6" t="n">
-        <v>2.72</v>
+        <v>8.529999999999999</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>15/09/2023 13:42</t>
+          <t>16/09/2023 03:43</t>
         </is>
       </c>
       <c r="T6" t="n">
-        <v>2.26</v>
+        <v>12.64</v>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>16/09/2023 16:12</t>
+          <t>16/09/2023 16:47</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-kabylie/YFXa8c8H/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/mc-alger-es-ben-aknoun/WjyqCu9h/</t>
         </is>
       </c>
     </row>
@@ -1861,71 +1861,71 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Oran</t>
+          <t>Biskra</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" t="n">
-        <v>2.49</v>
+        <v>1.98</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>28/09/2023 19:27</t>
+          <t>28/09/2023 04:12</t>
         </is>
       </c>
       <c r="L16" t="n">
-        <v>2.14</v>
+        <v>2.1</v>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>29/09/2023 13:29</t>
+          <t>29/09/2023 16:44</t>
         </is>
       </c>
       <c r="N16" t="n">
-        <v>2.88</v>
+        <v>2.89</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>28/09/2023 19:27</t>
+          <t>28/09/2023 04:12</t>
         </is>
       </c>
       <c r="P16" t="n">
-        <v>2.74</v>
+        <v>2.77</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>29/09/2023 14:49</t>
+          <t>29/09/2023 16:44</t>
         </is>
       </c>
       <c r="R16" t="n">
-        <v>3.18</v>
+        <v>3.97</v>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>28/09/2023 19:27</t>
+          <t>28/09/2023 04:12</t>
         </is>
       </c>
       <c r="T16" t="n">
-        <v>4.43</v>
+        <v>4.54</v>
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>29/09/2023 15:47</t>
+          <t>29/09/2023 16:44</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-oran/6qOsFaSf/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-biskra/OKYxGuDl/</t>
         </is>
       </c>
     </row>
@@ -1953,7 +1953,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Magra</t>
+          <t>Khenchela</t>
         </is>
       </c>
       <c r="G17" t="n">
@@ -1961,14 +1961,14 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Biskra</t>
+          <t>Kabylie</t>
         </is>
       </c>
       <c r="I17" t="n">
         <v>1</v>
       </c>
       <c r="J17" t="n">
-        <v>1.98</v>
+        <v>2.63</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
@@ -1976,15 +1976,15 @@
         </is>
       </c>
       <c r="L17" t="n">
-        <v>2.1</v>
+        <v>2.05</v>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>29/09/2023 16:44</t>
+          <t>29/09/2023 16:41</t>
         </is>
       </c>
       <c r="N17" t="n">
-        <v>2.89</v>
+        <v>2.62</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1992,15 +1992,15 @@
         </is>
       </c>
       <c r="P17" t="n">
-        <v>2.77</v>
+        <v>2.75</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>29/09/2023 16:44</t>
+          <t>29/09/2023 16:41</t>
         </is>
       </c>
       <c r="R17" t="n">
-        <v>3.97</v>
+        <v>3.02</v>
       </c>
       <c r="S17" t="inlineStr">
         <is>
@@ -2008,16 +2008,16 @@
         </is>
       </c>
       <c r="T17" t="n">
-        <v>4.54</v>
+        <v>4.88</v>
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>29/09/2023 16:44</t>
+          <t>29/09/2023 16:27</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-biskra/OKYxGuDl/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-kabylie/pUZYGLcr/</t>
         </is>
       </c>
     </row>
@@ -2045,71 +2045,71 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Khenchela</t>
+          <t>US Souf</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Kabylie</t>
+          <t>Oran</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>2.63</v>
+        <v>2.49</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>28/09/2023 04:12</t>
+          <t>28/09/2023 19:27</t>
         </is>
       </c>
       <c r="L18" t="n">
-        <v>2.05</v>
+        <v>2.14</v>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>29/09/2023 16:41</t>
+          <t>29/09/2023 13:29</t>
         </is>
       </c>
       <c r="N18" t="n">
-        <v>2.62</v>
+        <v>2.88</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>28/09/2023 04:12</t>
+          <t>28/09/2023 19:27</t>
         </is>
       </c>
       <c r="P18" t="n">
-        <v>2.75</v>
+        <v>2.74</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>29/09/2023 16:41</t>
+          <t>29/09/2023 14:49</t>
         </is>
       </c>
       <c r="R18" t="n">
-        <v>3.02</v>
+        <v>3.18</v>
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>28/09/2023 04:12</t>
+          <t>28/09/2023 19:27</t>
         </is>
       </c>
       <c r="T18" t="n">
-        <v>4.88</v>
+        <v>4.43</v>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>29/09/2023 16:27</t>
+          <t>29/09/2023 15:47</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-kabylie/pUZYGLcr/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-oran/6qOsFaSf/</t>
         </is>
       </c>
     </row>
@@ -3241,71 +3241,71 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Paradou</t>
+          <t>US Souf</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Oran</t>
+          <t>Constantine</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J31" t="n">
-        <v>1.48</v>
+        <v>3.14</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>19/10/2023 04:42</t>
+          <t>10/11/2023 06:42</t>
         </is>
       </c>
       <c r="L31" t="n">
-        <v>1.46</v>
+        <v>3.21</v>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>10/11/2023 14:57</t>
+          <t>10/11/2023 15:16</t>
         </is>
       </c>
       <c r="N31" t="n">
-        <v>3.71</v>
+        <v>2.82</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>19/10/2023 04:42</t>
+          <t>10/11/2023 06:42</t>
         </is>
       </c>
       <c r="P31" t="n">
-        <v>3.91</v>
+        <v>2.86</v>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>10/11/2023 14:57</t>
+          <t>10/11/2023 13:35</t>
         </is>
       </c>
       <c r="R31" t="n">
-        <v>6.42</v>
+        <v>2.5</v>
       </c>
       <c r="S31" t="inlineStr">
         <is>
-          <t>19/10/2023 04:42</t>
+          <t>10/11/2023 06:42</t>
         </is>
       </c>
       <c r="T31" t="n">
-        <v>8.550000000000001</v>
+        <v>2.53</v>
       </c>
       <c r="U31" t="inlineStr">
         <is>
-          <t>10/11/2023 14:57</t>
+          <t>10/11/2023 15:16</t>
         </is>
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/paradou-oran/ALKA1eA0/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-constantine/6mEJaZvD/</t>
         </is>
       </c>
     </row>
@@ -3333,71 +3333,71 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Paradou</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Constantine</t>
+          <t>Oran</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>3.14</v>
+        <v>1.48</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>10/11/2023 06:42</t>
+          <t>19/10/2023 04:42</t>
         </is>
       </c>
       <c r="L32" t="n">
-        <v>3.21</v>
+        <v>1.46</v>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>10/11/2023 15:16</t>
+          <t>10/11/2023 14:57</t>
         </is>
       </c>
       <c r="N32" t="n">
-        <v>2.82</v>
+        <v>3.71</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>10/11/2023 06:42</t>
+          <t>19/10/2023 04:42</t>
         </is>
       </c>
       <c r="P32" t="n">
-        <v>2.86</v>
+        <v>3.91</v>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>10/11/2023 13:35</t>
+          <t>10/11/2023 14:57</t>
         </is>
       </c>
       <c r="R32" t="n">
-        <v>2.5</v>
+        <v>6.42</v>
       </c>
       <c r="S32" t="inlineStr">
         <is>
-          <t>10/11/2023 06:42</t>
+          <t>19/10/2023 04:42</t>
         </is>
       </c>
       <c r="T32" t="n">
-        <v>2.53</v>
+        <v>8.550000000000001</v>
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>10/11/2023 15:16</t>
+          <t>10/11/2023 14:57</t>
         </is>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-constantine/6mEJaZvD/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/paradou-oran/ALKA1eA0/</t>
         </is>
       </c>
     </row>
@@ -5698,6 +5698,282 @@
       <c r="V57" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-khenchela/S0Nbao6R/</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E58" s="2" t="n">
+        <v>45262.69791666666</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Saoura</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>ES Setif</t>
+        </is>
+      </c>
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>01/12/2023 05:12</t>
+        </is>
+      </c>
+      <c r="L58" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>02/12/2023 16:40</t>
+        </is>
+      </c>
+      <c r="N58" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>01/12/2023 05:12</t>
+        </is>
+      </c>
+      <c r="P58" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>02/12/2023 16:40</t>
+        </is>
+      </c>
+      <c r="R58" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="S58" t="inlineStr">
+        <is>
+          <t>01/12/2023 05:12</t>
+        </is>
+      </c>
+      <c r="T58" t="n">
+        <v>5.44</v>
+      </c>
+      <c r="U58" t="inlineStr">
+        <is>
+          <t>02/12/2023 16:40</t>
+        </is>
+      </c>
+      <c r="V58" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/saoura-es-setif/Kb2wh3b1/</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E59" s="2" t="n">
+        <v>45262.69791666666</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>ASO Chlef</t>
+        </is>
+      </c>
+      <c r="G59" t="n">
+        <v>2</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>US Souf</t>
+        </is>
+      </c>
+      <c r="I59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>01/12/2023 05:12</t>
+        </is>
+      </c>
+      <c r="L59" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>02/12/2023 16:27</t>
+        </is>
+      </c>
+      <c r="N59" t="n">
+        <v>4.37</v>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>01/12/2023 05:12</t>
+        </is>
+      </c>
+      <c r="P59" t="n">
+        <v>4.85</v>
+      </c>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>02/12/2023 16:27</t>
+        </is>
+      </c>
+      <c r="R59" t="n">
+        <v>8.279999999999999</v>
+      </c>
+      <c r="S59" t="inlineStr">
+        <is>
+          <t>01/12/2023 05:12</t>
+        </is>
+      </c>
+      <c r="T59" t="n">
+        <v>11.33</v>
+      </c>
+      <c r="U59" t="inlineStr">
+        <is>
+          <t>02/12/2023 16:27</t>
+        </is>
+      </c>
+      <c r="V59" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/aso-chlef-us-souf/xzDYhqqe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E60" s="2" t="n">
+        <v>45262.75</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Oran</t>
+        </is>
+      </c>
+      <c r="G60" t="n">
+        <v>1</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>Kabylie</t>
+        </is>
+      </c>
+      <c r="I60" t="n">
+        <v>3</v>
+      </c>
+      <c r="J60" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>01/12/2023 06:13</t>
+        </is>
+      </c>
+      <c r="L60" t="n">
+        <v>2.77</v>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>02/12/2023 17:55</t>
+        </is>
+      </c>
+      <c r="N60" t="n">
+        <v>2.48</v>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>01/12/2023 06:13</t>
+        </is>
+      </c>
+      <c r="P60" t="n">
+        <v>2.65</v>
+      </c>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>02/12/2023 17:55</t>
+        </is>
+      </c>
+      <c r="R60" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="S60" t="inlineStr">
+        <is>
+          <t>01/12/2023 06:13</t>
+        </is>
+      </c>
+      <c r="T60" t="n">
+        <v>3.14</v>
+      </c>
+      <c r="U60" t="inlineStr">
+        <is>
+          <t>02/12/2023 17:55</t>
+        </is>
+      </c>
+      <c r="V60" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-kabylie/pxfPF6j8/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 07-12-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/algeria_ligue-1_2023-2024.xlsx
+++ b/2023/algeria_ligue-1_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V60"/>
+  <dimension ref="A1:V61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5977,6 +5977,98 @@
         </is>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E61" s="2" t="n">
+        <v>45267.79166666666</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Paradou</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>MC Alger</t>
+        </is>
+      </c>
+      <c r="I61" t="n">
+        <v>1</v>
+      </c>
+      <c r="J61" t="n">
+        <v>3.44</v>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>06/12/2023 07:12</t>
+        </is>
+      </c>
+      <c r="L61" t="n">
+        <v>8.82</v>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>07/12/2023 18:38</t>
+        </is>
+      </c>
+      <c r="N61" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>06/12/2023 07:12</t>
+        </is>
+      </c>
+      <c r="P61" t="n">
+        <v>3.82</v>
+      </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>07/12/2023 18:38</t>
+        </is>
+      </c>
+      <c r="R61" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="S61" t="inlineStr">
+        <is>
+          <t>06/12/2023 07:12</t>
+        </is>
+      </c>
+      <c r="T61" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="U61" t="inlineStr">
+        <is>
+          <t>07/12/2023 18:38</t>
+        </is>
+      </c>
+      <c r="V61" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/paradou-mc-alger/ITA1dIkm/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizado por script em 08-12-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/algeria_ligue-1_2023-2024.xlsx
+++ b/2023/algeria_ligue-1_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V61"/>
+  <dimension ref="A1:V63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -849,71 +849,71 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Magra</t>
+          <t>MC Alger</t>
         </is>
       </c>
       <c r="G5" t="n">
+        <v>4</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Ben Aknoun</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
         <v>0</v>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Kabylie</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>1</v>
-      </c>
       <c r="J5" t="n">
-        <v>2.84</v>
+        <v>1.4</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>15/09/2023 13:42</t>
+          <t>16/09/2023 03:43</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>3.8</v>
+        <v>1.3</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>16/09/2023 16:12</t>
+          <t>16/09/2023 10:40</t>
         </is>
       </c>
       <c r="N5" t="n">
-        <v>2.63</v>
+        <v>4.19</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>15/09/2023 13:42</t>
+          <t>16/09/2023 03:43</t>
         </is>
       </c>
       <c r="P5" t="n">
-        <v>2.84</v>
+        <v>4.81</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>16/09/2023 15:03</t>
+          <t>16/09/2023 16:47</t>
         </is>
       </c>
       <c r="R5" t="n">
-        <v>2.72</v>
+        <v>8.529999999999999</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>15/09/2023 13:42</t>
+          <t>16/09/2023 03:43</t>
         </is>
       </c>
       <c r="T5" t="n">
-        <v>2.26</v>
+        <v>12.64</v>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>16/09/2023 16:12</t>
+          <t>16/09/2023 16:47</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-kabylie/YFXa8c8H/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/mc-alger-es-ben-aknoun/WjyqCu9h/</t>
         </is>
       </c>
     </row>
@@ -941,71 +941,71 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>MC Alger</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Ben Aknoun</t>
+          <t>Kabylie</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>1.4</v>
+        <v>2.84</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>16/09/2023 03:43</t>
+          <t>15/09/2023 13:42</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>1.3</v>
+        <v>3.8</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>16/09/2023 10:40</t>
+          <t>16/09/2023 16:12</t>
         </is>
       </c>
       <c r="N6" t="n">
-        <v>4.19</v>
+        <v>2.63</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>16/09/2023 03:43</t>
+          <t>15/09/2023 13:42</t>
         </is>
       </c>
       <c r="P6" t="n">
-        <v>4.81</v>
+        <v>2.84</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>16/09/2023 16:47</t>
+          <t>16/09/2023 15:03</t>
         </is>
       </c>
       <c r="R6" t="n">
-        <v>8.529999999999999</v>
+        <v>2.72</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>16/09/2023 03:43</t>
+          <t>15/09/2023 13:42</t>
         </is>
       </c>
       <c r="T6" t="n">
-        <v>12.64</v>
+        <v>2.26</v>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>16/09/2023 16:47</t>
+          <t>16/09/2023 16:12</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/mc-alger-es-ben-aknoun/WjyqCu9h/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-kabylie/YFXa8c8H/</t>
         </is>
       </c>
     </row>
@@ -5725,22 +5725,22 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Saoura</t>
+          <t>ASO Chlef</t>
         </is>
       </c>
       <c r="G58" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>ES Setif</t>
+          <t>US Souf</t>
         </is>
       </c>
       <c r="I58" t="n">
         <v>0</v>
       </c>
       <c r="J58" t="n">
-        <v>1.88</v>
+        <v>1.35</v>
       </c>
       <c r="K58" t="inlineStr">
         <is>
@@ -5748,15 +5748,15 @@
         </is>
       </c>
       <c r="L58" t="n">
-        <v>1.75</v>
+        <v>1.32</v>
       </c>
       <c r="M58" t="inlineStr">
         <is>
-          <t>02/12/2023 16:40</t>
+          <t>02/12/2023 16:27</t>
         </is>
       </c>
       <c r="N58" t="n">
-        <v>3.01</v>
+        <v>4.37</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -5764,15 +5764,15 @@
         </is>
       </c>
       <c r="P58" t="n">
-        <v>3.32</v>
+        <v>4.85</v>
       </c>
       <c r="Q58" t="inlineStr">
         <is>
-          <t>02/12/2023 16:40</t>
+          <t>02/12/2023 16:27</t>
         </is>
       </c>
       <c r="R58" t="n">
-        <v>4.3</v>
+        <v>8.279999999999999</v>
       </c>
       <c r="S58" t="inlineStr">
         <is>
@@ -5780,16 +5780,16 @@
         </is>
       </c>
       <c r="T58" t="n">
-        <v>5.44</v>
+        <v>11.33</v>
       </c>
       <c r="U58" t="inlineStr">
         <is>
-          <t>02/12/2023 16:40</t>
+          <t>02/12/2023 16:27</t>
         </is>
       </c>
       <c r="V58" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/saoura-es-setif/Kb2wh3b1/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/aso-chlef-us-souf/xzDYhqqe/</t>
         </is>
       </c>
     </row>
@@ -5817,22 +5817,22 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>ASO Chlef</t>
+          <t>Saoura</t>
         </is>
       </c>
       <c r="G59" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>ES Setif</t>
         </is>
       </c>
       <c r="I59" t="n">
         <v>0</v>
       </c>
       <c r="J59" t="n">
-        <v>1.35</v>
+        <v>1.88</v>
       </c>
       <c r="K59" t="inlineStr">
         <is>
@@ -5840,15 +5840,15 @@
         </is>
       </c>
       <c r="L59" t="n">
-        <v>1.32</v>
+        <v>1.75</v>
       </c>
       <c r="M59" t="inlineStr">
         <is>
-          <t>02/12/2023 16:27</t>
+          <t>02/12/2023 16:40</t>
         </is>
       </c>
       <c r="N59" t="n">
-        <v>4.37</v>
+        <v>3.01</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -5856,15 +5856,15 @@
         </is>
       </c>
       <c r="P59" t="n">
-        <v>4.85</v>
+        <v>3.32</v>
       </c>
       <c r="Q59" t="inlineStr">
         <is>
-          <t>02/12/2023 16:27</t>
+          <t>02/12/2023 16:40</t>
         </is>
       </c>
       <c r="R59" t="n">
-        <v>8.279999999999999</v>
+        <v>4.3</v>
       </c>
       <c r="S59" t="inlineStr">
         <is>
@@ -5872,16 +5872,16 @@
         </is>
       </c>
       <c r="T59" t="n">
-        <v>11.33</v>
+        <v>5.44</v>
       </c>
       <c r="U59" t="inlineStr">
         <is>
-          <t>02/12/2023 16:27</t>
+          <t>02/12/2023 16:40</t>
         </is>
       </c>
       <c r="V59" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/aso-chlef-us-souf/xzDYhqqe/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/saoura-es-setif/Kb2wh3b1/</t>
         </is>
       </c>
     </row>
@@ -6066,6 +6066,190 @@
       <c r="V61" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/algeria/ligue-1/paradou-mc-alger/ITA1dIkm/</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E62" s="2" t="n">
+        <v>45268.63541666666</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Khenchela</t>
+        </is>
+      </c>
+      <c r="G62" t="n">
+        <v>2</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>El Bayadh</t>
+        </is>
+      </c>
+      <c r="I62" t="n">
+        <v>0</v>
+      </c>
+      <c r="J62" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>07/12/2023 07:08</t>
+        </is>
+      </c>
+      <c r="L62" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>08/12/2023 15:10</t>
+        </is>
+      </c>
+      <c r="N62" t="n">
+        <v>2.72</v>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>07/12/2023 07:08</t>
+        </is>
+      </c>
+      <c r="P62" t="n">
+        <v>3.09</v>
+      </c>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>08/12/2023 15:10</t>
+        </is>
+      </c>
+      <c r="R62" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="S62" t="inlineStr">
+        <is>
+          <t>07/12/2023 07:08</t>
+        </is>
+      </c>
+      <c r="T62" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="U62" t="inlineStr">
+        <is>
+          <t>08/12/2023 15:06</t>
+        </is>
+      </c>
+      <c r="V62" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-el-bayadh/vwCccbzs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E63" s="2" t="n">
+        <v>45268.75</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Kabylie</t>
+        </is>
+      </c>
+      <c r="G63" t="n">
+        <v>1</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>Ben Aknoun</t>
+        </is>
+      </c>
+      <c r="I63" t="n">
+        <v>0</v>
+      </c>
+      <c r="J63" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>07/12/2023 06:11</t>
+        </is>
+      </c>
+      <c r="L63" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>08/12/2023 17:18</t>
+        </is>
+      </c>
+      <c r="N63" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>07/12/2023 06:11</t>
+        </is>
+      </c>
+      <c r="P63" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>08/12/2023 17:18</t>
+        </is>
+      </c>
+      <c r="R63" t="n">
+        <v>6.88</v>
+      </c>
+      <c r="S63" t="inlineStr">
+        <is>
+          <t>07/12/2023 06:11</t>
+        </is>
+      </c>
+      <c r="T63" t="n">
+        <v>13.66</v>
+      </c>
+      <c r="U63" t="inlineStr">
+        <is>
+          <t>08/12/2023 17:18</t>
+        </is>
+      </c>
+      <c r="V63" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/kabylie-es-ben-aknoun/n92IhzkC/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 09-12-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/algeria_ligue-1_2023-2024.xlsx
+++ b/2023/algeria_ligue-1_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V63"/>
+  <dimension ref="A1:V66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3241,71 +3241,71 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Paradou</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Constantine</t>
+          <t>Oran</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>3.14</v>
+        <v>1.48</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>10/11/2023 06:42</t>
+          <t>19/10/2023 04:42</t>
         </is>
       </c>
       <c r="L31" t="n">
-        <v>3.21</v>
+        <v>1.46</v>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>10/11/2023 15:16</t>
+          <t>10/11/2023 14:57</t>
         </is>
       </c>
       <c r="N31" t="n">
-        <v>2.82</v>
+        <v>3.71</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>10/11/2023 06:42</t>
+          <t>19/10/2023 04:42</t>
         </is>
       </c>
       <c r="P31" t="n">
-        <v>2.86</v>
+        <v>3.91</v>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>10/11/2023 13:35</t>
+          <t>10/11/2023 14:57</t>
         </is>
       </c>
       <c r="R31" t="n">
-        <v>2.5</v>
+        <v>6.42</v>
       </c>
       <c r="S31" t="inlineStr">
         <is>
-          <t>10/11/2023 06:42</t>
+          <t>19/10/2023 04:42</t>
         </is>
       </c>
       <c r="T31" t="n">
-        <v>2.53</v>
+        <v>8.550000000000001</v>
       </c>
       <c r="U31" t="inlineStr">
         <is>
-          <t>10/11/2023 15:16</t>
+          <t>10/11/2023 14:57</t>
         </is>
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-constantine/6mEJaZvD/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/paradou-oran/ALKA1eA0/</t>
         </is>
       </c>
     </row>
@@ -3333,71 +3333,71 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Paradou</t>
+          <t>US Souf</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Oran</t>
+          <t>Constantine</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J32" t="n">
-        <v>1.48</v>
+        <v>3.14</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>19/10/2023 04:42</t>
+          <t>10/11/2023 06:42</t>
         </is>
       </c>
       <c r="L32" t="n">
-        <v>1.46</v>
+        <v>3.21</v>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>10/11/2023 14:57</t>
+          <t>10/11/2023 15:16</t>
         </is>
       </c>
       <c r="N32" t="n">
-        <v>3.71</v>
+        <v>2.82</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>19/10/2023 04:42</t>
+          <t>10/11/2023 06:42</t>
         </is>
       </c>
       <c r="P32" t="n">
-        <v>3.91</v>
+        <v>2.86</v>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>10/11/2023 14:57</t>
+          <t>10/11/2023 13:35</t>
         </is>
       </c>
       <c r="R32" t="n">
-        <v>6.42</v>
+        <v>2.5</v>
       </c>
       <c r="S32" t="inlineStr">
         <is>
-          <t>19/10/2023 04:42</t>
+          <t>10/11/2023 06:42</t>
         </is>
       </c>
       <c r="T32" t="n">
-        <v>8.550000000000001</v>
+        <v>2.53</v>
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>10/11/2023 14:57</t>
+          <t>10/11/2023 15:16</t>
         </is>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/paradou-oran/ALKA1eA0/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-constantine/6mEJaZvD/</t>
         </is>
       </c>
     </row>
@@ -4161,71 +4161,71 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Constantine</t>
+          <t>El Bayadh</t>
         </is>
       </c>
       <c r="G41" t="n">
+        <v>4</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>US Souf</t>
+        </is>
+      </c>
+      <c r="I41" t="n">
         <v>0</v>
       </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>Magra</t>
-        </is>
-      </c>
-      <c r="I41" t="n">
-        <v>1</v>
-      </c>
       <c r="J41" t="n">
-        <v>1.59</v>
+        <v>1.45</v>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>26/10/2023 04:42</t>
+          <t>16/11/2023 03:42</t>
         </is>
       </c>
       <c r="L41" t="n">
-        <v>1.31</v>
+        <v>1.45</v>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>17/11/2023 15:24</t>
+          <t>17/11/2023 15:18</t>
         </is>
       </c>
       <c r="N41" t="n">
-        <v>3.47</v>
+        <v>3.74</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>26/10/2023 04:42</t>
+          <t>16/11/2023 03:42</t>
         </is>
       </c>
       <c r="P41" t="n">
-        <v>4.98</v>
+        <v>4.01</v>
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>17/11/2023 15:24</t>
+          <t>17/11/2023 15:18</t>
         </is>
       </c>
       <c r="R41" t="n">
-        <v>5.42</v>
+        <v>7.38</v>
       </c>
       <c r="S41" t="inlineStr">
         <is>
-          <t>26/10/2023 04:42</t>
+          <t>16/11/2023 03:42</t>
         </is>
       </c>
       <c r="T41" t="n">
-        <v>10.79</v>
+        <v>8.609999999999999</v>
       </c>
       <c r="U41" t="inlineStr">
         <is>
-          <t>17/11/2023 15:24</t>
+          <t>17/11/2023 15:18</t>
         </is>
       </c>
       <c r="V41" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-magra/jgeqGfPg/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-us-souf/UqfmFEv0/</t>
         </is>
       </c>
     </row>
@@ -4253,71 +4253,71 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>El Bayadh</t>
+          <t>Constantine</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" t="n">
-        <v>1.45</v>
+        <v>1.59</v>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>16/11/2023 03:42</t>
+          <t>26/10/2023 04:42</t>
         </is>
       </c>
       <c r="L42" t="n">
-        <v>1.45</v>
+        <v>1.31</v>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>17/11/2023 15:18</t>
+          <t>17/11/2023 15:24</t>
         </is>
       </c>
       <c r="N42" t="n">
-        <v>3.74</v>
+        <v>3.47</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>16/11/2023 03:42</t>
+          <t>26/10/2023 04:42</t>
         </is>
       </c>
       <c r="P42" t="n">
-        <v>4.01</v>
+        <v>4.98</v>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>17/11/2023 15:18</t>
+          <t>17/11/2023 15:24</t>
         </is>
       </c>
       <c r="R42" t="n">
-        <v>7.38</v>
+        <v>5.42</v>
       </c>
       <c r="S42" t="inlineStr">
         <is>
-          <t>16/11/2023 03:42</t>
+          <t>26/10/2023 04:42</t>
         </is>
       </c>
       <c r="T42" t="n">
-        <v>8.609999999999999</v>
+        <v>10.79</v>
       </c>
       <c r="U42" t="inlineStr">
         <is>
-          <t>17/11/2023 15:18</t>
+          <t>17/11/2023 15:24</t>
         </is>
       </c>
       <c r="V42" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-us-souf/UqfmFEv0/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-magra/jgeqGfPg/</t>
         </is>
       </c>
     </row>
@@ -4897,22 +4897,22 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Magra</t>
+          <t>Paradou</t>
         </is>
       </c>
       <c r="G49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>El Bayadh</t>
+          <t>Constantine</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J49" t="n">
-        <v>2.07</v>
+        <v>1.79</v>
       </c>
       <c r="K49" t="inlineStr">
         <is>
@@ -4920,15 +4920,15 @@
         </is>
       </c>
       <c r="L49" t="n">
-        <v>2.15</v>
+        <v>1.98</v>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>24/11/2023 14:19</t>
+          <t>24/11/2023 15:00</t>
         </is>
       </c>
       <c r="N49" t="n">
-        <v>2.88</v>
+        <v>3.27</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4936,15 +4936,15 @@
         </is>
       </c>
       <c r="P49" t="n">
-        <v>2.9</v>
+        <v>3.08</v>
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>24/11/2023 15:12</t>
+          <t>24/11/2023 15:00</t>
         </is>
       </c>
       <c r="R49" t="n">
-        <v>4.25</v>
+        <v>4.96</v>
       </c>
       <c r="S49" t="inlineStr">
         <is>
@@ -4952,16 +4952,16 @@
         </is>
       </c>
       <c r="T49" t="n">
-        <v>4.06</v>
+        <v>4.37</v>
       </c>
       <c r="U49" t="inlineStr">
         <is>
-          <t>24/11/2023 14:19</t>
+          <t>24/11/2023 15:00</t>
         </is>
       </c>
       <c r="V49" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-el-bayadh/jog1n073/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/paradou-constantine/dOgcmthc/</t>
         </is>
       </c>
     </row>
@@ -4989,22 +4989,22 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Paradou</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="G50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Constantine</t>
+          <t>El Bayadh</t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J50" t="n">
-        <v>1.79</v>
+        <v>2.07</v>
       </c>
       <c r="K50" t="inlineStr">
         <is>
@@ -5012,15 +5012,15 @@
         </is>
       </c>
       <c r="L50" t="n">
-        <v>1.98</v>
+        <v>2.15</v>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>24/11/2023 15:00</t>
+          <t>24/11/2023 14:19</t>
         </is>
       </c>
       <c r="N50" t="n">
-        <v>3.27</v>
+        <v>2.88</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -5028,15 +5028,15 @@
         </is>
       </c>
       <c r="P50" t="n">
-        <v>3.08</v>
+        <v>2.9</v>
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>24/11/2023 15:00</t>
+          <t>24/11/2023 15:12</t>
         </is>
       </c>
       <c r="R50" t="n">
-        <v>4.96</v>
+        <v>4.25</v>
       </c>
       <c r="S50" t="inlineStr">
         <is>
@@ -5044,16 +5044,16 @@
         </is>
       </c>
       <c r="T50" t="n">
-        <v>4.37</v>
+        <v>4.06</v>
       </c>
       <c r="U50" t="inlineStr">
         <is>
-          <t>24/11/2023 15:00</t>
+          <t>24/11/2023 14:19</t>
         </is>
       </c>
       <c r="V50" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/paradou-constantine/dOgcmthc/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-el-bayadh/jog1n073/</t>
         </is>
       </c>
     </row>
@@ -6250,6 +6250,282 @@
       <c r="V63" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/algeria/ligue-1/kabylie-es-ben-aknoun/n92IhzkC/</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E64" s="2" t="n">
+        <v>45269.625</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Magra</t>
+        </is>
+      </c>
+      <c r="G64" t="n">
+        <v>1</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>ASO Chlef</t>
+        </is>
+      </c>
+      <c r="I64" t="n">
+        <v>1</v>
+      </c>
+      <c r="J64" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>08/12/2023 15:43</t>
+        </is>
+      </c>
+      <c r="L64" t="n">
+        <v>2.42</v>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>09/12/2023 14:55</t>
+        </is>
+      </c>
+      <c r="N64" t="n">
+        <v>2.82</v>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>08/12/2023 15:43</t>
+        </is>
+      </c>
+      <c r="P64" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>09/12/2023 14:55</t>
+        </is>
+      </c>
+      <c r="R64" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="S64" t="inlineStr">
+        <is>
+          <t>08/12/2023 15:43</t>
+        </is>
+      </c>
+      <c r="T64" t="n">
+        <v>3.35</v>
+      </c>
+      <c r="U64" t="inlineStr">
+        <is>
+          <t>09/12/2023 14:55</t>
+        </is>
+      </c>
+      <c r="V64" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-aso-chlef/CjA5ex5g/</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E65" s="2" t="n">
+        <v>45269.625</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>US Souf</t>
+        </is>
+      </c>
+      <c r="G65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>Saoura</t>
+        </is>
+      </c>
+      <c r="I65" t="n">
+        <v>1</v>
+      </c>
+      <c r="J65" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>08/12/2023 15:43</t>
+        </is>
+      </c>
+      <c r="L65" t="n">
+        <v>3.07</v>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>09/12/2023 13:02</t>
+        </is>
+      </c>
+      <c r="N65" t="n">
+        <v>2.91</v>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>08/12/2023 15:43</t>
+        </is>
+      </c>
+      <c r="P65" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>09/12/2023 13:02</t>
+        </is>
+      </c>
+      <c r="R65" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="S65" t="inlineStr">
+        <is>
+          <t>08/12/2023 15:43</t>
+        </is>
+      </c>
+      <c r="T65" t="n">
+        <v>2.57</v>
+      </c>
+      <c r="U65" t="inlineStr">
+        <is>
+          <t>09/12/2023 14:31</t>
+        </is>
+      </c>
+      <c r="V65" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-saoura/YP0QjEJO/</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E66" s="2" t="n">
+        <v>45269.75</v>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>ES Setif</t>
+        </is>
+      </c>
+      <c r="G66" t="n">
+        <v>2</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>Biskra</t>
+        </is>
+      </c>
+      <c r="I66" t="n">
+        <v>2</v>
+      </c>
+      <c r="J66" t="n">
+        <v>1.69</v>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>08/12/2023 15:43</t>
+        </is>
+      </c>
+      <c r="L66" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>09/12/2023 17:56</t>
+        </is>
+      </c>
+      <c r="N66" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>08/12/2023 15:43</t>
+        </is>
+      </c>
+      <c r="P66" t="n">
+        <v>3.87</v>
+      </c>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>09/12/2023 17:57</t>
+        </is>
+      </c>
+      <c r="R66" t="n">
+        <v>5.16</v>
+      </c>
+      <c r="S66" t="inlineStr">
+        <is>
+          <t>08/12/2023 15:43</t>
+        </is>
+      </c>
+      <c r="T66" t="n">
+        <v>8.279999999999999</v>
+      </c>
+      <c r="U66" t="inlineStr">
+        <is>
+          <t>09/12/2023 17:57</t>
+        </is>
+      </c>
+      <c r="V66" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/es-setif-biskra/QgE9fdKa/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 15-12-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/algeria_ligue-1_2023-2024.xlsx
+++ b/2023/algeria_ligue-1_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V66"/>
+  <dimension ref="A1:V70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -849,71 +849,71 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>MC Alger</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Ben Aknoun</t>
+          <t>Kabylie</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>1.4</v>
+        <v>2.84</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>16/09/2023 03:43</t>
+          <t>15/09/2023 13:42</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>1.3</v>
+        <v>3.8</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>16/09/2023 10:40</t>
+          <t>16/09/2023 16:12</t>
         </is>
       </c>
       <c r="N5" t="n">
-        <v>4.19</v>
+        <v>2.63</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>16/09/2023 03:43</t>
+          <t>15/09/2023 13:42</t>
         </is>
       </c>
       <c r="P5" t="n">
-        <v>4.81</v>
+        <v>2.84</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>16/09/2023 16:47</t>
+          <t>16/09/2023 15:03</t>
         </is>
       </c>
       <c r="R5" t="n">
-        <v>8.529999999999999</v>
+        <v>2.72</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>16/09/2023 03:43</t>
+          <t>15/09/2023 13:42</t>
         </is>
       </c>
       <c r="T5" t="n">
-        <v>12.64</v>
+        <v>2.26</v>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>16/09/2023 16:47</t>
+          <t>16/09/2023 16:12</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/mc-alger-es-ben-aknoun/WjyqCu9h/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-kabylie/YFXa8c8H/</t>
         </is>
       </c>
     </row>
@@ -941,71 +941,71 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Magra</t>
+          <t>MC Alger</t>
         </is>
       </c>
       <c r="G6" t="n">
+        <v>4</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Ben Aknoun</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
         <v>0</v>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Kabylie</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>1</v>
-      </c>
       <c r="J6" t="n">
-        <v>2.84</v>
+        <v>1.4</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>15/09/2023 13:42</t>
+          <t>16/09/2023 03:43</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>3.8</v>
+        <v>1.3</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>16/09/2023 16:12</t>
+          <t>16/09/2023 10:40</t>
         </is>
       </c>
       <c r="N6" t="n">
-        <v>2.63</v>
+        <v>4.19</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>15/09/2023 13:42</t>
+          <t>16/09/2023 03:43</t>
         </is>
       </c>
       <c r="P6" t="n">
-        <v>2.84</v>
+        <v>4.81</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>16/09/2023 15:03</t>
+          <t>16/09/2023 16:47</t>
         </is>
       </c>
       <c r="R6" t="n">
-        <v>2.72</v>
+        <v>8.529999999999999</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>15/09/2023 13:42</t>
+          <t>16/09/2023 03:43</t>
         </is>
       </c>
       <c r="T6" t="n">
-        <v>2.26</v>
+        <v>12.64</v>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>16/09/2023 16:12</t>
+          <t>16/09/2023 16:47</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-kabylie/YFXa8c8H/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/mc-alger-es-ben-aknoun/WjyqCu9h/</t>
         </is>
       </c>
     </row>
@@ -1953,71 +1953,71 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Khenchela</t>
+          <t>US Souf</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Kabylie</t>
+          <t>Oran</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>2.63</v>
+        <v>2.49</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>28/09/2023 04:12</t>
+          <t>28/09/2023 19:27</t>
         </is>
       </c>
       <c r="L17" t="n">
-        <v>2.05</v>
+        <v>2.14</v>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>29/09/2023 16:41</t>
+          <t>29/09/2023 13:29</t>
         </is>
       </c>
       <c r="N17" t="n">
-        <v>2.62</v>
+        <v>2.88</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>28/09/2023 04:12</t>
+          <t>28/09/2023 19:27</t>
         </is>
       </c>
       <c r="P17" t="n">
-        <v>2.75</v>
+        <v>2.74</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>29/09/2023 16:41</t>
+          <t>29/09/2023 14:49</t>
         </is>
       </c>
       <c r="R17" t="n">
-        <v>3.02</v>
+        <v>3.18</v>
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>28/09/2023 04:12</t>
+          <t>28/09/2023 19:27</t>
         </is>
       </c>
       <c r="T17" t="n">
-        <v>4.88</v>
+        <v>4.43</v>
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>29/09/2023 16:27</t>
+          <t>29/09/2023 15:47</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-kabylie/pUZYGLcr/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-oran/6qOsFaSf/</t>
         </is>
       </c>
     </row>
@@ -2045,71 +2045,71 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Khenchela</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Oran</t>
+          <t>Kabylie</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="n">
-        <v>2.49</v>
+        <v>2.63</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>28/09/2023 19:27</t>
+          <t>28/09/2023 04:12</t>
         </is>
       </c>
       <c r="L18" t="n">
-        <v>2.14</v>
+        <v>2.05</v>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>29/09/2023 13:29</t>
+          <t>29/09/2023 16:41</t>
         </is>
       </c>
       <c r="N18" t="n">
-        <v>2.88</v>
+        <v>2.62</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>28/09/2023 19:27</t>
+          <t>28/09/2023 04:12</t>
         </is>
       </c>
       <c r="P18" t="n">
-        <v>2.74</v>
+        <v>2.75</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>29/09/2023 14:49</t>
+          <t>29/09/2023 16:41</t>
         </is>
       </c>
       <c r="R18" t="n">
-        <v>3.18</v>
+        <v>3.02</v>
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>28/09/2023 19:27</t>
+          <t>28/09/2023 04:12</t>
         </is>
       </c>
       <c r="T18" t="n">
-        <v>4.43</v>
+        <v>4.88</v>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>29/09/2023 15:47</t>
+          <t>29/09/2023 16:27</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-oran/6qOsFaSf/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-kabylie/pUZYGLcr/</t>
         </is>
       </c>
     </row>
@@ -3609,71 +3609,71 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Khenchela</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Biskra</t>
+          <t>Ben Aknoun</t>
         </is>
       </c>
       <c r="I35" t="n">
         <v>1</v>
       </c>
       <c r="J35" t="n">
-        <v>1.74</v>
+        <v>1.61</v>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>10/11/2023 03:13</t>
+          <t>11/11/2023 10:12</t>
         </is>
       </c>
       <c r="L35" t="n">
-        <v>1.29</v>
+        <v>1.62</v>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>11/11/2023 10:24</t>
+          <t>11/11/2023 14:48</t>
         </is>
       </c>
       <c r="N35" t="n">
-        <v>3.19</v>
+        <v>3.51</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>10/11/2023 03:13</t>
+          <t>11/11/2023 10:12</t>
         </is>
       </c>
       <c r="P35" t="n">
-        <v>4.87</v>
+        <v>3.56</v>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>11/11/2023 14:54</t>
+          <t>11/11/2023 14:48</t>
         </is>
       </c>
       <c r="R35" t="n">
-        <v>4.9</v>
+        <v>5.97</v>
       </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>10/11/2023 03:13</t>
+          <t>11/11/2023 10:12</t>
         </is>
       </c>
       <c r="T35" t="n">
-        <v>13.77</v>
+        <v>6.3</v>
       </c>
       <c r="U35" t="inlineStr">
         <is>
-          <t>11/11/2023 14:54</t>
+          <t>11/11/2023 14:48</t>
         </is>
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-biskra/GbL62yef/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-es-ben-aknoun/lCJE0FP6/</t>
         </is>
       </c>
     </row>
@@ -3701,71 +3701,71 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Magra</t>
+          <t>Khenchela</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Ben Aknoun</t>
+          <t>Biskra</t>
         </is>
       </c>
       <c r="I36" t="n">
         <v>1</v>
       </c>
       <c r="J36" t="n">
-        <v>1.61</v>
+        <v>1.74</v>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>11/11/2023 10:12</t>
+          <t>10/11/2023 03:13</t>
         </is>
       </c>
       <c r="L36" t="n">
-        <v>1.62</v>
+        <v>1.29</v>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>11/11/2023 14:48</t>
+          <t>11/11/2023 10:24</t>
         </is>
       </c>
       <c r="N36" t="n">
-        <v>3.51</v>
+        <v>3.19</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>11/11/2023 10:12</t>
+          <t>10/11/2023 03:13</t>
         </is>
       </c>
       <c r="P36" t="n">
-        <v>3.56</v>
+        <v>4.87</v>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>11/11/2023 14:48</t>
+          <t>11/11/2023 14:54</t>
         </is>
       </c>
       <c r="R36" t="n">
-        <v>5.97</v>
+        <v>4.9</v>
       </c>
       <c r="S36" t="inlineStr">
         <is>
-          <t>11/11/2023 10:12</t>
+          <t>10/11/2023 03:13</t>
         </is>
       </c>
       <c r="T36" t="n">
-        <v>6.3</v>
+        <v>13.77</v>
       </c>
       <c r="U36" t="inlineStr">
         <is>
-          <t>11/11/2023 14:48</t>
+          <t>11/11/2023 14:54</t>
         </is>
       </c>
       <c r="V36" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-es-ben-aknoun/lCJE0FP6/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-biskra/GbL62yef/</t>
         </is>
       </c>
     </row>
@@ -4161,71 +4161,71 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>El Bayadh</t>
+          <t>Constantine</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" t="n">
-        <v>1.45</v>
+        <v>1.59</v>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>16/11/2023 03:42</t>
+          <t>26/10/2023 04:42</t>
         </is>
       </c>
       <c r="L41" t="n">
-        <v>1.45</v>
+        <v>1.31</v>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>17/11/2023 15:18</t>
+          <t>17/11/2023 15:24</t>
         </is>
       </c>
       <c r="N41" t="n">
-        <v>3.74</v>
+        <v>3.47</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>16/11/2023 03:42</t>
+          <t>26/10/2023 04:42</t>
         </is>
       </c>
       <c r="P41" t="n">
-        <v>4.01</v>
+        <v>4.98</v>
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>17/11/2023 15:18</t>
+          <t>17/11/2023 15:24</t>
         </is>
       </c>
       <c r="R41" t="n">
-        <v>7.38</v>
+        <v>5.42</v>
       </c>
       <c r="S41" t="inlineStr">
         <is>
-          <t>16/11/2023 03:42</t>
+          <t>26/10/2023 04:42</t>
         </is>
       </c>
       <c r="T41" t="n">
-        <v>8.609999999999999</v>
+        <v>10.79</v>
       </c>
       <c r="U41" t="inlineStr">
         <is>
-          <t>17/11/2023 15:18</t>
+          <t>17/11/2023 15:24</t>
         </is>
       </c>
       <c r="V41" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-us-souf/UqfmFEv0/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-magra/jgeqGfPg/</t>
         </is>
       </c>
     </row>
@@ -4253,71 +4253,71 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Constantine</t>
+          <t>El Bayadh</t>
         </is>
       </c>
       <c r="G42" t="n">
+        <v>4</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>US Souf</t>
+        </is>
+      </c>
+      <c r="I42" t="n">
         <v>0</v>
       </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>Magra</t>
-        </is>
-      </c>
-      <c r="I42" t="n">
-        <v>1</v>
-      </c>
       <c r="J42" t="n">
-        <v>1.59</v>
+        <v>1.45</v>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>26/10/2023 04:42</t>
+          <t>16/11/2023 03:42</t>
         </is>
       </c>
       <c r="L42" t="n">
-        <v>1.31</v>
+        <v>1.45</v>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>17/11/2023 15:24</t>
+          <t>17/11/2023 15:18</t>
         </is>
       </c>
       <c r="N42" t="n">
-        <v>3.47</v>
+        <v>3.74</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>26/10/2023 04:42</t>
+          <t>16/11/2023 03:42</t>
         </is>
       </c>
       <c r="P42" t="n">
-        <v>4.98</v>
+        <v>4.01</v>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>17/11/2023 15:24</t>
+          <t>17/11/2023 15:18</t>
         </is>
       </c>
       <c r="R42" t="n">
-        <v>5.42</v>
+        <v>7.38</v>
       </c>
       <c r="S42" t="inlineStr">
         <is>
-          <t>26/10/2023 04:42</t>
+          <t>16/11/2023 03:42</t>
         </is>
       </c>
       <c r="T42" t="n">
-        <v>10.79</v>
+        <v>8.609999999999999</v>
       </c>
       <c r="U42" t="inlineStr">
         <is>
-          <t>17/11/2023 15:24</t>
+          <t>17/11/2023 15:18</t>
         </is>
       </c>
       <c r="V42" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-magra/jgeqGfPg/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-us-souf/UqfmFEv0/</t>
         </is>
       </c>
     </row>
@@ -4897,22 +4897,22 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Paradou</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="G49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Constantine</t>
+          <t>El Bayadh</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J49" t="n">
-        <v>1.79</v>
+        <v>2.07</v>
       </c>
       <c r="K49" t="inlineStr">
         <is>
@@ -4920,15 +4920,15 @@
         </is>
       </c>
       <c r="L49" t="n">
-        <v>1.98</v>
+        <v>2.15</v>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>24/11/2023 15:00</t>
+          <t>24/11/2023 14:19</t>
         </is>
       </c>
       <c r="N49" t="n">
-        <v>3.27</v>
+        <v>2.88</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4936,15 +4936,15 @@
         </is>
       </c>
       <c r="P49" t="n">
-        <v>3.08</v>
+        <v>2.9</v>
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>24/11/2023 15:00</t>
+          <t>24/11/2023 15:12</t>
         </is>
       </c>
       <c r="R49" t="n">
-        <v>4.96</v>
+        <v>4.25</v>
       </c>
       <c r="S49" t="inlineStr">
         <is>
@@ -4952,16 +4952,16 @@
         </is>
       </c>
       <c r="T49" t="n">
-        <v>4.37</v>
+        <v>4.06</v>
       </c>
       <c r="U49" t="inlineStr">
         <is>
-          <t>24/11/2023 15:00</t>
+          <t>24/11/2023 14:19</t>
         </is>
       </c>
       <c r="V49" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/paradou-constantine/dOgcmthc/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-el-bayadh/jog1n073/</t>
         </is>
       </c>
     </row>
@@ -4989,22 +4989,22 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Magra</t>
+          <t>Paradou</t>
         </is>
       </c>
       <c r="G50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>El Bayadh</t>
+          <t>Constantine</t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J50" t="n">
-        <v>2.07</v>
+        <v>1.79</v>
       </c>
       <c r="K50" t="inlineStr">
         <is>
@@ -5012,15 +5012,15 @@
         </is>
       </c>
       <c r="L50" t="n">
-        <v>2.15</v>
+        <v>1.98</v>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>24/11/2023 14:19</t>
+          <t>24/11/2023 15:00</t>
         </is>
       </c>
       <c r="N50" t="n">
-        <v>2.88</v>
+        <v>3.27</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -5028,15 +5028,15 @@
         </is>
       </c>
       <c r="P50" t="n">
-        <v>2.9</v>
+        <v>3.08</v>
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>24/11/2023 15:12</t>
+          <t>24/11/2023 15:00</t>
         </is>
       </c>
       <c r="R50" t="n">
-        <v>4.25</v>
+        <v>4.96</v>
       </c>
       <c r="S50" t="inlineStr">
         <is>
@@ -5044,16 +5044,16 @@
         </is>
       </c>
       <c r="T50" t="n">
-        <v>4.06</v>
+        <v>4.37</v>
       </c>
       <c r="U50" t="inlineStr">
         <is>
-          <t>24/11/2023 14:19</t>
+          <t>24/11/2023 15:00</t>
         </is>
       </c>
       <c r="V50" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-el-bayadh/jog1n073/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/paradou-constantine/dOgcmthc/</t>
         </is>
       </c>
     </row>
@@ -6526,6 +6526,374 @@
       <c r="V66" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/algeria/ligue-1/es-setif-biskra/QgE9fdKa/</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E67" s="2" t="n">
+        <v>45275.63541666666</v>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>El Bayadh</t>
+        </is>
+      </c>
+      <c r="G67" t="n">
+        <v>1</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>USM Alger</t>
+        </is>
+      </c>
+      <c r="I67" t="n">
+        <v>1</v>
+      </c>
+      <c r="J67" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>14/12/2023 01:12</t>
+        </is>
+      </c>
+      <c r="L67" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>15/12/2023 15:13</t>
+        </is>
+      </c>
+      <c r="N67" t="n">
+        <v>2.86</v>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>14/12/2023 01:12</t>
+        </is>
+      </c>
+      <c r="P67" t="n">
+        <v>2.85</v>
+      </c>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>15/12/2023 15:10</t>
+        </is>
+      </c>
+      <c r="R67" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="S67" t="inlineStr">
+        <is>
+          <t>14/12/2023 01:12</t>
+        </is>
+      </c>
+      <c r="T67" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="U67" t="inlineStr">
+        <is>
+          <t>15/12/2023 15:13</t>
+        </is>
+      </c>
+      <c r="V67" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-usm-alger/Ywta5DYH/</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E68" s="2" t="n">
+        <v>45275.63541666666</v>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Ben Aknoun</t>
+        </is>
+      </c>
+      <c r="G68" t="n">
+        <v>1</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>CR Belouizdad</t>
+        </is>
+      </c>
+      <c r="I68" t="n">
+        <v>1</v>
+      </c>
+      <c r="J68" t="n">
+        <v>6.41</v>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>14/12/2023 00:12</t>
+        </is>
+      </c>
+      <c r="L68" t="n">
+        <v>5.81</v>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>15/12/2023 15:12</t>
+        </is>
+      </c>
+      <c r="N68" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>14/12/2023 00:12</t>
+        </is>
+      </c>
+      <c r="P68" t="n">
+        <v>3.59</v>
+      </c>
+      <c r="Q68" t="inlineStr">
+        <is>
+          <t>15/12/2023 15:12</t>
+        </is>
+      </c>
+      <c r="R68" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="S68" t="inlineStr">
+        <is>
+          <t>14/12/2023 00:12</t>
+        </is>
+      </c>
+      <c r="T68" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="U68" t="inlineStr">
+        <is>
+          <t>15/12/2023 15:12</t>
+        </is>
+      </c>
+      <c r="V68" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/es-ben-aknoun-cr-belouizdad/CjWzBH4t/</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E69" s="2" t="n">
+        <v>45275.69791666666</v>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Constantine</t>
+        </is>
+      </c>
+      <c r="G69" t="n">
+        <v>2</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>Kabylie</t>
+        </is>
+      </c>
+      <c r="I69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J69" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>14/12/2023 01:12</t>
+        </is>
+      </c>
+      <c r="L69" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>15/12/2023 16:40</t>
+        </is>
+      </c>
+      <c r="N69" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>14/12/2023 01:12</t>
+        </is>
+      </c>
+      <c r="P69" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>15/12/2023 16:40</t>
+        </is>
+      </c>
+      <c r="R69" t="n">
+        <v>4.95</v>
+      </c>
+      <c r="S69" t="inlineStr">
+        <is>
+          <t>14/12/2023 01:12</t>
+        </is>
+      </c>
+      <c r="T69" t="n">
+        <v>6.09</v>
+      </c>
+      <c r="U69" t="inlineStr">
+        <is>
+          <t>15/12/2023 16:35</t>
+        </is>
+      </c>
+      <c r="V69" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-kabylie/zVv9FcdP/</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E70" s="2" t="n">
+        <v>45275.75</v>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>ASO Chlef</t>
+        </is>
+      </c>
+      <c r="G70" t="n">
+        <v>1</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>Paradou</t>
+        </is>
+      </c>
+      <c r="I70" t="n">
+        <v>1</v>
+      </c>
+      <c r="J70" t="n">
+        <v>2</v>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>14/12/2023 01:12</t>
+        </is>
+      </c>
+      <c r="L70" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>15/12/2023 17:50</t>
+        </is>
+      </c>
+      <c r="N70" t="n">
+        <v>2.89</v>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>14/12/2023 01:12</t>
+        </is>
+      </c>
+      <c r="P70" t="n">
+        <v>3.34</v>
+      </c>
+      <c r="Q70" t="inlineStr">
+        <is>
+          <t>15/12/2023 17:55</t>
+        </is>
+      </c>
+      <c r="R70" t="n">
+        <v>4.04</v>
+      </c>
+      <c r="S70" t="inlineStr">
+        <is>
+          <t>14/12/2023 01:12</t>
+        </is>
+      </c>
+      <c r="T70" t="n">
+        <v>5.61</v>
+      </c>
+      <c r="U70" t="inlineStr">
+        <is>
+          <t>15/12/2023 17:17</t>
+        </is>
+      </c>
+      <c r="V70" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/aso-chlef-paradou/2uPm8Fla/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 16-12-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/algeria_ligue-1_2023-2024.xlsx
+++ b/2023/algeria_ligue-1_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V70"/>
+  <dimension ref="A1:V71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6897,6 +6897,98 @@
         </is>
       </c>
     </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E71" s="2" t="n">
+        <v>45276.625</v>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>US Souf</t>
+        </is>
+      </c>
+      <c r="G71" t="n">
+        <v>1</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>ES Setif</t>
+        </is>
+      </c>
+      <c r="I71" t="n">
+        <v>3</v>
+      </c>
+      <c r="J71" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>14/12/2023 09:13</t>
+        </is>
+      </c>
+      <c r="L71" t="n">
+        <v>3.07</v>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>16/12/2023 14:36</t>
+        </is>
+      </c>
+      <c r="N71" t="n">
+        <v>2.86</v>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>14/12/2023 09:13</t>
+        </is>
+      </c>
+      <c r="P71" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>16/12/2023 13:05</t>
+        </is>
+      </c>
+      <c r="R71" t="n">
+        <v>2.09</v>
+      </c>
+      <c r="S71" t="inlineStr">
+        <is>
+          <t>14/12/2023 09:13</t>
+        </is>
+      </c>
+      <c r="T71" t="n">
+        <v>2.57</v>
+      </c>
+      <c r="U71" t="inlineStr">
+        <is>
+          <t>16/12/2023 14:36</t>
+        </is>
+      </c>
+      <c r="V71" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-es-setif/zgNe6gJB/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizado por script em 19-12-2023 02:45
</commit_message>
<xml_diff>
--- a/2023/algeria_ligue-1_2023-2024.xlsx
+++ b/2023/algeria_ligue-1_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V71"/>
+  <dimension ref="A1:V74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1861,7 +1861,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Magra</t>
+          <t>Khenchela</t>
         </is>
       </c>
       <c r="G16" t="n">
@@ -1869,14 +1869,14 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Biskra</t>
+          <t>Kabylie</t>
         </is>
       </c>
       <c r="I16" t="n">
         <v>1</v>
       </c>
       <c r="J16" t="n">
-        <v>1.98</v>
+        <v>2.63</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
@@ -1884,15 +1884,15 @@
         </is>
       </c>
       <c r="L16" t="n">
-        <v>2.1</v>
+        <v>2.05</v>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>29/09/2023 16:44</t>
+          <t>29/09/2023 16:41</t>
         </is>
       </c>
       <c r="N16" t="n">
-        <v>2.89</v>
+        <v>2.62</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1900,15 +1900,15 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>2.77</v>
+        <v>2.75</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>29/09/2023 16:44</t>
+          <t>29/09/2023 16:41</t>
         </is>
       </c>
       <c r="R16" t="n">
-        <v>3.97</v>
+        <v>3.02</v>
       </c>
       <c r="S16" t="inlineStr">
         <is>
@@ -1916,16 +1916,16 @@
         </is>
       </c>
       <c r="T16" t="n">
-        <v>4.54</v>
+        <v>4.88</v>
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>29/09/2023 16:44</t>
+          <t>29/09/2023 16:27</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-biskra/OKYxGuDl/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-kabylie/pUZYGLcr/</t>
         </is>
       </c>
     </row>
@@ -1953,71 +1953,71 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Oran</t>
+          <t>Biskra</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" t="n">
-        <v>2.49</v>
+        <v>1.98</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>28/09/2023 19:27</t>
+          <t>28/09/2023 04:12</t>
         </is>
       </c>
       <c r="L17" t="n">
-        <v>2.14</v>
+        <v>2.1</v>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>29/09/2023 13:29</t>
+          <t>29/09/2023 16:44</t>
         </is>
       </c>
       <c r="N17" t="n">
-        <v>2.88</v>
+        <v>2.89</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>28/09/2023 19:27</t>
+          <t>28/09/2023 04:12</t>
         </is>
       </c>
       <c r="P17" t="n">
-        <v>2.74</v>
+        <v>2.77</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>29/09/2023 14:49</t>
+          <t>29/09/2023 16:44</t>
         </is>
       </c>
       <c r="R17" t="n">
-        <v>3.18</v>
+        <v>3.97</v>
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>28/09/2023 19:27</t>
+          <t>28/09/2023 04:12</t>
         </is>
       </c>
       <c r="T17" t="n">
-        <v>4.43</v>
+        <v>4.54</v>
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>29/09/2023 15:47</t>
+          <t>29/09/2023 16:44</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-oran/6qOsFaSf/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-biskra/OKYxGuDl/</t>
         </is>
       </c>
     </row>
@@ -2045,71 +2045,71 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Khenchela</t>
+          <t>US Souf</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Kabylie</t>
+          <t>Oran</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>2.63</v>
+        <v>2.49</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>28/09/2023 04:12</t>
+          <t>28/09/2023 19:27</t>
         </is>
       </c>
       <c r="L18" t="n">
-        <v>2.05</v>
+        <v>2.14</v>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>29/09/2023 16:41</t>
+          <t>29/09/2023 13:29</t>
         </is>
       </c>
       <c r="N18" t="n">
-        <v>2.62</v>
+        <v>2.88</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>28/09/2023 04:12</t>
+          <t>28/09/2023 19:27</t>
         </is>
       </c>
       <c r="P18" t="n">
-        <v>2.75</v>
+        <v>2.74</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>29/09/2023 16:41</t>
+          <t>29/09/2023 14:49</t>
         </is>
       </c>
       <c r="R18" t="n">
-        <v>3.02</v>
+        <v>3.18</v>
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>28/09/2023 04:12</t>
+          <t>28/09/2023 19:27</t>
         </is>
       </c>
       <c r="T18" t="n">
-        <v>4.88</v>
+        <v>4.43</v>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>29/09/2023 16:27</t>
+          <t>29/09/2023 15:47</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-kabylie/pUZYGLcr/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-oran/6qOsFaSf/</t>
         </is>
       </c>
     </row>
@@ -3609,71 +3609,71 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Magra</t>
+          <t>Khenchela</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Ben Aknoun</t>
+          <t>Biskra</t>
         </is>
       </c>
       <c r="I35" t="n">
         <v>1</v>
       </c>
       <c r="J35" t="n">
-        <v>1.61</v>
+        <v>1.74</v>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>11/11/2023 10:12</t>
+          <t>10/11/2023 03:13</t>
         </is>
       </c>
       <c r="L35" t="n">
-        <v>1.62</v>
+        <v>1.29</v>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>11/11/2023 14:48</t>
+          <t>11/11/2023 10:24</t>
         </is>
       </c>
       <c r="N35" t="n">
-        <v>3.51</v>
+        <v>3.19</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>11/11/2023 10:12</t>
+          <t>10/11/2023 03:13</t>
         </is>
       </c>
       <c r="P35" t="n">
-        <v>3.56</v>
+        <v>4.87</v>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>11/11/2023 14:48</t>
+          <t>11/11/2023 14:54</t>
         </is>
       </c>
       <c r="R35" t="n">
-        <v>5.97</v>
+        <v>4.9</v>
       </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>11/11/2023 10:12</t>
+          <t>10/11/2023 03:13</t>
         </is>
       </c>
       <c r="T35" t="n">
-        <v>6.3</v>
+        <v>13.77</v>
       </c>
       <c r="U35" t="inlineStr">
         <is>
-          <t>11/11/2023 14:48</t>
+          <t>11/11/2023 14:54</t>
         </is>
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-es-ben-aknoun/lCJE0FP6/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-biskra/GbL62yef/</t>
         </is>
       </c>
     </row>
@@ -3701,71 +3701,71 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Khenchela</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Biskra</t>
+          <t>Ben Aknoun</t>
         </is>
       </c>
       <c r="I36" t="n">
         <v>1</v>
       </c>
       <c r="J36" t="n">
-        <v>1.74</v>
+        <v>1.61</v>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>10/11/2023 03:13</t>
+          <t>11/11/2023 10:12</t>
         </is>
       </c>
       <c r="L36" t="n">
-        <v>1.29</v>
+        <v>1.62</v>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>11/11/2023 10:24</t>
+          <t>11/11/2023 14:48</t>
         </is>
       </c>
       <c r="N36" t="n">
-        <v>3.19</v>
+        <v>3.51</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>10/11/2023 03:13</t>
+          <t>11/11/2023 10:12</t>
         </is>
       </c>
       <c r="P36" t="n">
-        <v>4.87</v>
+        <v>3.56</v>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>11/11/2023 14:54</t>
+          <t>11/11/2023 14:48</t>
         </is>
       </c>
       <c r="R36" t="n">
-        <v>4.9</v>
+        <v>5.97</v>
       </c>
       <c r="S36" t="inlineStr">
         <is>
-          <t>10/11/2023 03:13</t>
+          <t>11/11/2023 10:12</t>
         </is>
       </c>
       <c r="T36" t="n">
-        <v>13.77</v>
+        <v>6.3</v>
       </c>
       <c r="U36" t="inlineStr">
         <is>
-          <t>11/11/2023 14:54</t>
+          <t>11/11/2023 14:48</t>
         </is>
       </c>
       <c r="V36" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-biskra/GbL62yef/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-es-ben-aknoun/lCJE0FP6/</t>
         </is>
       </c>
     </row>
@@ -6986,6 +6986,282 @@
       <c r="V71" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-es-setif/zgNe6gJB/</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E72" s="2" t="n">
+        <v>45276.70833333334</v>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Saoura</t>
+        </is>
+      </c>
+      <c r="G72" t="n">
+        <v>2</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>Magra</t>
+        </is>
+      </c>
+      <c r="I72" t="n">
+        <v>1</v>
+      </c>
+      <c r="J72" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>14/12/2023 09:42</t>
+        </is>
+      </c>
+      <c r="L72" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>16/12/2023 16:02</t>
+        </is>
+      </c>
+      <c r="N72" t="n">
+        <v>3.85</v>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>14/12/2023 09:42</t>
+        </is>
+      </c>
+      <c r="P72" t="n">
+        <v>4.18</v>
+      </c>
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>16/12/2023 15:02</t>
+        </is>
+      </c>
+      <c r="R72" t="n">
+        <v>8.01</v>
+      </c>
+      <c r="S72" t="inlineStr">
+        <is>
+          <t>14/12/2023 09:42</t>
+        </is>
+      </c>
+      <c r="T72" t="n">
+        <v>10.57</v>
+      </c>
+      <c r="U72" t="inlineStr">
+        <is>
+          <t>16/12/2023 16:02</t>
+        </is>
+      </c>
+      <c r="V72" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/saoura-magra/tWNi7Z35/</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E73" s="2" t="n">
+        <v>45276.75</v>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>MC Alger</t>
+        </is>
+      </c>
+      <c r="G73" t="n">
+        <v>3</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>Khenchela</t>
+        </is>
+      </c>
+      <c r="I73" t="n">
+        <v>0</v>
+      </c>
+      <c r="J73" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>14/12/2023 09:42</t>
+        </is>
+      </c>
+      <c r="L73" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>16/12/2023 17:24</t>
+        </is>
+      </c>
+      <c r="N73" t="n">
+        <v>3.86</v>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>14/12/2023 09:42</t>
+        </is>
+      </c>
+      <c r="P73" t="n">
+        <v>4.52</v>
+      </c>
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>16/12/2023 17:24</t>
+        </is>
+      </c>
+      <c r="R73" t="n">
+        <v>7.89</v>
+      </c>
+      <c r="S73" t="inlineStr">
+        <is>
+          <t>14/12/2023 09:42</t>
+        </is>
+      </c>
+      <c r="T73" t="n">
+        <v>12.14</v>
+      </c>
+      <c r="U73" t="inlineStr">
+        <is>
+          <t>16/12/2023 17:24</t>
+        </is>
+      </c>
+      <c r="V73" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/mc-alger-khenchela/p4Ur9eZh/</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E74" s="2" t="n">
+        <v>45276.79166666666</v>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Oran</t>
+        </is>
+      </c>
+      <c r="G74" t="n">
+        <v>0</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Biskra</t>
+        </is>
+      </c>
+      <c r="I74" t="n">
+        <v>1</v>
+      </c>
+      <c r="J74" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>14/12/2023 09:42</t>
+        </is>
+      </c>
+      <c r="L74" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>16/12/2023 18:55</t>
+        </is>
+      </c>
+      <c r="N74" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>14/12/2023 09:42</t>
+        </is>
+      </c>
+      <c r="P74" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="Q74" t="inlineStr">
+        <is>
+          <t>16/12/2023 18:59</t>
+        </is>
+      </c>
+      <c r="R74" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="S74" t="inlineStr">
+        <is>
+          <t>14/12/2023 09:42</t>
+        </is>
+      </c>
+      <c r="T74" t="n">
+        <v>5.16</v>
+      </c>
+      <c r="U74" t="inlineStr">
+        <is>
+          <t>16/12/2023 18:59</t>
+        </is>
+      </c>
+      <c r="V74" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-biskra/6DVvAyKn/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 02-01-2024 20:45
</commit_message>
<xml_diff>
--- a/2023/algeria_ligue-1_2023-2024.xlsx
+++ b/2023/algeria_ligue-1_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V74"/>
+  <dimension ref="A1:V81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -849,71 +849,71 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Magra</t>
+          <t>MC Alger</t>
         </is>
       </c>
       <c r="G5" t="n">
+        <v>4</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Ben Aknoun</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
         <v>0</v>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Kabylie</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>1</v>
-      </c>
       <c r="J5" t="n">
-        <v>2.84</v>
+        <v>1.4</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>15/09/2023 13:42</t>
+          <t>16/09/2023 03:43</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>3.8</v>
+        <v>1.3</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>16/09/2023 16:12</t>
+          <t>16/09/2023 10:40</t>
         </is>
       </c>
       <c r="N5" t="n">
-        <v>2.63</v>
+        <v>4.19</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>15/09/2023 13:42</t>
+          <t>16/09/2023 03:43</t>
         </is>
       </c>
       <c r="P5" t="n">
-        <v>2.84</v>
+        <v>4.81</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>16/09/2023 15:03</t>
+          <t>16/09/2023 16:47</t>
         </is>
       </c>
       <c r="R5" t="n">
-        <v>2.72</v>
+        <v>8.529999999999999</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>15/09/2023 13:42</t>
+          <t>16/09/2023 03:43</t>
         </is>
       </c>
       <c r="T5" t="n">
-        <v>2.26</v>
+        <v>12.64</v>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>16/09/2023 16:12</t>
+          <t>16/09/2023 16:47</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-kabylie/YFXa8c8H/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/mc-alger-es-ben-aknoun/WjyqCu9h/</t>
         </is>
       </c>
     </row>
@@ -941,71 +941,71 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>MC Alger</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Ben Aknoun</t>
+          <t>Kabylie</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>1.4</v>
+        <v>2.84</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>16/09/2023 03:43</t>
+          <t>15/09/2023 13:42</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>1.3</v>
+        <v>3.8</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>16/09/2023 10:40</t>
+          <t>16/09/2023 16:12</t>
         </is>
       </c>
       <c r="N6" t="n">
-        <v>4.19</v>
+        <v>2.63</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>16/09/2023 03:43</t>
+          <t>15/09/2023 13:42</t>
         </is>
       </c>
       <c r="P6" t="n">
-        <v>4.81</v>
+        <v>2.84</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>16/09/2023 16:47</t>
+          <t>16/09/2023 15:03</t>
         </is>
       </c>
       <c r="R6" t="n">
-        <v>8.529999999999999</v>
+        <v>2.72</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>16/09/2023 03:43</t>
+          <t>15/09/2023 13:42</t>
         </is>
       </c>
       <c r="T6" t="n">
-        <v>12.64</v>
+        <v>2.26</v>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>16/09/2023 16:47</t>
+          <t>16/09/2023 16:12</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/mc-alger-es-ben-aknoun/WjyqCu9h/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-kabylie/YFXa8c8H/</t>
         </is>
       </c>
     </row>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Constantine</t>
+          <t>Ben Aknoun</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -1133,63 +1133,63 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>MC Alger</t>
+          <t>ASO Chlef</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" t="n">
-        <v>1.98</v>
+        <v>2.81</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>21/09/2023 05:12</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>3.68</v>
+        <v>2.51</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>22/09/2023 16:51</t>
+          <t>22/09/2023 16:00</t>
         </is>
       </c>
       <c r="N8" t="n">
-        <v>2.89</v>
+        <v>3.04</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>21/09/2023 05:12</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="P8" t="n">
-        <v>2.92</v>
+        <v>3.06</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>22/09/2023 16:51</t>
+          <t>22/09/2023 16:34</t>
         </is>
       </c>
       <c r="R8" t="n">
-        <v>3.97</v>
+        <v>2.64</v>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>21/09/2023 05:12</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="T8" t="n">
-        <v>2.26</v>
+        <v>3.01</v>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>22/09/2023 16:51</t>
+          <t>22/09/2023 16:00</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-mc-alger/Eoq3MszL/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/es-ben-aknoun-aso-chlef/WMgbNNKE/</t>
         </is>
       </c>
     </row>
@@ -1217,7 +1217,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Ben Aknoun</t>
+          <t>Constantine</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -1225,63 +1225,63 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>ASO Chlef</t>
+          <t>MC Alger</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>2.81</v>
+        <v>1.98</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>21/09/2023 05:12</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>2.51</v>
+        <v>3.68</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>22/09/2023 16:00</t>
+          <t>22/09/2023 16:51</t>
         </is>
       </c>
       <c r="N9" t="n">
-        <v>3.04</v>
+        <v>2.89</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>21/09/2023 05:12</t>
         </is>
       </c>
       <c r="P9" t="n">
-        <v>3.06</v>
+        <v>2.92</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>22/09/2023 16:34</t>
+          <t>22/09/2023 16:51</t>
         </is>
       </c>
       <c r="R9" t="n">
-        <v>2.64</v>
+        <v>3.97</v>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>21/09/2023 05:12</t>
         </is>
       </c>
       <c r="T9" t="n">
-        <v>3.01</v>
+        <v>2.26</v>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>22/09/2023 16:00</t>
+          <t>22/09/2023 16:51</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/es-ben-aknoun-aso-chlef/WMgbNNKE/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-mc-alger/Eoq3MszL/</t>
         </is>
       </c>
     </row>
@@ -1861,71 +1861,71 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Khenchela</t>
+          <t>US Souf</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Kabylie</t>
+          <t>Oran</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>2.63</v>
+        <v>2.49</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>28/09/2023 04:12</t>
+          <t>28/09/2023 19:27</t>
         </is>
       </c>
       <c r="L16" t="n">
-        <v>2.05</v>
+        <v>2.14</v>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>29/09/2023 16:41</t>
+          <t>29/09/2023 13:29</t>
         </is>
       </c>
       <c r="N16" t="n">
-        <v>2.62</v>
+        <v>2.88</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>28/09/2023 04:12</t>
+          <t>28/09/2023 19:27</t>
         </is>
       </c>
       <c r="P16" t="n">
-        <v>2.75</v>
+        <v>2.74</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>29/09/2023 16:41</t>
+          <t>29/09/2023 14:49</t>
         </is>
       </c>
       <c r="R16" t="n">
-        <v>3.02</v>
+        <v>3.18</v>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>28/09/2023 04:12</t>
+          <t>28/09/2023 19:27</t>
         </is>
       </c>
       <c r="T16" t="n">
-        <v>4.88</v>
+        <v>4.43</v>
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>29/09/2023 16:27</t>
+          <t>29/09/2023 15:47</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-kabylie/pUZYGLcr/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-oran/6qOsFaSf/</t>
         </is>
       </c>
     </row>
@@ -2045,71 +2045,71 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Khenchela</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Oran</t>
+          <t>Kabylie</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="n">
-        <v>2.49</v>
+        <v>2.63</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>28/09/2023 19:27</t>
+          <t>28/09/2023 04:12</t>
         </is>
       </c>
       <c r="L18" t="n">
-        <v>2.14</v>
+        <v>2.05</v>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>29/09/2023 13:29</t>
+          <t>29/09/2023 16:41</t>
         </is>
       </c>
       <c r="N18" t="n">
-        <v>2.88</v>
+        <v>2.62</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>28/09/2023 19:27</t>
+          <t>28/09/2023 04:12</t>
         </is>
       </c>
       <c r="P18" t="n">
-        <v>2.74</v>
+        <v>2.75</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>29/09/2023 14:49</t>
+          <t>29/09/2023 16:41</t>
         </is>
       </c>
       <c r="R18" t="n">
-        <v>3.18</v>
+        <v>3.02</v>
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>28/09/2023 19:27</t>
+          <t>28/09/2023 04:12</t>
         </is>
       </c>
       <c r="T18" t="n">
-        <v>4.43</v>
+        <v>4.88</v>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>29/09/2023 15:47</t>
+          <t>29/09/2023 16:27</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-oran/6qOsFaSf/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-kabylie/pUZYGLcr/</t>
         </is>
       </c>
     </row>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Biskra</t>
+          <t>Oran</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -2513,14 +2513,14 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Paradou</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>2.18</v>
+        <v>1.98</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
@@ -2528,15 +2528,15 @@
         </is>
       </c>
       <c r="L23" t="n">
-        <v>2.03</v>
+        <v>1.65</v>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>06/10/2023 19:34</t>
+          <t>06/10/2023 17:55</t>
         </is>
       </c>
       <c r="N23" t="n">
-        <v>2.84</v>
+        <v>2.89</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2544,15 +2544,15 @@
         </is>
       </c>
       <c r="P23" t="n">
-        <v>3</v>
+        <v>3.28</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>06/10/2023 18:05</t>
+          <t>06/10/2023 19:03</t>
         </is>
       </c>
       <c r="R23" t="n">
-        <v>3.56</v>
+        <v>3.98</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
@@ -2560,16 +2560,16 @@
         </is>
       </c>
       <c r="T23" t="n">
-        <v>4.33</v>
+        <v>5.91</v>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>06/10/2023 19:34</t>
+          <t>06/10/2023 17:55</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-paradou/hhWUzskE/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-magra/WrVYZ04K/</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Oran</t>
+          <t>Biskra</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -2605,14 +2605,14 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Magra</t>
+          <t>Paradou</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J24" t="n">
-        <v>1.98</v>
+        <v>2.18</v>
       </c>
       <c r="K24" t="inlineStr">
         <is>
@@ -2620,15 +2620,15 @@
         </is>
       </c>
       <c r="L24" t="n">
-        <v>1.65</v>
+        <v>2.03</v>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>06/10/2023 17:55</t>
+          <t>06/10/2023 19:34</t>
         </is>
       </c>
       <c r="N24" t="n">
-        <v>2.89</v>
+        <v>2.84</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2636,15 +2636,15 @@
         </is>
       </c>
       <c r="P24" t="n">
-        <v>3.28</v>
+        <v>3</v>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>06/10/2023 19:03</t>
+          <t>06/10/2023 18:05</t>
         </is>
       </c>
       <c r="R24" t="n">
-        <v>3.98</v>
+        <v>3.56</v>
       </c>
       <c r="S24" t="inlineStr">
         <is>
@@ -2652,16 +2652,16 @@
         </is>
       </c>
       <c r="T24" t="n">
-        <v>5.91</v>
+        <v>4.33</v>
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>06/10/2023 17:55</t>
+          <t>06/10/2023 19:34</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-magra/WrVYZ04K/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-paradou/hhWUzskE/</t>
         </is>
       </c>
     </row>
@@ -4161,71 +4161,71 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Constantine</t>
+          <t>El Bayadh</t>
         </is>
       </c>
       <c r="G41" t="n">
+        <v>4</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>US Souf</t>
+        </is>
+      </c>
+      <c r="I41" t="n">
         <v>0</v>
       </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>Magra</t>
-        </is>
-      </c>
-      <c r="I41" t="n">
-        <v>1</v>
-      </c>
       <c r="J41" t="n">
-        <v>1.59</v>
+        <v>1.45</v>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>26/10/2023 04:42</t>
+          <t>16/11/2023 03:42</t>
         </is>
       </c>
       <c r="L41" t="n">
-        <v>1.31</v>
+        <v>1.45</v>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>17/11/2023 15:24</t>
+          <t>17/11/2023 15:18</t>
         </is>
       </c>
       <c r="N41" t="n">
-        <v>3.47</v>
+        <v>3.74</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>26/10/2023 04:42</t>
+          <t>16/11/2023 03:42</t>
         </is>
       </c>
       <c r="P41" t="n">
-        <v>4.98</v>
+        <v>4.01</v>
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>17/11/2023 15:24</t>
+          <t>17/11/2023 15:18</t>
         </is>
       </c>
       <c r="R41" t="n">
-        <v>5.42</v>
+        <v>7.38</v>
       </c>
       <c r="S41" t="inlineStr">
         <is>
-          <t>26/10/2023 04:42</t>
+          <t>16/11/2023 03:42</t>
         </is>
       </c>
       <c r="T41" t="n">
-        <v>10.79</v>
+        <v>8.609999999999999</v>
       </c>
       <c r="U41" t="inlineStr">
         <is>
-          <t>17/11/2023 15:24</t>
+          <t>17/11/2023 15:18</t>
         </is>
       </c>
       <c r="V41" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-magra/jgeqGfPg/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-us-souf/UqfmFEv0/</t>
         </is>
       </c>
     </row>
@@ -4253,71 +4253,71 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>El Bayadh</t>
+          <t>Constantine</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" t="n">
-        <v>1.45</v>
+        <v>1.59</v>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>16/11/2023 03:42</t>
+          <t>26/10/2023 04:42</t>
         </is>
       </c>
       <c r="L42" t="n">
-        <v>1.45</v>
+        <v>1.31</v>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>17/11/2023 15:18</t>
+          <t>17/11/2023 15:24</t>
         </is>
       </c>
       <c r="N42" t="n">
-        <v>3.74</v>
+        <v>3.47</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>16/11/2023 03:42</t>
+          <t>26/10/2023 04:42</t>
         </is>
       </c>
       <c r="P42" t="n">
-        <v>4.01</v>
+        <v>4.98</v>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>17/11/2023 15:18</t>
+          <t>17/11/2023 15:24</t>
         </is>
       </c>
       <c r="R42" t="n">
-        <v>7.38</v>
+        <v>5.42</v>
       </c>
       <c r="S42" t="inlineStr">
         <is>
-          <t>16/11/2023 03:42</t>
+          <t>26/10/2023 04:42</t>
         </is>
       </c>
       <c r="T42" t="n">
-        <v>8.609999999999999</v>
+        <v>10.79</v>
       </c>
       <c r="U42" t="inlineStr">
         <is>
-          <t>17/11/2023 15:18</t>
+          <t>17/11/2023 15:24</t>
         </is>
       </c>
       <c r="V42" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-us-souf/UqfmFEv0/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-magra/jgeqGfPg/</t>
         </is>
       </c>
     </row>
@@ -5081,22 +5081,22 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Khenchela</t>
+          <t>US Souf</t>
         </is>
       </c>
       <c r="G51" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Ben Aknoun</t>
+          <t>MC Alger</t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J51" t="n">
-        <v>1.36</v>
+        <v>4.45</v>
       </c>
       <c r="K51" t="inlineStr">
         <is>
@@ -5104,7 +5104,7 @@
         </is>
       </c>
       <c r="L51" t="n">
-        <v>1.32</v>
+        <v>5.84</v>
       </c>
       <c r="M51" t="inlineStr">
         <is>
@@ -5112,7 +5112,7 @@
         </is>
       </c>
       <c r="N51" t="n">
-        <v>4.19</v>
+        <v>2.95</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -5120,7 +5120,7 @@
         </is>
       </c>
       <c r="P51" t="n">
-        <v>4.72</v>
+        <v>3.36</v>
       </c>
       <c r="Q51" t="inlineStr">
         <is>
@@ -5128,7 +5128,7 @@
         </is>
       </c>
       <c r="R51" t="n">
-        <v>7.76</v>
+        <v>1.89</v>
       </c>
       <c r="S51" t="inlineStr">
         <is>
@@ -5136,7 +5136,7 @@
         </is>
       </c>
       <c r="T51" t="n">
-        <v>11.86</v>
+        <v>1.7</v>
       </c>
       <c r="U51" t="inlineStr">
         <is>
@@ -5145,7 +5145,7 @@
       </c>
       <c r="V51" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-es-ben-aknoun/bwyflMxi/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-mc-alger/Uyh5oKM9/</t>
         </is>
       </c>
     </row>
@@ -5173,22 +5173,22 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Khenchela</t>
         </is>
       </c>
       <c r="G52" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>MC Alger</t>
+          <t>Ben Aknoun</t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J52" t="n">
-        <v>4.45</v>
+        <v>1.36</v>
       </c>
       <c r="K52" t="inlineStr">
         <is>
@@ -5196,7 +5196,7 @@
         </is>
       </c>
       <c r="L52" t="n">
-        <v>5.84</v>
+        <v>1.32</v>
       </c>
       <c r="M52" t="inlineStr">
         <is>
@@ -5204,7 +5204,7 @@
         </is>
       </c>
       <c r="N52" t="n">
-        <v>2.95</v>
+        <v>4.19</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -5212,7 +5212,7 @@
         </is>
       </c>
       <c r="P52" t="n">
-        <v>3.36</v>
+        <v>4.72</v>
       </c>
       <c r="Q52" t="inlineStr">
         <is>
@@ -5220,7 +5220,7 @@
         </is>
       </c>
       <c r="R52" t="n">
-        <v>1.89</v>
+        <v>7.76</v>
       </c>
       <c r="S52" t="inlineStr">
         <is>
@@ -5228,7 +5228,7 @@
         </is>
       </c>
       <c r="T52" t="n">
-        <v>1.7</v>
+        <v>11.86</v>
       </c>
       <c r="U52" t="inlineStr">
         <is>
@@ -5237,7 +5237,7 @@
       </c>
       <c r="V52" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-mc-alger/Uyh5oKM9/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-es-ben-aknoun/bwyflMxi/</t>
         </is>
       </c>
     </row>
@@ -7262,6 +7262,650 @@
       <c r="V74" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-biskra/6DVvAyKn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E75" s="2" t="n">
+        <v>45288.79166666666</v>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>CR Belouizdad</t>
+        </is>
+      </c>
+      <c r="G75" t="n">
+        <v>2</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Constantine</t>
+        </is>
+      </c>
+      <c r="I75" t="n">
+        <v>1</v>
+      </c>
+      <c r="J75" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>27/12/2023 07:12</t>
+        </is>
+      </c>
+      <c r="L75" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>28/12/2023 18:32</t>
+        </is>
+      </c>
+      <c r="N75" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>27/12/2023 07:12</t>
+        </is>
+      </c>
+      <c r="P75" t="n">
+        <v>3.57</v>
+      </c>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>28/12/2023 18:32</t>
+        </is>
+      </c>
+      <c r="R75" t="n">
+        <v>4.87</v>
+      </c>
+      <c r="S75" t="inlineStr">
+        <is>
+          <t>27/12/2023 07:12</t>
+        </is>
+      </c>
+      <c r="T75" t="n">
+        <v>7.23</v>
+      </c>
+      <c r="U75" t="inlineStr">
+        <is>
+          <t>28/12/2023 18:32</t>
+        </is>
+      </c>
+      <c r="V75" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/cr-belouizdad-constantine/tp3QLYIb/</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E76" s="2" t="n">
+        <v>45289.63541666666</v>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Khenchela</t>
+        </is>
+      </c>
+      <c r="G76" t="n">
+        <v>2</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>ASO Chlef</t>
+        </is>
+      </c>
+      <c r="I76" t="n">
+        <v>1</v>
+      </c>
+      <c r="J76" t="n">
+        <v>2.11</v>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>21/12/2023 03:42</t>
+        </is>
+      </c>
+      <c r="L76" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>29/12/2023 14:40</t>
+        </is>
+      </c>
+      <c r="N76" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>21/12/2023 03:42</t>
+        </is>
+      </c>
+      <c r="P76" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>29/12/2023 14:40</t>
+        </is>
+      </c>
+      <c r="R76" t="n">
+        <v>3.83</v>
+      </c>
+      <c r="S76" t="inlineStr">
+        <is>
+          <t>21/12/2023 03:42</t>
+        </is>
+      </c>
+      <c r="T76" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="U76" t="inlineStr">
+        <is>
+          <t>29/12/2023 14:40</t>
+        </is>
+      </c>
+      <c r="V76" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-aso-chlef/G2V34XmO/</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E77" s="2" t="n">
+        <v>45289.63541666666</v>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Magra</t>
+        </is>
+      </c>
+      <c r="G77" t="n">
+        <v>1</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>US Souf</t>
+        </is>
+      </c>
+      <c r="I77" t="n">
+        <v>0</v>
+      </c>
+      <c r="J77" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>28/12/2023 07:12</t>
+        </is>
+      </c>
+      <c r="L77" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>29/12/2023 15:07</t>
+        </is>
+      </c>
+      <c r="N77" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>28/12/2023 07:12</t>
+        </is>
+      </c>
+      <c r="P77" t="n">
+        <v>3.42</v>
+      </c>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>29/12/2023 15:07</t>
+        </is>
+      </c>
+      <c r="R77" t="n">
+        <v>5.55</v>
+      </c>
+      <c r="S77" t="inlineStr">
+        <is>
+          <t>28/12/2023 07:12</t>
+        </is>
+      </c>
+      <c r="T77" t="n">
+        <v>5.41</v>
+      </c>
+      <c r="U77" t="inlineStr">
+        <is>
+          <t>29/12/2023 15:07</t>
+        </is>
+      </c>
+      <c r="V77" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-us-souf/6RADOzZu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E78" s="2" t="n">
+        <v>45289.63541666666</v>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Paradou</t>
+        </is>
+      </c>
+      <c r="G78" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>Saoura</t>
+        </is>
+      </c>
+      <c r="I78" t="n">
+        <v>0</v>
+      </c>
+      <c r="J78" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>21/12/2023 03:42</t>
+        </is>
+      </c>
+      <c r="L78" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>29/12/2023 15:10</t>
+        </is>
+      </c>
+      <c r="N78" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>21/12/2023 03:42</t>
+        </is>
+      </c>
+      <c r="P78" t="n">
+        <v>2.84</v>
+      </c>
+      <c r="Q78" t="inlineStr">
+        <is>
+          <t>29/12/2023 15:10</t>
+        </is>
+      </c>
+      <c r="R78" t="n">
+        <v>3.77</v>
+      </c>
+      <c r="S78" t="inlineStr">
+        <is>
+          <t>21/12/2023 03:42</t>
+        </is>
+      </c>
+      <c r="T78" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="U78" t="inlineStr">
+        <is>
+          <t>29/12/2023 15:08</t>
+        </is>
+      </c>
+      <c r="V78" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/paradou-saoura/fgU73i3U/</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E79" s="2" t="n">
+        <v>45289.66666666666</v>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>ES Setif</t>
+        </is>
+      </c>
+      <c r="G79" t="n">
+        <v>1</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Oran</t>
+        </is>
+      </c>
+      <c r="I79" t="n">
+        <v>0</v>
+      </c>
+      <c r="J79" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>28/12/2023 07:12</t>
+        </is>
+      </c>
+      <c r="L79" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>29/12/2023 15:51</t>
+        </is>
+      </c>
+      <c r="N79" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>28/12/2023 07:12</t>
+        </is>
+      </c>
+      <c r="P79" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>29/12/2023 15:55</t>
+        </is>
+      </c>
+      <c r="R79" t="n">
+        <v>6.24</v>
+      </c>
+      <c r="S79" t="inlineStr">
+        <is>
+          <t>28/12/2023 07:12</t>
+        </is>
+      </c>
+      <c r="T79" t="n">
+        <v>10.82</v>
+      </c>
+      <c r="U79" t="inlineStr">
+        <is>
+          <t>29/12/2023 15:55</t>
+        </is>
+      </c>
+      <c r="V79" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/es-setif-oran/pI9HNfln/</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E80" s="2" t="n">
+        <v>45289.75</v>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>USM Alger</t>
+        </is>
+      </c>
+      <c r="G80" t="n">
+        <v>0</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>MC Alger</t>
+        </is>
+      </c>
+      <c r="I80" t="n">
+        <v>0</v>
+      </c>
+      <c r="J80" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>28/12/2023 07:12</t>
+        </is>
+      </c>
+      <c r="L80" t="n">
+        <v>3.62</v>
+      </c>
+      <c r="M80" t="inlineStr">
+        <is>
+          <t>29/12/2023 17:59</t>
+        </is>
+      </c>
+      <c r="N80" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>28/12/2023 07:12</t>
+        </is>
+      </c>
+      <c r="P80" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>29/12/2023 17:56</t>
+        </is>
+      </c>
+      <c r="R80" t="n">
+        <v>2.42</v>
+      </c>
+      <c r="S80" t="inlineStr">
+        <is>
+          <t>28/12/2023 07:12</t>
+        </is>
+      </c>
+      <c r="T80" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="U80" t="inlineStr">
+        <is>
+          <t>29/12/2023 17:59</t>
+        </is>
+      </c>
+      <c r="V80" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/usm-alger-mc-alger/jDDqjB3f/</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E81" s="2" t="n">
+        <v>45289.75</v>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Biskra</t>
+        </is>
+      </c>
+      <c r="G81" t="n">
+        <v>1</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Ben Aknoun</t>
+        </is>
+      </c>
+      <c r="I81" t="n">
+        <v>1</v>
+      </c>
+      <c r="J81" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>28/12/2023 07:12</t>
+        </is>
+      </c>
+      <c r="L81" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>29/12/2023 17:57</t>
+        </is>
+      </c>
+      <c r="N81" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>28/12/2023 07:12</t>
+        </is>
+      </c>
+      <c r="P81" t="n">
+        <v>4.05</v>
+      </c>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>29/12/2023 17:57</t>
+        </is>
+      </c>
+      <c r="R81" t="n">
+        <v>5.97</v>
+      </c>
+      <c r="S81" t="inlineStr">
+        <is>
+          <t>28/12/2023 07:12</t>
+        </is>
+      </c>
+      <c r="T81" t="n">
+        <v>9.98</v>
+      </c>
+      <c r="U81" t="inlineStr">
+        <is>
+          <t>29/12/2023 17:57</t>
+        </is>
+      </c>
+      <c r="V81" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-es-ben-aknoun/z72UKhY4/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 05-01-2024 20:45
</commit_message>
<xml_diff>
--- a/2023/algeria_ligue-1_2023-2024.xlsx
+++ b/2023/algeria_ligue-1_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V81"/>
+  <dimension ref="A1:V86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1493,71 +1493,71 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Biskra</t>
+          <t>Oran</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Saoura</t>
         </is>
       </c>
       <c r="I12" t="n">
         <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>1.71</v>
+        <v>2.54</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>22/09/2023 15:13</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="L12" t="n">
-        <v>1.65</v>
+        <v>2.34</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>23/09/2023 19:13</t>
+          <t>23/09/2023 18:03</t>
         </is>
       </c>
       <c r="N12" t="n">
-        <v>3.22</v>
+        <v>2.65</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>22/09/2023 15:13</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="P12" t="n">
-        <v>3.47</v>
+        <v>2.71</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>23/09/2023 19:13</t>
+          <t>23/09/2023 18:03</t>
         </is>
       </c>
       <c r="R12" t="n">
-        <v>4.87</v>
+        <v>3.11</v>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>22/09/2023 15:13</t>
+          <t>22/09/2023 08:13</t>
         </is>
       </c>
       <c r="T12" t="n">
-        <v>6.17</v>
+        <v>3.84</v>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>23/09/2023 19:13</t>
+          <t>23/09/2023 18:03</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-us-souf/KYnDaKS7/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-saoura/YyyeO358/</t>
         </is>
       </c>
     </row>
@@ -1585,71 +1585,71 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Oran</t>
+          <t>Biskra</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Saoura</t>
+          <t>US Souf</t>
         </is>
       </c>
       <c r="I13" t="n">
         <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>2.54</v>
+        <v>1.71</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>22/09/2023 15:13</t>
         </is>
       </c>
       <c r="L13" t="n">
-        <v>2.34</v>
+        <v>1.65</v>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>23/09/2023 18:03</t>
+          <t>23/09/2023 19:13</t>
         </is>
       </c>
       <c r="N13" t="n">
-        <v>2.65</v>
+        <v>3.22</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>22/09/2023 15:13</t>
         </is>
       </c>
       <c r="P13" t="n">
-        <v>2.71</v>
+        <v>3.47</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>23/09/2023 18:03</t>
+          <t>23/09/2023 19:13</t>
         </is>
       </c>
       <c r="R13" t="n">
-        <v>3.11</v>
+        <v>4.87</v>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>22/09/2023 08:13</t>
+          <t>22/09/2023 15:13</t>
         </is>
       </c>
       <c r="T13" t="n">
-        <v>3.84</v>
+        <v>6.17</v>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>23/09/2023 18:03</t>
+          <t>23/09/2023 19:13</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-saoura/YyyeO358/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-us-souf/KYnDaKS7/</t>
         </is>
       </c>
     </row>
@@ -2321,22 +2321,22 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Constantine</t>
+          <t>MC Alger</t>
         </is>
       </c>
       <c r="G21" t="n">
+        <v>5</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>ES Setif</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
         <v>3</v>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Saoura</t>
-        </is>
-      </c>
-      <c r="I21" t="n">
-        <v>0</v>
-      </c>
       <c r="J21" t="n">
-        <v>1.76</v>
+        <v>1.53</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
@@ -2344,15 +2344,15 @@
         </is>
       </c>
       <c r="L21" t="n">
-        <v>1.75</v>
+        <v>1.52</v>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>06/10/2023 16:25</t>
+          <t>06/10/2023 16:29</t>
         </is>
       </c>
       <c r="N21" t="n">
-        <v>3.23</v>
+        <v>3.6</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -2360,15 +2360,15 @@
         </is>
       </c>
       <c r="P21" t="n">
-        <v>3.26</v>
+        <v>3.71</v>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>06/10/2023 16:28</t>
+          <t>06/10/2023 16:34</t>
         </is>
       </c>
       <c r="R21" t="n">
-        <v>4.69</v>
+        <v>6.62</v>
       </c>
       <c r="S21" t="inlineStr">
         <is>
@@ -2376,16 +2376,16 @@
         </is>
       </c>
       <c r="T21" t="n">
-        <v>5.64</v>
+        <v>7.77</v>
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>06/10/2023 15:05</t>
+          <t>06/10/2023 16:34</t>
         </is>
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-saoura/2RL4UvSs/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/mc-alger-es-setif/OtADSIdf/</t>
         </is>
       </c>
     </row>
@@ -2413,22 +2413,22 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>MC Alger</t>
+          <t>Constantine</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>ES Setif</t>
+          <t>Saoura</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>1.53</v>
+        <v>1.76</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
@@ -2436,15 +2436,15 @@
         </is>
       </c>
       <c r="L22" t="n">
-        <v>1.52</v>
+        <v>1.75</v>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>06/10/2023 16:29</t>
+          <t>06/10/2023 16:25</t>
         </is>
       </c>
       <c r="N22" t="n">
-        <v>3.6</v>
+        <v>3.23</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2452,15 +2452,15 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>3.71</v>
+        <v>3.26</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>06/10/2023 16:34</t>
+          <t>06/10/2023 16:28</t>
         </is>
       </c>
       <c r="R22" t="n">
-        <v>6.62</v>
+        <v>4.69</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>
@@ -2468,16 +2468,16 @@
         </is>
       </c>
       <c r="T22" t="n">
-        <v>7.77</v>
+        <v>5.64</v>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>06/10/2023 16:34</t>
+          <t>06/10/2023 15:05</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/mc-alger-es-setif/OtADSIdf/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-saoura/2RL4UvSs/</t>
         </is>
       </c>
     </row>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Oran</t>
+          <t>Biskra</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -2513,14 +2513,14 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Magra</t>
+          <t>Paradou</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J23" t="n">
-        <v>1.98</v>
+        <v>2.18</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
@@ -2528,15 +2528,15 @@
         </is>
       </c>
       <c r="L23" t="n">
-        <v>1.65</v>
+        <v>2.03</v>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>06/10/2023 17:55</t>
+          <t>06/10/2023 19:34</t>
         </is>
       </c>
       <c r="N23" t="n">
-        <v>2.89</v>
+        <v>2.84</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2544,15 +2544,15 @@
         </is>
       </c>
       <c r="P23" t="n">
-        <v>3.28</v>
+        <v>3</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>06/10/2023 19:03</t>
+          <t>06/10/2023 18:05</t>
         </is>
       </c>
       <c r="R23" t="n">
-        <v>3.98</v>
+        <v>3.56</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
@@ -2560,16 +2560,16 @@
         </is>
       </c>
       <c r="T23" t="n">
-        <v>5.91</v>
+        <v>4.33</v>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>06/10/2023 17:55</t>
+          <t>06/10/2023 19:34</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-magra/WrVYZ04K/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-paradou/hhWUzskE/</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Biskra</t>
+          <t>Oran</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -2605,14 +2605,14 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Paradou</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>2.18</v>
+        <v>1.98</v>
       </c>
       <c r="K24" t="inlineStr">
         <is>
@@ -2620,15 +2620,15 @@
         </is>
       </c>
       <c r="L24" t="n">
-        <v>2.03</v>
+        <v>1.65</v>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>06/10/2023 19:34</t>
+          <t>06/10/2023 17:55</t>
         </is>
       </c>
       <c r="N24" t="n">
-        <v>2.84</v>
+        <v>2.89</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2636,15 +2636,15 @@
         </is>
       </c>
       <c r="P24" t="n">
-        <v>3</v>
+        <v>3.28</v>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>06/10/2023 18:05</t>
+          <t>06/10/2023 19:03</t>
         </is>
       </c>
       <c r="R24" t="n">
-        <v>3.56</v>
+        <v>3.98</v>
       </c>
       <c r="S24" t="inlineStr">
         <is>
@@ -2652,16 +2652,16 @@
         </is>
       </c>
       <c r="T24" t="n">
-        <v>4.33</v>
+        <v>5.91</v>
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>06/10/2023 19:34</t>
+          <t>06/10/2023 17:55</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-paradou/hhWUzskE/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-magra/WrVYZ04K/</t>
         </is>
       </c>
     </row>
@@ -3241,71 +3241,71 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Paradou</t>
+          <t>US Souf</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Oran</t>
+          <t>Constantine</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J31" t="n">
-        <v>1.48</v>
+        <v>3.14</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>19/10/2023 04:42</t>
+          <t>10/11/2023 06:42</t>
         </is>
       </c>
       <c r="L31" t="n">
-        <v>1.46</v>
+        <v>3.21</v>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>10/11/2023 14:57</t>
+          <t>10/11/2023 15:16</t>
         </is>
       </c>
       <c r="N31" t="n">
-        <v>3.71</v>
+        <v>2.82</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>19/10/2023 04:42</t>
+          <t>10/11/2023 06:42</t>
         </is>
       </c>
       <c r="P31" t="n">
-        <v>3.91</v>
+        <v>2.86</v>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>10/11/2023 14:57</t>
+          <t>10/11/2023 13:35</t>
         </is>
       </c>
       <c r="R31" t="n">
-        <v>6.42</v>
+        <v>2.5</v>
       </c>
       <c r="S31" t="inlineStr">
         <is>
-          <t>19/10/2023 04:42</t>
+          <t>10/11/2023 06:42</t>
         </is>
       </c>
       <c r="T31" t="n">
-        <v>8.550000000000001</v>
+        <v>2.53</v>
       </c>
       <c r="U31" t="inlineStr">
         <is>
-          <t>10/11/2023 14:57</t>
+          <t>10/11/2023 15:16</t>
         </is>
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/paradou-oran/ALKA1eA0/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-constantine/6mEJaZvD/</t>
         </is>
       </c>
     </row>
@@ -3333,71 +3333,71 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Paradou</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Constantine</t>
+          <t>Oran</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>3.14</v>
+        <v>1.48</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>10/11/2023 06:42</t>
+          <t>19/10/2023 04:42</t>
         </is>
       </c>
       <c r="L32" t="n">
-        <v>3.21</v>
+        <v>1.46</v>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>10/11/2023 15:16</t>
+          <t>10/11/2023 14:57</t>
         </is>
       </c>
       <c r="N32" t="n">
-        <v>2.82</v>
+        <v>3.71</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>10/11/2023 06:42</t>
+          <t>19/10/2023 04:42</t>
         </is>
       </c>
       <c r="P32" t="n">
-        <v>2.86</v>
+        <v>3.91</v>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>10/11/2023 13:35</t>
+          <t>10/11/2023 14:57</t>
         </is>
       </c>
       <c r="R32" t="n">
-        <v>2.5</v>
+        <v>6.42</v>
       </c>
       <c r="S32" t="inlineStr">
         <is>
-          <t>10/11/2023 06:42</t>
+          <t>19/10/2023 04:42</t>
         </is>
       </c>
       <c r="T32" t="n">
-        <v>2.53</v>
+        <v>8.550000000000001</v>
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>10/11/2023 15:16</t>
+          <t>10/11/2023 14:57</t>
         </is>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-constantine/6mEJaZvD/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/paradou-oran/ALKA1eA0/</t>
         </is>
       </c>
     </row>
@@ -4161,71 +4161,71 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>El Bayadh</t>
+          <t>Constantine</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" t="n">
-        <v>1.45</v>
+        <v>1.59</v>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>16/11/2023 03:42</t>
+          <t>26/10/2023 04:42</t>
         </is>
       </c>
       <c r="L41" t="n">
-        <v>1.45</v>
+        <v>1.31</v>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>17/11/2023 15:18</t>
+          <t>17/11/2023 15:24</t>
         </is>
       </c>
       <c r="N41" t="n">
-        <v>3.74</v>
+        <v>3.47</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>16/11/2023 03:42</t>
+          <t>26/10/2023 04:42</t>
         </is>
       </c>
       <c r="P41" t="n">
-        <v>4.01</v>
+        <v>4.98</v>
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>17/11/2023 15:18</t>
+          <t>17/11/2023 15:24</t>
         </is>
       </c>
       <c r="R41" t="n">
-        <v>7.38</v>
+        <v>5.42</v>
       </c>
       <c r="S41" t="inlineStr">
         <is>
-          <t>16/11/2023 03:42</t>
+          <t>26/10/2023 04:42</t>
         </is>
       </c>
       <c r="T41" t="n">
-        <v>8.609999999999999</v>
+        <v>10.79</v>
       </c>
       <c r="U41" t="inlineStr">
         <is>
-          <t>17/11/2023 15:18</t>
+          <t>17/11/2023 15:24</t>
         </is>
       </c>
       <c r="V41" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-us-souf/UqfmFEv0/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-magra/jgeqGfPg/</t>
         </is>
       </c>
     </row>
@@ -4253,71 +4253,71 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Constantine</t>
+          <t>El Bayadh</t>
         </is>
       </c>
       <c r="G42" t="n">
+        <v>4</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>US Souf</t>
+        </is>
+      </c>
+      <c r="I42" t="n">
         <v>0</v>
       </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>Magra</t>
-        </is>
-      </c>
-      <c r="I42" t="n">
-        <v>1</v>
-      </c>
       <c r="J42" t="n">
-        <v>1.59</v>
+        <v>1.45</v>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>26/10/2023 04:42</t>
+          <t>16/11/2023 03:42</t>
         </is>
       </c>
       <c r="L42" t="n">
-        <v>1.31</v>
+        <v>1.45</v>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>17/11/2023 15:24</t>
+          <t>17/11/2023 15:18</t>
         </is>
       </c>
       <c r="N42" t="n">
-        <v>3.47</v>
+        <v>3.74</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>26/10/2023 04:42</t>
+          <t>16/11/2023 03:42</t>
         </is>
       </c>
       <c r="P42" t="n">
-        <v>4.98</v>
+        <v>4.01</v>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>17/11/2023 15:24</t>
+          <t>17/11/2023 15:18</t>
         </is>
       </c>
       <c r="R42" t="n">
-        <v>5.42</v>
+        <v>7.38</v>
       </c>
       <c r="S42" t="inlineStr">
         <is>
-          <t>26/10/2023 04:42</t>
+          <t>16/11/2023 03:42</t>
         </is>
       </c>
       <c r="T42" t="n">
-        <v>10.79</v>
+        <v>8.609999999999999</v>
       </c>
       <c r="U42" t="inlineStr">
         <is>
-          <t>17/11/2023 15:24</t>
+          <t>17/11/2023 15:18</t>
         </is>
       </c>
       <c r="V42" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-magra/jgeqGfPg/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-us-souf/UqfmFEv0/</t>
         </is>
       </c>
     </row>
@@ -5081,22 +5081,22 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Khenchela</t>
         </is>
       </c>
       <c r="G51" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>MC Alger</t>
+          <t>Ben Aknoun</t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J51" t="n">
-        <v>4.45</v>
+        <v>1.36</v>
       </c>
       <c r="K51" t="inlineStr">
         <is>
@@ -5104,7 +5104,7 @@
         </is>
       </c>
       <c r="L51" t="n">
-        <v>5.84</v>
+        <v>1.32</v>
       </c>
       <c r="M51" t="inlineStr">
         <is>
@@ -5112,7 +5112,7 @@
         </is>
       </c>
       <c r="N51" t="n">
-        <v>2.95</v>
+        <v>4.19</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -5120,7 +5120,7 @@
         </is>
       </c>
       <c r="P51" t="n">
-        <v>3.36</v>
+        <v>4.72</v>
       </c>
       <c r="Q51" t="inlineStr">
         <is>
@@ -5128,7 +5128,7 @@
         </is>
       </c>
       <c r="R51" t="n">
-        <v>1.89</v>
+        <v>7.76</v>
       </c>
       <c r="S51" t="inlineStr">
         <is>
@@ -5136,7 +5136,7 @@
         </is>
       </c>
       <c r="T51" t="n">
-        <v>1.7</v>
+        <v>11.86</v>
       </c>
       <c r="U51" t="inlineStr">
         <is>
@@ -5145,7 +5145,7 @@
       </c>
       <c r="V51" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-mc-alger/Uyh5oKM9/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-es-ben-aknoun/bwyflMxi/</t>
         </is>
       </c>
     </row>
@@ -5173,22 +5173,22 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Khenchela</t>
+          <t>US Souf</t>
         </is>
       </c>
       <c r="G52" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Ben Aknoun</t>
+          <t>MC Alger</t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J52" t="n">
-        <v>1.36</v>
+        <v>4.45</v>
       </c>
       <c r="K52" t="inlineStr">
         <is>
@@ -5196,7 +5196,7 @@
         </is>
       </c>
       <c r="L52" t="n">
-        <v>1.32</v>
+        <v>5.84</v>
       </c>
       <c r="M52" t="inlineStr">
         <is>
@@ -5204,7 +5204,7 @@
         </is>
       </c>
       <c r="N52" t="n">
-        <v>4.19</v>
+        <v>2.95</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -5212,7 +5212,7 @@
         </is>
       </c>
       <c r="P52" t="n">
-        <v>4.72</v>
+        <v>3.36</v>
       </c>
       <c r="Q52" t="inlineStr">
         <is>
@@ -5220,7 +5220,7 @@
         </is>
       </c>
       <c r="R52" t="n">
-        <v>7.76</v>
+        <v>1.89</v>
       </c>
       <c r="S52" t="inlineStr">
         <is>
@@ -5228,7 +5228,7 @@
         </is>
       </c>
       <c r="T52" t="n">
-        <v>11.86</v>
+        <v>1.7</v>
       </c>
       <c r="U52" t="inlineStr">
         <is>
@@ -5237,7 +5237,7 @@
       </c>
       <c r="V52" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/khenchela-es-ben-aknoun/bwyflMxi/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-mc-alger/Uyh5oKM9/</t>
         </is>
       </c>
     </row>
@@ -6277,22 +6277,22 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Magra</t>
+          <t>US Souf</t>
         </is>
       </c>
       <c r="G64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>ASO Chlef</t>
+          <t>Saoura</t>
         </is>
       </c>
       <c r="I64" t="n">
         <v>1</v>
       </c>
       <c r="J64" t="n">
-        <v>2.38</v>
+        <v>3.28</v>
       </c>
       <c r="K64" t="inlineStr">
         <is>
@@ -6300,15 +6300,15 @@
         </is>
       </c>
       <c r="L64" t="n">
-        <v>2.42</v>
+        <v>3.07</v>
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>09/12/2023 14:55</t>
+          <t>09/12/2023 13:02</t>
         </is>
       </c>
       <c r="N64" t="n">
-        <v>2.82</v>
+        <v>2.91</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -6316,15 +6316,15 @@
         </is>
       </c>
       <c r="P64" t="n">
-        <v>2.9</v>
+        <v>2.92</v>
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>09/12/2023 14:55</t>
+          <t>09/12/2023 13:02</t>
         </is>
       </c>
       <c r="R64" t="n">
-        <v>3.47</v>
+        <v>2.41</v>
       </c>
       <c r="S64" t="inlineStr">
         <is>
@@ -6332,16 +6332,16 @@
         </is>
       </c>
       <c r="T64" t="n">
-        <v>3.35</v>
+        <v>2.57</v>
       </c>
       <c r="U64" t="inlineStr">
         <is>
-          <t>09/12/2023 14:55</t>
+          <t>09/12/2023 14:31</t>
         </is>
       </c>
       <c r="V64" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-aso-chlef/CjA5ex5g/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-saoura/YP0QjEJO/</t>
         </is>
       </c>
     </row>
@@ -6369,22 +6369,22 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="G65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Saoura</t>
+          <t>ASO Chlef</t>
         </is>
       </c>
       <c r="I65" t="n">
         <v>1</v>
       </c>
       <c r="J65" t="n">
-        <v>3.28</v>
+        <v>2.38</v>
       </c>
       <c r="K65" t="inlineStr">
         <is>
@@ -6392,15 +6392,15 @@
         </is>
       </c>
       <c r="L65" t="n">
-        <v>3.07</v>
+        <v>2.42</v>
       </c>
       <c r="M65" t="inlineStr">
         <is>
-          <t>09/12/2023 13:02</t>
+          <t>09/12/2023 14:55</t>
         </is>
       </c>
       <c r="N65" t="n">
-        <v>2.91</v>
+        <v>2.82</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -6408,15 +6408,15 @@
         </is>
       </c>
       <c r="P65" t="n">
-        <v>2.92</v>
+        <v>2.9</v>
       </c>
       <c r="Q65" t="inlineStr">
         <is>
-          <t>09/12/2023 13:02</t>
+          <t>09/12/2023 14:55</t>
         </is>
       </c>
       <c r="R65" t="n">
-        <v>2.41</v>
+        <v>3.47</v>
       </c>
       <c r="S65" t="inlineStr">
         <is>
@@ -6424,16 +6424,16 @@
         </is>
       </c>
       <c r="T65" t="n">
-        <v>2.57</v>
+        <v>3.35</v>
       </c>
       <c r="U65" t="inlineStr">
         <is>
-          <t>09/12/2023 14:31</t>
+          <t>09/12/2023 14:55</t>
         </is>
       </c>
       <c r="V65" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-saoura/YP0QjEJO/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-aso-chlef/CjA5ex5g/</t>
         </is>
       </c>
     </row>
@@ -7906,6 +7906,466 @@
       <c r="V81" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-es-ben-aknoun/z72UKhY4/</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E82" s="2" t="n">
+        <v>45296.63541666666</v>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Ben Aknoun</t>
+        </is>
+      </c>
+      <c r="G82" t="n">
+        <v>2</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Oran</t>
+        </is>
+      </c>
+      <c r="I82" t="n">
+        <v>1</v>
+      </c>
+      <c r="J82" t="n">
+        <v>2.42</v>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>04/01/2024 07:10</t>
+        </is>
+      </c>
+      <c r="L82" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="M82" t="inlineStr">
+        <is>
+          <t>05/01/2024 14:56</t>
+        </is>
+      </c>
+      <c r="N82" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>04/01/2024 07:10</t>
+        </is>
+      </c>
+      <c r="P82" t="n">
+        <v>2.73</v>
+      </c>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>05/01/2024 15:06</t>
+        </is>
+      </c>
+      <c r="R82" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="S82" t="inlineStr">
+        <is>
+          <t>04/01/2024 07:10</t>
+        </is>
+      </c>
+      <c r="T82" t="n">
+        <v>3.43</v>
+      </c>
+      <c r="U82" t="inlineStr">
+        <is>
+          <t>05/01/2024 14:58</t>
+        </is>
+      </c>
+      <c r="V82" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/es-ben-aknoun-oran/EDkdZimb/</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E83" s="2" t="n">
+        <v>45296.63541666666</v>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Magra</t>
+        </is>
+      </c>
+      <c r="G83" t="n">
+        <v>0</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>ES Setif</t>
+        </is>
+      </c>
+      <c r="I83" t="n">
+        <v>1</v>
+      </c>
+      <c r="J83" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>03/01/2024 08:01</t>
+        </is>
+      </c>
+      <c r="L83" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="M83" t="inlineStr">
+        <is>
+          <t>05/01/2024 15:01</t>
+        </is>
+      </c>
+      <c r="N83" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>03/01/2024 08:01</t>
+        </is>
+      </c>
+      <c r="P83" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="Q83" t="inlineStr">
+        <is>
+          <t>05/01/2024 15:01</t>
+        </is>
+      </c>
+      <c r="R83" t="n">
+        <v>3.09</v>
+      </c>
+      <c r="S83" t="inlineStr">
+        <is>
+          <t>03/01/2024 08:01</t>
+        </is>
+      </c>
+      <c r="T83" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="U83" t="inlineStr">
+        <is>
+          <t>05/01/2024 14:39</t>
+        </is>
+      </c>
+      <c r="V83" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-es-setif/YaHZHjIN/</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E84" s="2" t="n">
+        <v>45296.63541666666</v>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>US Souf</t>
+        </is>
+      </c>
+      <c r="G84" t="n">
+        <v>1</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Paradou</t>
+        </is>
+      </c>
+      <c r="I84" t="n">
+        <v>4</v>
+      </c>
+      <c r="J84" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>03/01/2024 15:42</t>
+        </is>
+      </c>
+      <c r="L84" t="n">
+        <v>4.36</v>
+      </c>
+      <c r="M84" t="inlineStr">
+        <is>
+          <t>05/01/2024 15:10</t>
+        </is>
+      </c>
+      <c r="N84" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>03/01/2024 15:42</t>
+        </is>
+      </c>
+      <c r="P84" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="Q84" t="inlineStr">
+        <is>
+          <t>05/01/2024 15:10</t>
+        </is>
+      </c>
+      <c r="R84" t="n">
+        <v>2.63</v>
+      </c>
+      <c r="S84" t="inlineStr">
+        <is>
+          <t>03/01/2024 15:42</t>
+        </is>
+      </c>
+      <c r="T84" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="U84" t="inlineStr">
+        <is>
+          <t>05/01/2024 15:10</t>
+        </is>
+      </c>
+      <c r="V84" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-paradou/f9IVIW2H/</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E85" s="2" t="n">
+        <v>45296.65625</v>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>ASO Chlef</t>
+        </is>
+      </c>
+      <c r="G85" t="n">
+        <v>0</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>USM Alger</t>
+        </is>
+      </c>
+      <c r="I85" t="n">
+        <v>1</v>
+      </c>
+      <c r="J85" t="n">
+        <v>2.09</v>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>04/01/2024 07:12</t>
+        </is>
+      </c>
+      <c r="L85" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="M85" t="inlineStr">
+        <is>
+          <t>05/01/2024 15:20</t>
+        </is>
+      </c>
+      <c r="N85" t="n">
+        <v>2.85</v>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>04/01/2024 07:12</t>
+        </is>
+      </c>
+      <c r="P85" t="n">
+        <v>3.18</v>
+      </c>
+      <c r="Q85" t="inlineStr">
+        <is>
+          <t>05/01/2024 15:40</t>
+        </is>
+      </c>
+      <c r="R85" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="S85" t="inlineStr">
+        <is>
+          <t>04/01/2024 07:12</t>
+        </is>
+      </c>
+      <c r="T85" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="U85" t="inlineStr">
+        <is>
+          <t>05/01/2024 15:20</t>
+        </is>
+      </c>
+      <c r="V85" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/aso-chlef-usm-alger/SMGwHAXT/</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E86" s="2" t="n">
+        <v>45296.77083333334</v>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Constantine</t>
+        </is>
+      </c>
+      <c r="G86" t="n">
+        <v>1</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>Biskra</t>
+        </is>
+      </c>
+      <c r="I86" t="n">
+        <v>1</v>
+      </c>
+      <c r="J86" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>03/01/2024 18:42</t>
+        </is>
+      </c>
+      <c r="L86" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="M86" t="inlineStr">
+        <is>
+          <t>05/01/2024 18:25</t>
+        </is>
+      </c>
+      <c r="N86" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>03/01/2024 18:42</t>
+        </is>
+      </c>
+      <c r="P86" t="n">
+        <v>4.53</v>
+      </c>
+      <c r="Q86" t="inlineStr">
+        <is>
+          <t>05/01/2024 18:27</t>
+        </is>
+      </c>
+      <c r="R86" t="n">
+        <v>7.01</v>
+      </c>
+      <c r="S86" t="inlineStr">
+        <is>
+          <t>03/01/2024 18:42</t>
+        </is>
+      </c>
+      <c r="T86" t="n">
+        <v>10.68</v>
+      </c>
+      <c r="U86" t="inlineStr">
+        <is>
+          <t>05/01/2024 18:27</t>
+        </is>
+      </c>
+      <c r="V86" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-biskra/pvohzYXi/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 07-01-2024 08:45
</commit_message>
<xml_diff>
--- a/2023/algeria_ligue-1_2023-2024.xlsx
+++ b/2023/algeria_ligue-1_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V86"/>
+  <dimension ref="A1:V88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2321,22 +2321,22 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>MC Alger</t>
+          <t>Constantine</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>ES Setif</t>
+          <t>Saoura</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>1.53</v>
+        <v>1.76</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
@@ -2344,15 +2344,15 @@
         </is>
       </c>
       <c r="L21" t="n">
-        <v>1.52</v>
+        <v>1.75</v>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>06/10/2023 16:29</t>
+          <t>06/10/2023 16:25</t>
         </is>
       </c>
       <c r="N21" t="n">
-        <v>3.6</v>
+        <v>3.23</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -2360,15 +2360,15 @@
         </is>
       </c>
       <c r="P21" t="n">
-        <v>3.71</v>
+        <v>3.26</v>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>06/10/2023 16:34</t>
+          <t>06/10/2023 16:28</t>
         </is>
       </c>
       <c r="R21" t="n">
-        <v>6.62</v>
+        <v>4.69</v>
       </c>
       <c r="S21" t="inlineStr">
         <is>
@@ -2376,16 +2376,16 @@
         </is>
       </c>
       <c r="T21" t="n">
-        <v>7.77</v>
+        <v>5.64</v>
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>06/10/2023 16:34</t>
+          <t>06/10/2023 15:05</t>
         </is>
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/mc-alger-es-setif/OtADSIdf/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-saoura/2RL4UvSs/</t>
         </is>
       </c>
     </row>
@@ -2413,22 +2413,22 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Constantine</t>
+          <t>MC Alger</t>
         </is>
       </c>
       <c r="G22" t="n">
+        <v>5</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>ES Setif</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
         <v>3</v>
       </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>Saoura</t>
-        </is>
-      </c>
-      <c r="I22" t="n">
-        <v>0</v>
-      </c>
       <c r="J22" t="n">
-        <v>1.76</v>
+        <v>1.53</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
@@ -2436,15 +2436,15 @@
         </is>
       </c>
       <c r="L22" t="n">
-        <v>1.75</v>
+        <v>1.52</v>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>06/10/2023 16:25</t>
+          <t>06/10/2023 16:29</t>
         </is>
       </c>
       <c r="N22" t="n">
-        <v>3.23</v>
+        <v>3.6</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2452,15 +2452,15 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>3.26</v>
+        <v>3.71</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>06/10/2023 16:28</t>
+          <t>06/10/2023 16:34</t>
         </is>
       </c>
       <c r="R22" t="n">
-        <v>4.69</v>
+        <v>6.62</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>
@@ -2468,16 +2468,16 @@
         </is>
       </c>
       <c r="T22" t="n">
-        <v>5.64</v>
+        <v>7.77</v>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>06/10/2023 15:05</t>
+          <t>06/10/2023 16:34</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-saoura/2RL4UvSs/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/mc-alger-es-setif/OtADSIdf/</t>
         </is>
       </c>
     </row>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Biskra</t>
+          <t>Oran</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -2513,14 +2513,14 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Paradou</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>2.18</v>
+        <v>1.98</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
@@ -2528,15 +2528,15 @@
         </is>
       </c>
       <c r="L23" t="n">
-        <v>2.03</v>
+        <v>1.65</v>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>06/10/2023 19:34</t>
+          <t>06/10/2023 17:55</t>
         </is>
       </c>
       <c r="N23" t="n">
-        <v>2.84</v>
+        <v>2.89</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2544,15 +2544,15 @@
         </is>
       </c>
       <c r="P23" t="n">
-        <v>3</v>
+        <v>3.28</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>06/10/2023 18:05</t>
+          <t>06/10/2023 19:03</t>
         </is>
       </c>
       <c r="R23" t="n">
-        <v>3.56</v>
+        <v>3.98</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
@@ -2560,16 +2560,16 @@
         </is>
       </c>
       <c r="T23" t="n">
-        <v>4.33</v>
+        <v>5.91</v>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>06/10/2023 19:34</t>
+          <t>06/10/2023 17:55</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-paradou/hhWUzskE/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-magra/WrVYZ04K/</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Oran</t>
+          <t>Biskra</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -2605,14 +2605,14 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Magra</t>
+          <t>Paradou</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J24" t="n">
-        <v>1.98</v>
+        <v>2.18</v>
       </c>
       <c r="K24" t="inlineStr">
         <is>
@@ -2620,15 +2620,15 @@
         </is>
       </c>
       <c r="L24" t="n">
-        <v>1.65</v>
+        <v>2.03</v>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>06/10/2023 17:55</t>
+          <t>06/10/2023 19:34</t>
         </is>
       </c>
       <c r="N24" t="n">
-        <v>2.89</v>
+        <v>2.84</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2636,15 +2636,15 @@
         </is>
       </c>
       <c r="P24" t="n">
-        <v>3.28</v>
+        <v>3</v>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>06/10/2023 19:03</t>
+          <t>06/10/2023 18:05</t>
         </is>
       </c>
       <c r="R24" t="n">
-        <v>3.98</v>
+        <v>3.56</v>
       </c>
       <c r="S24" t="inlineStr">
         <is>
@@ -2652,16 +2652,16 @@
         </is>
       </c>
       <c r="T24" t="n">
-        <v>5.91</v>
+        <v>4.33</v>
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>06/10/2023 17:55</t>
+          <t>06/10/2023 19:34</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/oran-magra/WrVYZ04K/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-paradou/hhWUzskE/</t>
         </is>
       </c>
     </row>
@@ -5725,22 +5725,22 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>ASO Chlef</t>
+          <t>Saoura</t>
         </is>
       </c>
       <c r="G58" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>ES Setif</t>
         </is>
       </c>
       <c r="I58" t="n">
         <v>0</v>
       </c>
       <c r="J58" t="n">
-        <v>1.35</v>
+        <v>1.88</v>
       </c>
       <c r="K58" t="inlineStr">
         <is>
@@ -5748,15 +5748,15 @@
         </is>
       </c>
       <c r="L58" t="n">
-        <v>1.32</v>
+        <v>1.75</v>
       </c>
       <c r="M58" t="inlineStr">
         <is>
-          <t>02/12/2023 16:27</t>
+          <t>02/12/2023 16:40</t>
         </is>
       </c>
       <c r="N58" t="n">
-        <v>4.37</v>
+        <v>3.01</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -5764,15 +5764,15 @@
         </is>
       </c>
       <c r="P58" t="n">
-        <v>4.85</v>
+        <v>3.32</v>
       </c>
       <c r="Q58" t="inlineStr">
         <is>
-          <t>02/12/2023 16:27</t>
+          <t>02/12/2023 16:40</t>
         </is>
       </c>
       <c r="R58" t="n">
-        <v>8.279999999999999</v>
+        <v>4.3</v>
       </c>
       <c r="S58" t="inlineStr">
         <is>
@@ -5780,16 +5780,16 @@
         </is>
       </c>
       <c r="T58" t="n">
-        <v>11.33</v>
+        <v>5.44</v>
       </c>
       <c r="U58" t="inlineStr">
         <is>
-          <t>02/12/2023 16:27</t>
+          <t>02/12/2023 16:40</t>
         </is>
       </c>
       <c r="V58" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/aso-chlef-us-souf/xzDYhqqe/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/saoura-es-setif/Kb2wh3b1/</t>
         </is>
       </c>
     </row>
@@ -5817,22 +5817,22 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Saoura</t>
+          <t>ASO Chlef</t>
         </is>
       </c>
       <c r="G59" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>ES Setif</t>
+          <t>US Souf</t>
         </is>
       </c>
       <c r="I59" t="n">
         <v>0</v>
       </c>
       <c r="J59" t="n">
-        <v>1.88</v>
+        <v>1.35</v>
       </c>
       <c r="K59" t="inlineStr">
         <is>
@@ -5840,15 +5840,15 @@
         </is>
       </c>
       <c r="L59" t="n">
-        <v>1.75</v>
+        <v>1.32</v>
       </c>
       <c r="M59" t="inlineStr">
         <is>
-          <t>02/12/2023 16:40</t>
+          <t>02/12/2023 16:27</t>
         </is>
       </c>
       <c r="N59" t="n">
-        <v>3.01</v>
+        <v>4.37</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -5856,15 +5856,15 @@
         </is>
       </c>
       <c r="P59" t="n">
-        <v>3.32</v>
+        <v>4.85</v>
       </c>
       <c r="Q59" t="inlineStr">
         <is>
-          <t>02/12/2023 16:40</t>
+          <t>02/12/2023 16:27</t>
         </is>
       </c>
       <c r="R59" t="n">
-        <v>4.3</v>
+        <v>8.279999999999999</v>
       </c>
       <c r="S59" t="inlineStr">
         <is>
@@ -5872,16 +5872,16 @@
         </is>
       </c>
       <c r="T59" t="n">
-        <v>5.44</v>
+        <v>11.33</v>
       </c>
       <c r="U59" t="inlineStr">
         <is>
-          <t>02/12/2023 16:40</t>
+          <t>02/12/2023 16:27</t>
         </is>
       </c>
       <c r="V59" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/saoura-es-setif/Kb2wh3b1/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/aso-chlef-us-souf/xzDYhqqe/</t>
         </is>
       </c>
     </row>
@@ -6277,22 +6277,22 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>US Souf</t>
+          <t>Magra</t>
         </is>
       </c>
       <c r="G64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Saoura</t>
+          <t>ASO Chlef</t>
         </is>
       </c>
       <c r="I64" t="n">
         <v>1</v>
       </c>
       <c r="J64" t="n">
-        <v>3.28</v>
+        <v>2.38</v>
       </c>
       <c r="K64" t="inlineStr">
         <is>
@@ -6300,15 +6300,15 @@
         </is>
       </c>
       <c r="L64" t="n">
-        <v>3.07</v>
+        <v>2.42</v>
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>09/12/2023 13:02</t>
+          <t>09/12/2023 14:55</t>
         </is>
       </c>
       <c r="N64" t="n">
-        <v>2.91</v>
+        <v>2.82</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -6316,15 +6316,15 @@
         </is>
       </c>
       <c r="P64" t="n">
-        <v>2.92</v>
+        <v>2.9</v>
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>09/12/2023 13:02</t>
+          <t>09/12/2023 14:55</t>
         </is>
       </c>
       <c r="R64" t="n">
-        <v>2.41</v>
+        <v>3.47</v>
       </c>
       <c r="S64" t="inlineStr">
         <is>
@@ -6332,16 +6332,16 @@
         </is>
       </c>
       <c r="T64" t="n">
-        <v>2.57</v>
+        <v>3.35</v>
       </c>
       <c r="U64" t="inlineStr">
         <is>
-          <t>09/12/2023 14:31</t>
+          <t>09/12/2023 14:55</t>
         </is>
       </c>
       <c r="V64" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-saoura/YP0QjEJO/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-aso-chlef/CjA5ex5g/</t>
         </is>
       </c>
     </row>
@@ -6369,22 +6369,22 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Magra</t>
+          <t>US Souf</t>
         </is>
       </c>
       <c r="G65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>ASO Chlef</t>
+          <t>Saoura</t>
         </is>
       </c>
       <c r="I65" t="n">
         <v>1</v>
       </c>
       <c r="J65" t="n">
-        <v>2.38</v>
+        <v>3.28</v>
       </c>
       <c r="K65" t="inlineStr">
         <is>
@@ -6392,15 +6392,15 @@
         </is>
       </c>
       <c r="L65" t="n">
-        <v>2.42</v>
+        <v>3.07</v>
       </c>
       <c r="M65" t="inlineStr">
         <is>
-          <t>09/12/2023 14:55</t>
+          <t>09/12/2023 13:02</t>
         </is>
       </c>
       <c r="N65" t="n">
-        <v>2.82</v>
+        <v>2.91</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -6408,15 +6408,15 @@
         </is>
       </c>
       <c r="P65" t="n">
-        <v>2.9</v>
+        <v>2.92</v>
       </c>
       <c r="Q65" t="inlineStr">
         <is>
-          <t>09/12/2023 14:55</t>
+          <t>09/12/2023 13:02</t>
         </is>
       </c>
       <c r="R65" t="n">
-        <v>3.47</v>
+        <v>2.41</v>
       </c>
       <c r="S65" t="inlineStr">
         <is>
@@ -6424,16 +6424,16 @@
         </is>
       </c>
       <c r="T65" t="n">
-        <v>3.35</v>
+        <v>2.57</v>
       </c>
       <c r="U65" t="inlineStr">
         <is>
-          <t>09/12/2023 14:55</t>
+          <t>09/12/2023 14:31</t>
         </is>
       </c>
       <c r="V65" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/magra-aso-chlef/CjA5ex5g/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/us-souf-saoura/YP0QjEJO/</t>
         </is>
       </c>
     </row>
@@ -6553,7 +6553,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>El Bayadh</t>
+          <t>Ben Aknoun</t>
         </is>
       </c>
       <c r="G67" t="n">
@@ -6561,63 +6561,63 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>USM Alger</t>
+          <t>CR Belouizdad</t>
         </is>
       </c>
       <c r="I67" t="n">
         <v>1</v>
       </c>
       <c r="J67" t="n">
-        <v>2.12</v>
+        <v>6.41</v>
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>14/12/2023 01:12</t>
+          <t>14/12/2023 00:12</t>
         </is>
       </c>
       <c r="L67" t="n">
-        <v>2.16</v>
+        <v>5.81</v>
       </c>
       <c r="M67" t="inlineStr">
         <is>
-          <t>15/12/2023 15:13</t>
+          <t>15/12/2023 15:12</t>
         </is>
       </c>
       <c r="N67" t="n">
-        <v>2.86</v>
+        <v>3.37</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>14/12/2023 01:12</t>
+          <t>14/12/2023 00:12</t>
         </is>
       </c>
       <c r="P67" t="n">
-        <v>2.85</v>
+        <v>3.59</v>
       </c>
       <c r="Q67" t="inlineStr">
         <is>
-          <t>15/12/2023 15:10</t>
+          <t>15/12/2023 15:12</t>
         </is>
       </c>
       <c r="R67" t="n">
-        <v>3.99</v>
+        <v>1.56</v>
       </c>
       <c r="S67" t="inlineStr">
         <is>
-          <t>14/12/2023 01:12</t>
+          <t>14/12/2023 00:12</t>
         </is>
       </c>
       <c r="T67" t="n">
-        <v>4.3</v>
+        <v>1.65</v>
       </c>
       <c r="U67" t="inlineStr">
         <is>
-          <t>15/12/2023 15:13</t>
+          <t>15/12/2023 15:12</t>
         </is>
       </c>
       <c r="V67" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-usm-alger/Ywta5DYH/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/es-ben-aknoun-cr-belouizdad/CjWzBH4t/</t>
         </is>
       </c>
     </row>
@@ -6645,7 +6645,7 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Ben Aknoun</t>
+          <t>El Bayadh</t>
         </is>
       </c>
       <c r="G68" t="n">
@@ -6653,63 +6653,63 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>CR Belouizdad</t>
+          <t>USM Alger</t>
         </is>
       </c>
       <c r="I68" t="n">
         <v>1</v>
       </c>
       <c r="J68" t="n">
-        <v>6.41</v>
+        <v>2.12</v>
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>14/12/2023 00:12</t>
+          <t>14/12/2023 01:12</t>
         </is>
       </c>
       <c r="L68" t="n">
-        <v>5.81</v>
+        <v>2.16</v>
       </c>
       <c r="M68" t="inlineStr">
         <is>
-          <t>15/12/2023 15:12</t>
+          <t>15/12/2023 15:13</t>
         </is>
       </c>
       <c r="N68" t="n">
-        <v>3.37</v>
+        <v>2.86</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>14/12/2023 00:12</t>
+          <t>14/12/2023 01:12</t>
         </is>
       </c>
       <c r="P68" t="n">
-        <v>3.59</v>
+        <v>2.85</v>
       </c>
       <c r="Q68" t="inlineStr">
         <is>
-          <t>15/12/2023 15:12</t>
+          <t>15/12/2023 15:10</t>
         </is>
       </c>
       <c r="R68" t="n">
-        <v>1.56</v>
+        <v>3.99</v>
       </c>
       <c r="S68" t="inlineStr">
         <is>
-          <t>14/12/2023 00:12</t>
+          <t>14/12/2023 01:12</t>
         </is>
       </c>
       <c r="T68" t="n">
-        <v>1.65</v>
+        <v>4.3</v>
       </c>
       <c r="U68" t="inlineStr">
         <is>
-          <t>15/12/2023 15:12</t>
+          <t>15/12/2023 15:13</t>
         </is>
       </c>
       <c r="V68" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/es-ben-aknoun-cr-belouizdad/CjWzBH4t/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/el-bayadh-usm-alger/Ywta5DYH/</t>
         </is>
       </c>
     </row>
@@ -7749,22 +7749,22 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>USM Alger</t>
+          <t>Biskra</t>
         </is>
       </c>
       <c r="G80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>MC Alger</t>
+          <t>Ben Aknoun</t>
         </is>
       </c>
       <c r="I80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J80" t="n">
-        <v>2.92</v>
+        <v>1.57</v>
       </c>
       <c r="K80" t="inlineStr">
         <is>
@@ -7772,15 +7772,15 @@
         </is>
       </c>
       <c r="L80" t="n">
-        <v>3.62</v>
+        <v>1.41</v>
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>29/12/2023 17:59</t>
+          <t>29/12/2023 17:57</t>
         </is>
       </c>
       <c r="N80" t="n">
-        <v>2.96</v>
+        <v>3.47</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
@@ -7788,15 +7788,15 @@
         </is>
       </c>
       <c r="P80" t="n">
-        <v>2.98</v>
+        <v>4.05</v>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
-          <t>29/12/2023 17:56</t>
+          <t>29/12/2023 17:57</t>
         </is>
       </c>
       <c r="R80" t="n">
-        <v>2.42</v>
+        <v>5.97</v>
       </c>
       <c r="S80" t="inlineStr">
         <is>
@@ -7804,16 +7804,16 @@
         </is>
       </c>
       <c r="T80" t="n">
-        <v>2.24</v>
+        <v>9.98</v>
       </c>
       <c r="U80" t="inlineStr">
         <is>
-          <t>29/12/2023 17:59</t>
+          <t>29/12/2023 17:57</t>
         </is>
       </c>
       <c r="V80" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/usm-alger-mc-alger/jDDqjB3f/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-es-ben-aknoun/z72UKhY4/</t>
         </is>
       </c>
     </row>
@@ -7841,22 +7841,22 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Biskra</t>
+          <t>USM Alger</t>
         </is>
       </c>
       <c r="G81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Ben Aknoun</t>
+          <t>MC Alger</t>
         </is>
       </c>
       <c r="I81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J81" t="n">
-        <v>1.57</v>
+        <v>2.92</v>
       </c>
       <c r="K81" t="inlineStr">
         <is>
@@ -7864,15 +7864,15 @@
         </is>
       </c>
       <c r="L81" t="n">
-        <v>1.41</v>
+        <v>3.62</v>
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>29/12/2023 17:57</t>
+          <t>29/12/2023 17:59</t>
         </is>
       </c>
       <c r="N81" t="n">
-        <v>3.47</v>
+        <v>2.96</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
@@ -7880,15 +7880,15 @@
         </is>
       </c>
       <c r="P81" t="n">
-        <v>4.05</v>
+        <v>2.98</v>
       </c>
       <c r="Q81" t="inlineStr">
         <is>
-          <t>29/12/2023 17:57</t>
+          <t>29/12/2023 17:56</t>
         </is>
       </c>
       <c r="R81" t="n">
-        <v>5.97</v>
+        <v>2.42</v>
       </c>
       <c r="S81" t="inlineStr">
         <is>
@@ -7896,16 +7896,16 @@
         </is>
       </c>
       <c r="T81" t="n">
-        <v>9.98</v>
+        <v>2.24</v>
       </c>
       <c r="U81" t="inlineStr">
         <is>
-          <t>29/12/2023 17:57</t>
+          <t>29/12/2023 17:59</t>
         </is>
       </c>
       <c r="V81" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/algeria/ligue-1/biskra-es-ben-aknoun/z72UKhY4/</t>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/usm-alger-mc-alger/jDDqjB3f/</t>
         </is>
       </c>
     </row>
@@ -8366,6 +8366,190 @@
       <c r="V86" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/algeria/ligue-1/constantine-biskra/pvohzYXi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E87" s="2" t="n">
+        <v>45297.66666666666</v>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Saoura</t>
+        </is>
+      </c>
+      <c r="G87" t="n">
+        <v>0</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>Khenchela</t>
+        </is>
+      </c>
+      <c r="I87" t="n">
+        <v>1</v>
+      </c>
+      <c r="J87" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>04/01/2024 09:12</t>
+        </is>
+      </c>
+      <c r="L87" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="M87" t="inlineStr">
+        <is>
+          <t>06/01/2024 15:57</t>
+        </is>
+      </c>
+      <c r="N87" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>04/01/2024 09:12</t>
+        </is>
+      </c>
+      <c r="P87" t="n">
+        <v>3.62</v>
+      </c>
+      <c r="Q87" t="inlineStr">
+        <is>
+          <t>06/01/2024 15:57</t>
+        </is>
+      </c>
+      <c r="R87" t="n">
+        <v>4.87</v>
+      </c>
+      <c r="S87" t="inlineStr">
+        <is>
+          <t>04/01/2024 09:12</t>
+        </is>
+      </c>
+      <c r="T87" t="n">
+        <v>8.130000000000001</v>
+      </c>
+      <c r="U87" t="inlineStr">
+        <is>
+          <t>06/01/2024 15:57</t>
+        </is>
+      </c>
+      <c r="V87" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/saoura-khenchela/Ec1YJCmB/</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>algeria</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>ligue-1</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E88" s="2" t="n">
+        <v>45297.75</v>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>MC Alger</t>
+        </is>
+      </c>
+      <c r="G88" t="n">
+        <v>1</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>Kabylie</t>
+        </is>
+      </c>
+      <c r="I88" t="n">
+        <v>1</v>
+      </c>
+      <c r="J88" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>04/01/2024 09:12</t>
+        </is>
+      </c>
+      <c r="L88" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="M88" t="inlineStr">
+        <is>
+          <t>06/01/2024 17:58</t>
+        </is>
+      </c>
+      <c r="N88" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>04/01/2024 09:12</t>
+        </is>
+      </c>
+      <c r="P88" t="n">
+        <v>3.79</v>
+      </c>
+      <c r="Q88" t="inlineStr">
+        <is>
+          <t>06/01/2024 17:58</t>
+        </is>
+      </c>
+      <c r="R88" t="n">
+        <v>7.24</v>
+      </c>
+      <c r="S88" t="inlineStr">
+        <is>
+          <t>04/01/2024 09:12</t>
+        </is>
+      </c>
+      <c r="T88" t="n">
+        <v>8.69</v>
+      </c>
+      <c r="U88" t="inlineStr">
+        <is>
+          <t>06/01/2024 17:58</t>
+        </is>
+      </c>
+      <c r="V88" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/algeria/ligue-1/mc-alger-kabylie/4r85CUuo/</t>
         </is>
       </c>
     </row>

</xml_diff>